<commit_message>
Update Report I and II Update backlog
</commit_message>
<xml_diff>
--- a/Documents/ProductBackLog/Capstone_Group6_ProductBackLog_SprintTaskList.xlsx
+++ b/Documents/ProductBackLog/Capstone_Group6_ProductBackLog_SprintTaskList.xlsx
@@ -3268,60 +3268,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="21" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3398,6 +3344,60 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="21" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3405,6 +3405,478 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="143">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3438,484 +3910,12 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -9107,27 +9107,27 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table13456789" displayName="Table13456789" ref="B10:O54" totalsRowShown="0" headerRowDxfId="18" dataDxfId="0" headerRowBorderDxfId="16" tableBorderDxfId="17" totalsRowBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table13456789" displayName="Table13456789" ref="B10:O54" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="B10:O54">
     <filterColumn colId="5"/>
     <filterColumn colId="12"/>
     <filterColumn colId="13"/>
   </autoFilter>
   <tableColumns count="14">
-    <tableColumn id="1" name="No." dataDxfId="14"/>
-    <tableColumn id="2" name="Task description" dataDxfId="13"/>
-    <tableColumn id="3" name="Type" dataDxfId="12"/>
-    <tableColumn id="4" name="Assign To" dataDxfId="11"/>
-    <tableColumn id="5" name="Status" dataDxfId="10"/>
-    <tableColumn id="7" name="Estimate" dataDxfId="9"/>
-    <tableColumn id="8" name="20/05" dataDxfId="8"/>
-    <tableColumn id="9" name="21/05" dataDxfId="7"/>
-    <tableColumn id="10" name="22/05" dataDxfId="6"/>
-    <tableColumn id="11" name="23/05" dataDxfId="5"/>
-    <tableColumn id="12" name="24/05" dataDxfId="4"/>
-    <tableColumn id="13" name="25/05" dataDxfId="3"/>
-    <tableColumn id="14" name="26/05" dataDxfId="2"/>
-    <tableColumn id="15" name="End" dataDxfId="1"/>
+    <tableColumn id="1" name="No." dataDxfId="13"/>
+    <tableColumn id="2" name="Task description" dataDxfId="12"/>
+    <tableColumn id="3" name="Type" dataDxfId="11"/>
+    <tableColumn id="4" name="Assign To" dataDxfId="10"/>
+    <tableColumn id="5" name="Status" dataDxfId="9"/>
+    <tableColumn id="7" name="Estimate" dataDxfId="8"/>
+    <tableColumn id="8" name="20/05" dataDxfId="7"/>
+    <tableColumn id="9" name="21/05" dataDxfId="6"/>
+    <tableColumn id="10" name="22/05" dataDxfId="5"/>
+    <tableColumn id="11" name="23/05" dataDxfId="4"/>
+    <tableColumn id="12" name="24/05" dataDxfId="3"/>
+    <tableColumn id="13" name="25/05" dataDxfId="2"/>
+    <tableColumn id="14" name="26/05" dataDxfId="1"/>
+    <tableColumn id="15" name="End" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9508,7 +9508,7 @@
       </c>
     </row>
     <row r="14" spans="2:7">
-      <c r="C14" s="330">
+      <c r="C14" s="354">
         <v>2</v>
       </c>
       <c r="D14" s="17" t="s">
@@ -9519,7 +9519,7 @@
       </c>
     </row>
     <row r="15" spans="2:7">
-      <c r="C15" s="331"/>
+      <c r="C15" s="355"/>
       <c r="D15" s="3" t="s">
         <v>2</v>
       </c>
@@ -9527,28 +9527,28 @@
       <c r="G15" s="26"/>
     </row>
     <row r="16" spans="2:7">
-      <c r="C16" s="331"/>
+      <c r="C16" s="355"/>
       <c r="D16" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E16" s="19"/>
     </row>
     <row r="17" spans="3:8">
-      <c r="C17" s="331"/>
+      <c r="C17" s="355"/>
       <c r="D17" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E17" s="19"/>
     </row>
     <row r="18" spans="3:8">
-      <c r="C18" s="332"/>
+      <c r="C18" s="361"/>
       <c r="D18" s="20" t="s">
         <v>5</v>
       </c>
       <c r="E18" s="21"/>
     </row>
     <row r="19" spans="3:8">
-      <c r="C19" s="335">
+      <c r="C19" s="368">
         <v>3</v>
       </c>
       <c r="D19" s="51" t="s">
@@ -9559,7 +9559,7 @@
       </c>
     </row>
     <row r="20" spans="3:8">
-      <c r="C20" s="336"/>
+      <c r="C20" s="369"/>
       <c r="D20" s="4" t="s">
         <v>7</v>
       </c>
@@ -9569,7 +9569,7 @@
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="3:8">
-      <c r="C21" s="336"/>
+      <c r="C21" s="369"/>
       <c r="D21" s="3" t="s">
         <v>8</v>
       </c>
@@ -9579,42 +9579,42 @@
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="3:8">
-      <c r="C22" s="336"/>
+      <c r="C22" s="369"/>
       <c r="D22" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E22" s="50"/>
     </row>
     <row r="23" spans="3:8">
-      <c r="C23" s="336"/>
+      <c r="C23" s="369"/>
       <c r="D23" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E23" s="50"/>
     </row>
     <row r="24" spans="3:8">
-      <c r="C24" s="336"/>
+      <c r="C24" s="369"/>
       <c r="D24" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E24" s="50"/>
     </row>
     <row r="25" spans="3:8">
-      <c r="C25" s="336"/>
+      <c r="C25" s="369"/>
       <c r="D25" s="6" t="s">
         <v>12</v>
       </c>
       <c r="E25" s="50"/>
     </row>
     <row r="26" spans="3:8">
-      <c r="C26" s="337"/>
+      <c r="C26" s="370"/>
       <c r="D26" s="20" t="s">
         <v>31</v>
       </c>
       <c r="E26" s="53"/>
     </row>
     <row r="27" spans="3:8">
-      <c r="C27" s="330">
+      <c r="C27" s="354">
         <v>4</v>
       </c>
       <c r="D27" s="22" t="s">
@@ -9625,56 +9625,56 @@
       </c>
     </row>
     <row r="28" spans="3:8">
-      <c r="C28" s="331"/>
+      <c r="C28" s="355"/>
       <c r="D28" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E28" s="19"/>
     </row>
     <row r="29" spans="3:8">
-      <c r="C29" s="331"/>
+      <c r="C29" s="355"/>
       <c r="D29" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E29" s="19"/>
     </row>
     <row r="30" spans="3:8">
-      <c r="C30" s="331"/>
+      <c r="C30" s="355"/>
       <c r="D30" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E30" s="19"/>
     </row>
     <row r="31" spans="3:8">
-      <c r="C31" s="331"/>
+      <c r="C31" s="355"/>
       <c r="D31" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E31" s="19"/>
     </row>
     <row r="32" spans="3:8">
-      <c r="C32" s="331"/>
+      <c r="C32" s="355"/>
       <c r="D32" s="8" t="s">
         <v>18</v>
       </c>
       <c r="E32" s="19"/>
     </row>
     <row r="33" spans="2:7">
-      <c r="C33" s="331"/>
+      <c r="C33" s="355"/>
       <c r="D33" s="9" t="s">
         <v>19</v>
       </c>
       <c r="E33" s="19"/>
     </row>
     <row r="34" spans="2:7">
-      <c r="C34" s="332"/>
+      <c r="C34" s="361"/>
       <c r="D34" s="20" t="s">
         <v>32</v>
       </c>
       <c r="E34" s="21"/>
     </row>
     <row r="35" spans="2:7">
-      <c r="C35" s="327">
+      <c r="C35" s="360">
         <v>5</v>
       </c>
       <c r="D35" s="46" t="s">
@@ -9685,14 +9685,14 @@
       </c>
     </row>
     <row r="36" spans="2:7">
-      <c r="C36" s="328"/>
+      <c r="C36" s="358"/>
       <c r="D36" s="27" t="s">
         <v>21</v>
       </c>
       <c r="E36" s="48"/>
     </row>
     <row r="37" spans="2:7">
-      <c r="C37" s="328"/>
+      <c r="C37" s="358"/>
       <c r="D37" s="28" t="s">
         <v>22</v>
       </c>
@@ -9700,14 +9700,14 @@
       <c r="G37" s="30"/>
     </row>
     <row r="38" spans="2:7">
-      <c r="C38" s="329"/>
+      <c r="C38" s="365"/>
       <c r="D38" s="29" t="s">
         <v>23</v>
       </c>
       <c r="E38" s="49"/>
     </row>
     <row r="39" spans="2:7">
-      <c r="C39" s="330">
+      <c r="C39" s="354">
         <v>6</v>
       </c>
       <c r="D39" s="22" t="s">
@@ -9718,21 +9718,21 @@
       </c>
     </row>
     <row r="40" spans="2:7">
-      <c r="C40" s="331"/>
+      <c r="C40" s="355"/>
       <c r="D40" s="8" t="s">
         <v>25</v>
       </c>
       <c r="E40" s="19"/>
     </row>
     <row r="41" spans="2:7">
-      <c r="C41" s="332"/>
+      <c r="C41" s="361"/>
       <c r="D41" s="23" t="s">
         <v>26</v>
       </c>
       <c r="E41" s="21"/>
     </row>
     <row r="42" spans="2:7">
-      <c r="C42" s="333" t="s">
+      <c r="C42" s="366" t="s">
         <v>42</v>
       </c>
       <c r="D42" s="24" t="s">
@@ -9743,7 +9743,7 @@
       </c>
     </row>
     <row r="43" spans="2:7">
-      <c r="C43" s="334"/>
+      <c r="C43" s="367"/>
       <c r="D43" s="25" t="s">
         <v>44</v>
       </c>
@@ -9783,10 +9783,10 @@
       </c>
     </row>
     <row r="52" spans="2:5">
-      <c r="C52" s="340" t="s">
+      <c r="C52" s="364" t="s">
         <v>53</v>
       </c>
-      <c r="D52" s="340"/>
+      <c r="D52" s="364"/>
       <c r="E52" s="42"/>
     </row>
     <row r="53" spans="2:5">
@@ -9808,10 +9808,10 @@
       <c r="E54" s="40"/>
     </row>
     <row r="55" spans="2:5">
-      <c r="C55" s="338" t="s">
+      <c r="C55" s="362" t="s">
         <v>27</v>
       </c>
-      <c r="D55" s="339"/>
+      <c r="D55" s="363"/>
       <c r="E55" s="36"/>
     </row>
     <row r="56" spans="2:5">
@@ -9833,10 +9833,10 @@
       <c r="E57" s="40"/>
     </row>
     <row r="58" spans="2:5">
-      <c r="C58" s="338" t="s">
+      <c r="C58" s="362" t="s">
         <v>58</v>
       </c>
-      <c r="D58" s="339"/>
+      <c r="D58" s="363"/>
       <c r="E58" s="36"/>
     </row>
     <row r="59" spans="2:5">
@@ -9849,7 +9849,7 @@
       <c r="E59" s="37"/>
     </row>
     <row r="60" spans="2:5">
-      <c r="C60" s="331">
+      <c r="C60" s="355">
         <v>1</v>
       </c>
       <c r="D60" s="31" t="s">
@@ -9858,70 +9858,70 @@
       <c r="E60" s="19"/>
     </row>
     <row r="61" spans="2:5">
-      <c r="C61" s="331"/>
+      <c r="C61" s="355"/>
       <c r="D61" s="32" t="s">
         <v>60</v>
       </c>
       <c r="E61" s="19"/>
     </row>
     <row r="62" spans="2:5">
-      <c r="C62" s="331"/>
+      <c r="C62" s="355"/>
       <c r="D62" s="33" t="s">
         <v>61</v>
       </c>
       <c r="E62" s="21"/>
     </row>
     <row r="63" spans="2:5">
-      <c r="C63" s="331"/>
+      <c r="C63" s="355"/>
       <c r="D63" s="32" t="s">
         <v>62</v>
       </c>
       <c r="E63" s="18"/>
     </row>
     <row r="64" spans="2:5">
-      <c r="C64" s="331"/>
+      <c r="C64" s="355"/>
       <c r="D64" s="33" t="s">
         <v>28</v>
       </c>
       <c r="E64" s="19"/>
     </row>
     <row r="65" spans="3:5">
-      <c r="C65" s="331"/>
+      <c r="C65" s="355"/>
       <c r="D65" s="34" t="s">
         <v>63</v>
       </c>
       <c r="E65" s="21"/>
     </row>
     <row r="66" spans="3:5">
-      <c r="C66" s="331"/>
+      <c r="C66" s="355"/>
       <c r="D66" s="35" t="s">
         <v>64</v>
       </c>
       <c r="E66" s="18"/>
     </row>
     <row r="67" spans="3:5">
-      <c r="C67" s="331"/>
+      <c r="C67" s="355"/>
       <c r="D67" s="32" t="s">
         <v>65</v>
       </c>
       <c r="E67" s="19"/>
     </row>
     <row r="68" spans="3:5">
-      <c r="C68" s="331"/>
+      <c r="C68" s="355"/>
       <c r="D68" s="35" t="s">
         <v>66</v>
       </c>
       <c r="E68" s="21"/>
     </row>
     <row r="69" spans="3:5">
-      <c r="C69" s="332"/>
+      <c r="C69" s="361"/>
       <c r="D69" s="34" t="s">
         <v>29</v>
       </c>
       <c r="E69" s="18"/>
     </row>
     <row r="70" spans="3:5">
-      <c r="C70" s="327">
+      <c r="C70" s="360">
         <v>2</v>
       </c>
       <c r="D70" s="57" t="s">
@@ -9930,35 +9930,35 @@
       <c r="E70" s="47"/>
     </row>
     <row r="71" spans="3:5">
-      <c r="C71" s="328"/>
+      <c r="C71" s="358"/>
       <c r="D71" s="32" t="s">
         <v>67</v>
       </c>
       <c r="E71" s="48"/>
     </row>
     <row r="72" spans="3:5">
-      <c r="C72" s="328"/>
+      <c r="C72" s="358"/>
       <c r="D72" s="33" t="s">
         <v>68</v>
       </c>
       <c r="E72" s="48"/>
     </row>
     <row r="73" spans="3:5">
-      <c r="C73" s="328"/>
+      <c r="C73" s="358"/>
       <c r="D73" s="32" t="s">
         <v>69</v>
       </c>
       <c r="E73" s="48"/>
     </row>
     <row r="74" spans="3:5">
-      <c r="C74" s="328"/>
+      <c r="C74" s="358"/>
       <c r="D74" s="32" t="s">
         <v>134</v>
       </c>
       <c r="E74" s="49"/>
     </row>
     <row r="75" spans="3:5">
-      <c r="C75" s="330">
+      <c r="C75" s="354">
         <v>3</v>
       </c>
       <c r="D75" s="44" t="s">
@@ -9967,42 +9967,42 @@
       <c r="E75" s="18"/>
     </row>
     <row r="76" spans="3:5">
-      <c r="C76" s="331"/>
+      <c r="C76" s="355"/>
       <c r="D76" s="32" t="s">
         <v>71</v>
       </c>
       <c r="E76" s="19"/>
     </row>
     <row r="77" spans="3:5">
-      <c r="C77" s="331"/>
+      <c r="C77" s="355"/>
       <c r="D77" s="33" t="s">
         <v>72</v>
       </c>
       <c r="E77" s="21"/>
     </row>
     <row r="78" spans="3:5">
-      <c r="C78" s="331"/>
+      <c r="C78" s="355"/>
       <c r="D78" s="32" t="s">
         <v>73</v>
       </c>
       <c r="E78" s="18"/>
     </row>
     <row r="79" spans="3:5">
-      <c r="C79" s="331"/>
+      <c r="C79" s="355"/>
       <c r="D79" s="33" t="s">
         <v>74</v>
       </c>
       <c r="E79" s="19"/>
     </row>
     <row r="80" spans="3:5" ht="15.75" thickBot="1">
-      <c r="C80" s="341"/>
+      <c r="C80" s="356"/>
       <c r="D80" s="32" t="s">
         <v>75</v>
       </c>
       <c r="E80" s="21"/>
     </row>
     <row r="81" spans="3:5">
-      <c r="C81" s="342">
+      <c r="C81" s="357">
         <v>4</v>
       </c>
       <c r="D81" s="57" t="s">
@@ -10011,63 +10011,63 @@
       <c r="E81" s="48"/>
     </row>
     <row r="82" spans="3:5">
-      <c r="C82" s="328"/>
+      <c r="C82" s="358"/>
       <c r="D82" s="32" t="s">
         <v>77</v>
       </c>
       <c r="E82" s="48"/>
     </row>
     <row r="83" spans="3:5">
-      <c r="C83" s="328"/>
+      <c r="C83" s="358"/>
       <c r="D83" s="33" t="s">
         <v>78</v>
       </c>
       <c r="E83" s="48"/>
     </row>
     <row r="84" spans="3:5">
-      <c r="C84" s="328"/>
+      <c r="C84" s="358"/>
       <c r="D84" s="32" t="s">
         <v>79</v>
       </c>
       <c r="E84" s="48"/>
     </row>
     <row r="85" spans="3:5">
-      <c r="C85" s="328"/>
+      <c r="C85" s="358"/>
       <c r="D85" s="33" t="s">
         <v>80</v>
       </c>
       <c r="E85" s="48"/>
     </row>
     <row r="86" spans="3:5">
-      <c r="C86" s="328"/>
+      <c r="C86" s="358"/>
       <c r="D86" s="32" t="s">
         <v>137</v>
       </c>
       <c r="E86" s="48"/>
     </row>
     <row r="87" spans="3:5">
-      <c r="C87" s="328"/>
+      <c r="C87" s="358"/>
       <c r="D87" s="35" t="s">
         <v>81</v>
       </c>
       <c r="E87" s="48"/>
     </row>
     <row r="88" spans="3:5">
-      <c r="C88" s="328"/>
+      <c r="C88" s="358"/>
       <c r="D88" s="34" t="s">
         <v>82</v>
       </c>
       <c r="E88" s="48"/>
     </row>
     <row r="89" spans="3:5" ht="15.75" thickBot="1">
-      <c r="C89" s="343"/>
+      <c r="C89" s="359"/>
       <c r="D89" s="35" t="s">
         <v>83</v>
       </c>
       <c r="E89" s="48"/>
     </row>
     <row r="90" spans="3:5">
-      <c r="C90" s="330">
+      <c r="C90" s="354">
         <v>5</v>
       </c>
       <c r="D90" s="44" t="s">
@@ -10076,28 +10076,28 @@
       <c r="E90" s="18"/>
     </row>
     <row r="91" spans="3:5">
-      <c r="C91" s="331"/>
+      <c r="C91" s="355"/>
       <c r="D91" s="33" t="s">
         <v>85</v>
       </c>
       <c r="E91" s="19"/>
     </row>
     <row r="92" spans="3:5">
-      <c r="C92" s="331"/>
+      <c r="C92" s="355"/>
       <c r="D92" s="32" t="s">
         <v>86</v>
       </c>
       <c r="E92" s="21"/>
     </row>
     <row r="93" spans="3:5">
-      <c r="C93" s="331"/>
+      <c r="C93" s="355"/>
       <c r="D93" s="33" t="s">
         <v>87</v>
       </c>
       <c r="E93" s="18"/>
     </row>
     <row r="94" spans="3:5">
-      <c r="C94" s="327">
+      <c r="C94" s="360">
         <v>6</v>
       </c>
       <c r="D94" s="57" t="s">
@@ -10106,21 +10106,21 @@
       <c r="E94" s="48"/>
     </row>
     <row r="95" spans="3:5">
-      <c r="C95" s="328"/>
+      <c r="C95" s="358"/>
       <c r="D95" s="33" t="s">
         <v>89</v>
       </c>
       <c r="E95" s="48"/>
     </row>
     <row r="96" spans="3:5">
-      <c r="C96" s="328"/>
+      <c r="C96" s="358"/>
       <c r="D96" s="32" t="s">
         <v>90</v>
       </c>
       <c r="E96" s="48"/>
     </row>
     <row r="97" spans="3:5">
-      <c r="C97" s="330">
+      <c r="C97" s="354">
         <v>7</v>
       </c>
       <c r="D97" s="44" t="s">
@@ -10129,35 +10129,35 @@
       <c r="E97" s="18"/>
     </row>
     <row r="98" spans="3:5">
-      <c r="C98" s="331"/>
+      <c r="C98" s="355"/>
       <c r="D98" s="32" t="s">
         <v>92</v>
       </c>
       <c r="E98" s="18"/>
     </row>
     <row r="99" spans="3:5">
-      <c r="C99" s="331"/>
+      <c r="C99" s="355"/>
       <c r="D99" s="33" t="s">
         <v>93</v>
       </c>
       <c r="E99" s="18"/>
     </row>
     <row r="100" spans="3:5">
-      <c r="C100" s="331"/>
+      <c r="C100" s="355"/>
       <c r="D100" s="32" t="s">
         <v>94</v>
       </c>
       <c r="E100" s="18"/>
     </row>
     <row r="101" spans="3:5">
-      <c r="C101" s="332"/>
+      <c r="C101" s="361"/>
       <c r="D101" s="33" t="s">
         <v>95</v>
       </c>
       <c r="E101" s="18"/>
     </row>
     <row r="102" spans="3:5">
-      <c r="C102" s="327">
+      <c r="C102" s="360">
         <v>8</v>
       </c>
       <c r="D102" s="57" t="s">
@@ -10166,21 +10166,21 @@
       <c r="E102" s="48"/>
     </row>
     <row r="103" spans="3:5">
-      <c r="C103" s="328"/>
+      <c r="C103" s="358"/>
       <c r="D103" s="33" t="s">
         <v>97</v>
       </c>
       <c r="E103" s="48"/>
     </row>
     <row r="104" spans="3:5">
-      <c r="C104" s="328"/>
+      <c r="C104" s="358"/>
       <c r="D104" s="32" t="s">
         <v>98</v>
       </c>
       <c r="E104" s="48"/>
     </row>
     <row r="105" spans="3:5">
-      <c r="C105" s="330" t="s">
+      <c r="C105" s="354" t="s">
         <v>99</v>
       </c>
       <c r="D105" s="58" t="s">
@@ -10191,12 +10191,23 @@
       </c>
     </row>
     <row r="106" spans="3:5">
-      <c r="C106" s="331"/>
+      <c r="C106" s="355"/>
       <c r="D106" s="38"/>
       <c r="E106" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="C19:C26"/>
+    <mergeCell ref="C27:C34"/>
+    <mergeCell ref="C70:C74"/>
+    <mergeCell ref="C60:C69"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C52:D52"/>
     <mergeCell ref="C105:C106"/>
     <mergeCell ref="C75:C80"/>
     <mergeCell ref="C81:C89"/>
@@ -10204,17 +10215,6 @@
     <mergeCell ref="C94:C96"/>
     <mergeCell ref="C97:C101"/>
     <mergeCell ref="C102:C104"/>
-    <mergeCell ref="C70:C74"/>
-    <mergeCell ref="C60:C69"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="C19:C26"/>
-    <mergeCell ref="C27:C34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="44" orientation="portrait" r:id="rId1"/>
@@ -12748,12 +12748,12 @@
       <c r="C6" s="14"/>
     </row>
     <row r="7" spans="2:27" ht="18">
-      <c r="B7" s="344" t="s">
+      <c r="B7" s="371" t="s">
         <v>285</v>
       </c>
-      <c r="C7" s="344"/>
-      <c r="D7" s="344"/>
-      <c r="E7" s="344"/>
+      <c r="C7" s="371"/>
+      <c r="D7" s="371"/>
+      <c r="E7" s="371"/>
     </row>
     <row r="10" spans="2:27" s="107" customFormat="1" ht="12" customHeight="1">
       <c r="B10" s="117" t="s">
@@ -16929,12 +16929,12 @@
       <c r="C6" s="14"/>
     </row>
     <row r="7" spans="2:14" ht="18">
-      <c r="B7" s="344" t="s">
+      <c r="B7" s="371" t="s">
         <v>317</v>
       </c>
-      <c r="C7" s="344"/>
-      <c r="D7" s="344"/>
-      <c r="E7" s="344"/>
+      <c r="C7" s="371"/>
+      <c r="D7" s="371"/>
+      <c r="E7" s="371"/>
     </row>
     <row r="10" spans="2:14" s="107" customFormat="1" ht="12" customHeight="1">
       <c r="B10" s="117" t="s">
@@ -18550,12 +18550,12 @@
       <c r="C6" s="14"/>
     </row>
     <row r="7" spans="2:13" ht="18">
-      <c r="B7" s="344" t="s">
+      <c r="B7" s="371" t="s">
         <v>348</v>
       </c>
-      <c r="C7" s="344"/>
-      <c r="D7" s="344"/>
-      <c r="E7" s="344"/>
+      <c r="C7" s="371"/>
+      <c r="D7" s="371"/>
+      <c r="E7" s="371"/>
     </row>
     <row r="10" spans="2:13" s="107" customFormat="1" ht="12" customHeight="1">
       <c r="B10" s="275" t="s">
@@ -19819,12 +19819,12 @@
       <c r="C6" s="14"/>
     </row>
     <row r="7" spans="2:15" ht="18">
-      <c r="B7" s="344" t="s">
+      <c r="B7" s="371" t="s">
         <v>372</v>
       </c>
-      <c r="C7" s="344"/>
-      <c r="D7" s="344"/>
-      <c r="E7" s="344"/>
+      <c r="C7" s="371"/>
+      <c r="D7" s="371"/>
+      <c r="E7" s="371"/>
     </row>
     <row r="10" spans="2:15" s="107" customFormat="1" ht="12" customHeight="1">
       <c r="B10" s="275" t="s">
@@ -19907,10 +19907,10 @@
       <c r="M11" s="316">
         <v>0</v>
       </c>
-      <c r="N11" s="345">
-        <v>0</v>
-      </c>
-      <c r="O11" s="345">
+      <c r="N11" s="327">
+        <v>0</v>
+      </c>
+      <c r="O11" s="327">
         <v>0</v>
       </c>
     </row>
@@ -19931,8 +19931,8 @@
       <c r="K12" s="317"/>
       <c r="L12" s="317"/>
       <c r="M12" s="318"/>
-      <c r="N12" s="346"/>
-      <c r="O12" s="346"/>
+      <c r="N12" s="328"/>
+      <c r="O12" s="328"/>
     </row>
     <row r="13" spans="2:15">
       <c r="B13" s="291">
@@ -19971,10 +19971,10 @@
       <c r="M13" s="318">
         <v>0</v>
       </c>
-      <c r="N13" s="346">
-        <v>0</v>
-      </c>
-      <c r="O13" s="346">
+      <c r="N13" s="328">
+        <v>0</v>
+      </c>
+      <c r="O13" s="328">
         <v>0</v>
       </c>
     </row>
@@ -20015,10 +20015,10 @@
       <c r="M14" s="318">
         <v>1</v>
       </c>
-      <c r="N14" s="346">
-        <v>0</v>
-      </c>
-      <c r="O14" s="346">
+      <c r="N14" s="328">
+        <v>0</v>
+      </c>
+      <c r="O14" s="328">
         <v>0</v>
       </c>
     </row>
@@ -20059,10 +20059,10 @@
       <c r="M15" s="316">
         <v>2</v>
       </c>
-      <c r="N15" s="346">
+      <c r="N15" s="328">
         <v>2</v>
       </c>
-      <c r="O15" s="346">
+      <c r="O15" s="328">
         <v>2</v>
       </c>
     </row>
@@ -20083,8 +20083,8 @@
       <c r="K16" s="317"/>
       <c r="L16" s="317"/>
       <c r="M16" s="318"/>
-      <c r="N16" s="347"/>
-      <c r="O16" s="347"/>
+      <c r="N16" s="329"/>
+      <c r="O16" s="329"/>
     </row>
     <row r="17" spans="2:15" s="197" customFormat="1">
       <c r="B17" s="291">
@@ -20120,13 +20120,13 @@
       <c r="L17" s="317">
         <v>2</v>
       </c>
-      <c r="M17" s="349">
+      <c r="M17" s="331">
         <v>2</v>
       </c>
-      <c r="N17" s="350">
+      <c r="N17" s="332">
         <v>2</v>
       </c>
-      <c r="O17" s="350">
+      <c r="O17" s="332">
         <v>2</v>
       </c>
     </row>
@@ -20164,13 +20164,13 @@
       <c r="L18" s="317">
         <v>4</v>
       </c>
-      <c r="M18" s="349">
+      <c r="M18" s="331">
         <v>4</v>
       </c>
-      <c r="N18" s="350">
+      <c r="N18" s="332">
         <v>4</v>
       </c>
-      <c r="O18" s="350">
+      <c r="O18" s="332">
         <v>4</v>
       </c>
     </row>
@@ -20208,13 +20208,13 @@
       <c r="L19" s="326">
         <v>6</v>
       </c>
-      <c r="M19" s="351">
+      <c r="M19" s="333">
         <v>6</v>
       </c>
-      <c r="N19" s="350">
+      <c r="N19" s="332">
         <v>6</v>
       </c>
-      <c r="O19" s="350">
+      <c r="O19" s="332">
         <v>6</v>
       </c>
     </row>
@@ -20235,8 +20235,8 @@
       <c r="K20" s="314"/>
       <c r="L20" s="314"/>
       <c r="M20" s="316"/>
-      <c r="N20" s="346"/>
-      <c r="O20" s="346"/>
+      <c r="N20" s="328"/>
+      <c r="O20" s="328"/>
     </row>
     <row r="21" spans="2:15">
       <c r="B21" s="291">
@@ -20275,10 +20275,10 @@
       <c r="M21" s="316">
         <v>1</v>
       </c>
-      <c r="N21" s="346">
-        <v>0</v>
-      </c>
-      <c r="O21" s="346">
+      <c r="N21" s="328">
+        <v>0</v>
+      </c>
+      <c r="O21" s="328">
         <v>0</v>
       </c>
     </row>
@@ -20319,10 +20319,10 @@
       <c r="M22" s="316">
         <v>1</v>
       </c>
-      <c r="N22" s="346">
-        <v>0</v>
-      </c>
-      <c r="O22" s="346">
+      <c r="N22" s="328">
+        <v>0</v>
+      </c>
+      <c r="O22" s="328">
         <v>0</v>
       </c>
     </row>
@@ -20363,10 +20363,10 @@
       <c r="M23" s="316">
         <v>1</v>
       </c>
-      <c r="N23" s="346">
-        <v>0</v>
-      </c>
-      <c r="O23" s="346">
+      <c r="N23" s="328">
+        <v>0</v>
+      </c>
+      <c r="O23" s="328">
         <v>0</v>
       </c>
     </row>
@@ -20387,8 +20387,8 @@
       <c r="K24" s="317"/>
       <c r="L24" s="317"/>
       <c r="M24" s="318"/>
-      <c r="N24" s="346"/>
-      <c r="O24" s="346"/>
+      <c r="N24" s="328"/>
+      <c r="O24" s="328"/>
     </row>
     <row r="25" spans="2:15">
       <c r="B25" s="291">
@@ -20427,10 +20427,10 @@
       <c r="M25" s="318">
         <v>4</v>
       </c>
-      <c r="N25" s="346">
+      <c r="N25" s="328">
         <v>4</v>
       </c>
-      <c r="O25" s="346">
+      <c r="O25" s="328">
         <v>4</v>
       </c>
     </row>
@@ -20471,10 +20471,10 @@
       <c r="M26" s="318">
         <v>2</v>
       </c>
-      <c r="N26" s="346">
+      <c r="N26" s="328">
         <v>2</v>
       </c>
-      <c r="O26" s="346">
+      <c r="O26" s="328">
         <v>2</v>
       </c>
     </row>
@@ -20515,10 +20515,10 @@
       <c r="M27" s="318">
         <v>4</v>
       </c>
-      <c r="N27" s="346">
+      <c r="N27" s="328">
         <v>4</v>
       </c>
-      <c r="O27" s="346">
+      <c r="O27" s="328">
         <v>4</v>
       </c>
     </row>
@@ -20559,10 +20559,10 @@
       <c r="M28" s="318">
         <v>2</v>
       </c>
-      <c r="N28" s="346">
+      <c r="N28" s="328">
         <v>2</v>
       </c>
-      <c r="O28" s="346">
+      <c r="O28" s="328">
         <v>2</v>
       </c>
     </row>
@@ -20581,8 +20581,8 @@
       <c r="K29" s="319"/>
       <c r="L29" s="319"/>
       <c r="M29" s="320"/>
-      <c r="N29" s="346"/>
-      <c r="O29" s="346"/>
+      <c r="N29" s="328"/>
+      <c r="O29" s="328"/>
     </row>
     <row r="30" spans="2:15">
       <c r="B30" s="297">
@@ -20599,8 +20599,8 @@
       <c r="K30" s="314"/>
       <c r="L30" s="314"/>
       <c r="M30" s="316"/>
-      <c r="N30" s="346"/>
-      <c r="O30" s="346"/>
+      <c r="N30" s="328"/>
+      <c r="O30" s="328"/>
     </row>
     <row r="31" spans="2:15">
       <c r="B31" s="291">
@@ -20617,8 +20617,8 @@
       <c r="K31" s="319"/>
       <c r="L31" s="319"/>
       <c r="M31" s="320"/>
-      <c r="N31" s="346"/>
-      <c r="O31" s="346"/>
+      <c r="N31" s="328"/>
+      <c r="O31" s="328"/>
     </row>
     <row r="32" spans="2:15">
       <c r="B32" s="297">
@@ -20635,8 +20635,8 @@
       <c r="K32" s="314"/>
       <c r="L32" s="314"/>
       <c r="M32" s="316"/>
-      <c r="N32" s="346"/>
-      <c r="O32" s="346"/>
+      <c r="N32" s="328"/>
+      <c r="O32" s="328"/>
     </row>
     <row r="33" spans="2:15">
       <c r="B33" s="291">
@@ -20653,8 +20653,8 @@
       <c r="K33" s="319"/>
       <c r="L33" s="319"/>
       <c r="M33" s="320"/>
-      <c r="N33" s="346"/>
-      <c r="O33" s="346"/>
+      <c r="N33" s="328"/>
+      <c r="O33" s="328"/>
     </row>
     <row r="34" spans="2:15">
       <c r="B34" s="297">
@@ -20671,8 +20671,8 @@
       <c r="K34" s="319"/>
       <c r="L34" s="319"/>
       <c r="M34" s="320"/>
-      <c r="N34" s="346"/>
-      <c r="O34" s="346"/>
+      <c r="N34" s="328"/>
+      <c r="O34" s="328"/>
     </row>
     <row r="35" spans="2:15">
       <c r="B35" s="291">
@@ -20689,8 +20689,8 @@
       <c r="K35" s="314"/>
       <c r="L35" s="314"/>
       <c r="M35" s="316"/>
-      <c r="N35" s="346"/>
-      <c r="O35" s="346"/>
+      <c r="N35" s="328"/>
+      <c r="O35" s="328"/>
     </row>
     <row r="36" spans="2:15">
       <c r="B36" s="297">
@@ -20707,8 +20707,8 @@
       <c r="K36" s="314"/>
       <c r="L36" s="314"/>
       <c r="M36" s="316"/>
-      <c r="N36" s="346"/>
-      <c r="O36" s="346"/>
+      <c r="N36" s="328"/>
+      <c r="O36" s="328"/>
     </row>
     <row r="37" spans="2:15">
       <c r="B37" s="291">
@@ -20725,8 +20725,8 @@
       <c r="K37" s="314"/>
       <c r="L37" s="314"/>
       <c r="M37" s="316"/>
-      <c r="N37" s="346"/>
-      <c r="O37" s="346"/>
+      <c r="N37" s="328"/>
+      <c r="O37" s="328"/>
     </row>
     <row r="38" spans="2:15">
       <c r="B38" s="297">
@@ -20743,8 +20743,8 @@
       <c r="K38" s="314"/>
       <c r="L38" s="314"/>
       <c r="M38" s="316"/>
-      <c r="N38" s="346"/>
-      <c r="O38" s="346"/>
+      <c r="N38" s="328"/>
+      <c r="O38" s="328"/>
     </row>
     <row r="39" spans="2:15">
       <c r="B39" s="291">
@@ -20761,8 +20761,8 @@
       <c r="K39" s="314"/>
       <c r="L39" s="314"/>
       <c r="M39" s="316"/>
-      <c r="N39" s="346"/>
-      <c r="O39" s="346"/>
+      <c r="N39" s="328"/>
+      <c r="O39" s="328"/>
     </row>
     <row r="40" spans="2:15">
       <c r="B40" s="297">
@@ -20779,8 +20779,8 @@
       <c r="K40" s="314"/>
       <c r="L40" s="314"/>
       <c r="M40" s="316"/>
-      <c r="N40" s="346"/>
-      <c r="O40" s="346"/>
+      <c r="N40" s="328"/>
+      <c r="O40" s="328"/>
     </row>
     <row r="41" spans="2:15">
       <c r="B41" s="291">
@@ -20797,8 +20797,8 @@
       <c r="K41" s="314"/>
       <c r="L41" s="314"/>
       <c r="M41" s="316"/>
-      <c r="N41" s="346"/>
-      <c r="O41" s="346"/>
+      <c r="N41" s="328"/>
+      <c r="O41" s="328"/>
     </row>
     <row r="42" spans="2:15">
       <c r="B42" s="297">
@@ -20815,8 +20815,8 @@
       <c r="K42" s="314"/>
       <c r="L42" s="314"/>
       <c r="M42" s="316"/>
-      <c r="N42" s="346"/>
-      <c r="O42" s="346"/>
+      <c r="N42" s="328"/>
+      <c r="O42" s="328"/>
     </row>
     <row r="43" spans="2:15">
       <c r="B43" s="291">
@@ -20833,8 +20833,8 @@
       <c r="K43" s="314"/>
       <c r="L43" s="314"/>
       <c r="M43" s="316"/>
-      <c r="N43" s="346"/>
-      <c r="O43" s="346"/>
+      <c r="N43" s="328"/>
+      <c r="O43" s="328"/>
     </row>
     <row r="44" spans="2:15">
       <c r="B44" s="297">
@@ -20851,8 +20851,8 @@
       <c r="K44" s="314"/>
       <c r="L44" s="314"/>
       <c r="M44" s="316"/>
-      <c r="N44" s="346"/>
-      <c r="O44" s="346"/>
+      <c r="N44" s="328"/>
+      <c r="O44" s="328"/>
     </row>
     <row r="45" spans="2:15">
       <c r="B45" s="291">
@@ -20869,8 +20869,8 @@
       <c r="K45" s="314"/>
       <c r="L45" s="314"/>
       <c r="M45" s="316"/>
-      <c r="N45" s="346"/>
-      <c r="O45" s="346"/>
+      <c r="N45" s="328"/>
+      <c r="O45" s="328"/>
     </row>
     <row r="46" spans="2:15">
       <c r="B46" s="297">
@@ -20887,8 +20887,8 @@
       <c r="K46" s="314"/>
       <c r="L46" s="314"/>
       <c r="M46" s="316"/>
-      <c r="N46" s="346"/>
-      <c r="O46" s="346"/>
+      <c r="N46" s="328"/>
+      <c r="O46" s="328"/>
     </row>
     <row r="47" spans="2:15">
       <c r="B47" s="291">
@@ -20905,8 +20905,8 @@
       <c r="K47" s="314"/>
       <c r="L47" s="314"/>
       <c r="M47" s="316"/>
-      <c r="N47" s="346"/>
-      <c r="O47" s="346"/>
+      <c r="N47" s="328"/>
+      <c r="O47" s="328"/>
     </row>
     <row r="48" spans="2:15">
       <c r="B48" s="297">
@@ -20923,8 +20923,8 @@
       <c r="K48" s="314"/>
       <c r="L48" s="314"/>
       <c r="M48" s="316"/>
-      <c r="N48" s="346"/>
-      <c r="O48" s="346"/>
+      <c r="N48" s="328"/>
+      <c r="O48" s="328"/>
     </row>
     <row r="49" spans="2:15">
       <c r="B49" s="291">
@@ -20941,8 +20941,8 @@
       <c r="K49" s="314"/>
       <c r="L49" s="314"/>
       <c r="M49" s="316"/>
-      <c r="N49" s="346"/>
-      <c r="O49" s="346"/>
+      <c r="N49" s="328"/>
+      <c r="O49" s="328"/>
     </row>
     <row r="50" spans="2:15">
       <c r="B50" s="297">
@@ -20959,8 +20959,8 @@
       <c r="K50" s="314"/>
       <c r="L50" s="314"/>
       <c r="M50" s="316"/>
-      <c r="N50" s="346"/>
-      <c r="O50" s="346"/>
+      <c r="N50" s="328"/>
+      <c r="O50" s="328"/>
     </row>
     <row r="51" spans="2:15">
       <c r="B51" s="291">
@@ -20977,8 +20977,8 @@
       <c r="K51" s="314"/>
       <c r="L51" s="314"/>
       <c r="M51" s="316"/>
-      <c r="N51" s="346"/>
-      <c r="O51" s="346"/>
+      <c r="N51" s="328"/>
+      <c r="O51" s="328"/>
     </row>
     <row r="52" spans="2:15">
       <c r="B52" s="297">
@@ -20995,8 +20995,8 @@
       <c r="K52" s="314"/>
       <c r="L52" s="314"/>
       <c r="M52" s="316"/>
-      <c r="N52" s="346"/>
-      <c r="O52" s="346"/>
+      <c r="N52" s="328"/>
+      <c r="O52" s="328"/>
     </row>
     <row r="53" spans="2:15">
       <c r="B53" s="291">
@@ -21013,8 +21013,8 @@
       <c r="K53" s="313"/>
       <c r="L53" s="313"/>
       <c r="M53" s="323"/>
-      <c r="N53" s="346"/>
-      <c r="O53" s="346"/>
+      <c r="N53" s="328"/>
+      <c r="O53" s="328"/>
     </row>
     <row r="54" spans="2:15">
       <c r="B54" s="304" t="s">
@@ -21031,8 +21031,8 @@
       <c r="K54" s="324"/>
       <c r="L54" s="324"/>
       <c r="M54" s="325"/>
-      <c r="N54" s="348"/>
-      <c r="O54" s="348"/>
+      <c r="N54" s="330"/>
+      <c r="O54" s="330"/>
     </row>
     <row r="101" spans="2:15" s="97" customFormat="1">
       <c r="B101" t="s">
@@ -21344,7 +21344,7 @@
   <dimension ref="B2:O119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21382,12 +21382,12 @@
       <c r="C6" s="14"/>
     </row>
     <row r="7" spans="2:15" ht="18">
-      <c r="B7" s="344" t="s">
+      <c r="B7" s="371" t="s">
         <v>372</v>
       </c>
-      <c r="C7" s="344"/>
-      <c r="D7" s="344"/>
-      <c r="E7" s="344"/>
+      <c r="C7" s="371"/>
+      <c r="D7" s="371"/>
+      <c r="E7" s="371"/>
     </row>
     <row r="10" spans="2:15" s="107" customFormat="1" ht="12" customHeight="1">
       <c r="B10" s="275" t="s">
@@ -21434,16 +21434,16 @@
       </c>
     </row>
     <row r="11" spans="2:15">
-      <c r="B11" s="353">
+      <c r="B11" s="335">
         <v>1</v>
       </c>
-      <c r="C11" s="352" t="s">
+      <c r="C11" s="334" t="s">
         <v>373</v>
       </c>
       <c r="D11" s="289" t="s">
         <v>125</v>
       </c>
-      <c r="E11" s="354" t="s">
+      <c r="E11" s="336" t="s">
         <v>351</v>
       </c>
       <c r="F11" s="285" t="s">
@@ -21452,26 +21452,28 @@
       <c r="G11" s="321">
         <v>8</v>
       </c>
-      <c r="H11" s="326"/>
+      <c r="H11" s="326">
+        <v>6</v>
+      </c>
       <c r="I11" s="326"/>
       <c r="J11" s="326"/>
       <c r="K11" s="326"/>
       <c r="L11" s="326"/>
-      <c r="M11" s="351"/>
-      <c r="N11" s="355"/>
-      <c r="O11" s="355"/>
+      <c r="M11" s="333"/>
+      <c r="N11" s="337"/>
+      <c r="O11" s="337"/>
     </row>
     <row r="12" spans="2:15">
-      <c r="B12" s="356">
+      <c r="B12" s="338">
         <v>2</v>
       </c>
-      <c r="C12" s="352" t="s">
+      <c r="C12" s="334" t="s">
         <v>381</v>
       </c>
       <c r="D12" s="289" t="s">
         <v>125</v>
       </c>
-      <c r="E12" s="354" t="s">
+      <c r="E12" s="336" t="s">
         <v>351</v>
       </c>
       <c r="F12" s="285" t="s">
@@ -21480,46 +21482,48 @@
       <c r="G12" s="321">
         <v>2</v>
       </c>
-      <c r="H12" s="326"/>
-      <c r="I12" s="357"/>
-      <c r="J12" s="357"/>
-      <c r="K12" s="357"/>
-      <c r="L12" s="357"/>
-      <c r="M12" s="349"/>
-      <c r="N12" s="350"/>
-      <c r="O12" s="350"/>
+      <c r="H12" s="326">
+        <v>2</v>
+      </c>
+      <c r="I12" s="339"/>
+      <c r="J12" s="339"/>
+      <c r="K12" s="339"/>
+      <c r="L12" s="339"/>
+      <c r="M12" s="331"/>
+      <c r="N12" s="332"/>
+      <c r="O12" s="332"/>
     </row>
     <row r="13" spans="2:15">
-      <c r="B13" s="353">
+      <c r="B13" s="335">
         <v>3</v>
       </c>
-      <c r="C13" s="352" t="s">
+      <c r="C13" s="334" t="s">
         <v>358</v>
       </c>
       <c r="D13" s="289"/>
-      <c r="E13" s="354"/>
+      <c r="E13" s="336"/>
       <c r="F13" s="285"/>
       <c r="G13" s="321"/>
       <c r="H13" s="326"/>
-      <c r="I13" s="357"/>
-      <c r="J13" s="357"/>
-      <c r="K13" s="357"/>
-      <c r="L13" s="357"/>
-      <c r="M13" s="349"/>
-      <c r="N13" s="350"/>
-      <c r="O13" s="350"/>
+      <c r="I13" s="339"/>
+      <c r="J13" s="339"/>
+      <c r="K13" s="339"/>
+      <c r="L13" s="339"/>
+      <c r="M13" s="331"/>
+      <c r="N13" s="332"/>
+      <c r="O13" s="332"/>
     </row>
     <row r="14" spans="2:15">
-      <c r="B14" s="356">
+      <c r="B14" s="338">
         <v>4</v>
       </c>
-      <c r="C14" s="358" t="s">
+      <c r="C14" s="340" t="s">
         <v>382</v>
       </c>
       <c r="D14" s="289" t="s">
         <v>107</v>
       </c>
-      <c r="E14" s="354" t="s">
+      <c r="E14" s="336" t="s">
         <v>351</v>
       </c>
       <c r="F14" s="285" t="s">
@@ -21528,26 +21532,28 @@
       <c r="G14" s="321">
         <v>2</v>
       </c>
-      <c r="H14" s="326"/>
-      <c r="I14" s="357"/>
-      <c r="J14" s="357"/>
-      <c r="K14" s="357"/>
-      <c r="L14" s="357"/>
-      <c r="M14" s="349"/>
-      <c r="N14" s="350"/>
-      <c r="O14" s="350"/>
+      <c r="H14" s="326">
+        <v>2</v>
+      </c>
+      <c r="I14" s="339"/>
+      <c r="J14" s="339"/>
+      <c r="K14" s="339"/>
+      <c r="L14" s="339"/>
+      <c r="M14" s="331"/>
+      <c r="N14" s="332"/>
+      <c r="O14" s="332"/>
     </row>
     <row r="15" spans="2:15">
-      <c r="B15" s="353">
+      <c r="B15" s="335">
         <v>5</v>
       </c>
-      <c r="C15" s="358" t="s">
+      <c r="C15" s="340" t="s">
         <v>383</v>
       </c>
       <c r="D15" s="289" t="s">
         <v>107</v>
       </c>
-      <c r="E15" s="354" t="s">
+      <c r="E15" s="336" t="s">
         <v>351</v>
       </c>
       <c r="F15" s="285" t="s">
@@ -21556,46 +21562,48 @@
       <c r="G15" s="321">
         <v>4</v>
       </c>
-      <c r="H15" s="326"/>
-      <c r="I15" s="357"/>
-      <c r="J15" s="357"/>
-      <c r="K15" s="357"/>
+      <c r="H15" s="326">
+        <v>4</v>
+      </c>
+      <c r="I15" s="339"/>
+      <c r="J15" s="339"/>
+      <c r="K15" s="339"/>
       <c r="L15" s="326"/>
-      <c r="M15" s="351"/>
-      <c r="N15" s="350"/>
-      <c r="O15" s="350"/>
+      <c r="M15" s="333"/>
+      <c r="N15" s="332"/>
+      <c r="O15" s="332"/>
     </row>
     <row r="16" spans="2:15" s="197" customFormat="1">
-      <c r="B16" s="356">
+      <c r="B16" s="338">
         <v>6</v>
       </c>
-      <c r="C16" s="352" t="s">
+      <c r="C16" s="334" t="s">
         <v>359</v>
       </c>
       <c r="D16" s="289"/>
-      <c r="E16" s="354"/>
+      <c r="E16" s="336"/>
       <c r="F16" s="285"/>
       <c r="G16" s="321"/>
       <c r="H16" s="326"/>
-      <c r="I16" s="357"/>
-      <c r="J16" s="357"/>
-      <c r="K16" s="357"/>
-      <c r="L16" s="357"/>
-      <c r="M16" s="349"/>
-      <c r="N16" s="350"/>
-      <c r="O16" s="350"/>
+      <c r="I16" s="339"/>
+      <c r="J16" s="339"/>
+      <c r="K16" s="339"/>
+      <c r="L16" s="339"/>
+      <c r="M16" s="331"/>
+      <c r="N16" s="332"/>
+      <c r="O16" s="332"/>
     </row>
     <row r="17" spans="2:15" s="197" customFormat="1">
-      <c r="B17" s="353">
+      <c r="B17" s="335">
         <v>7</v>
       </c>
-      <c r="C17" s="358" t="s">
+      <c r="C17" s="340" t="s">
         <v>360</v>
       </c>
       <c r="D17" s="289" t="s">
         <v>107</v>
       </c>
-      <c r="E17" s="354" t="s">
+      <c r="E17" s="336" t="s">
         <v>349</v>
       </c>
       <c r="F17" s="285" t="s">
@@ -21604,26 +21612,28 @@
       <c r="G17" s="321">
         <v>2</v>
       </c>
-      <c r="H17" s="326"/>
-      <c r="I17" s="357"/>
-      <c r="J17" s="357"/>
-      <c r="K17" s="357"/>
-      <c r="L17" s="357"/>
-      <c r="M17" s="349"/>
-      <c r="N17" s="350"/>
-      <c r="O17" s="350"/>
+      <c r="H17" s="326">
+        <v>2</v>
+      </c>
+      <c r="I17" s="339"/>
+      <c r="J17" s="339"/>
+      <c r="K17" s="339"/>
+      <c r="L17" s="339"/>
+      <c r="M17" s="331"/>
+      <c r="N17" s="332"/>
+      <c r="O17" s="332"/>
     </row>
     <row r="18" spans="2:15" s="197" customFormat="1">
-      <c r="B18" s="356">
+      <c r="B18" s="338">
         <v>8</v>
       </c>
-      <c r="C18" s="358" t="s">
+      <c r="C18" s="340" t="s">
         <v>361</v>
       </c>
       <c r="D18" s="289" t="s">
         <v>107</v>
       </c>
-      <c r="E18" s="354" t="s">
+      <c r="E18" s="336" t="s">
         <v>349</v>
       </c>
       <c r="F18" s="285" t="s">
@@ -21632,26 +21642,28 @@
       <c r="G18" s="321">
         <v>4</v>
       </c>
-      <c r="H18" s="326"/>
-      <c r="I18" s="357"/>
-      <c r="J18" s="357"/>
-      <c r="K18" s="357"/>
-      <c r="L18" s="357"/>
-      <c r="M18" s="349"/>
-      <c r="N18" s="350"/>
-      <c r="O18" s="350"/>
+      <c r="H18" s="326">
+        <v>4</v>
+      </c>
+      <c r="I18" s="339"/>
+      <c r="J18" s="339"/>
+      <c r="K18" s="339"/>
+      <c r="L18" s="339"/>
+      <c r="M18" s="331"/>
+      <c r="N18" s="332"/>
+      <c r="O18" s="332"/>
     </row>
     <row r="19" spans="2:15" s="197" customFormat="1">
-      <c r="B19" s="353">
+      <c r="B19" s="335">
         <v>9</v>
       </c>
-      <c r="C19" s="358" t="s">
+      <c r="C19" s="340" t="s">
         <v>362</v>
       </c>
       <c r="D19" s="289" t="s">
         <v>107</v>
       </c>
-      <c r="E19" s="354" t="s">
+      <c r="E19" s="336" t="s">
         <v>349</v>
       </c>
       <c r="F19" s="285" t="s">
@@ -21660,26 +21672,28 @@
       <c r="G19" s="321">
         <v>6</v>
       </c>
-      <c r="H19" s="326"/>
-      <c r="I19" s="357"/>
-      <c r="J19" s="357"/>
+      <c r="H19" s="326">
+        <v>6</v>
+      </c>
+      <c r="I19" s="339"/>
+      <c r="J19" s="339"/>
       <c r="K19" s="326"/>
       <c r="L19" s="326"/>
-      <c r="M19" s="351"/>
-      <c r="N19" s="350"/>
-      <c r="O19" s="350"/>
+      <c r="M19" s="333"/>
+      <c r="N19" s="332"/>
+      <c r="O19" s="332"/>
     </row>
     <row r="20" spans="2:15">
-      <c r="B20" s="356">
+      <c r="B20" s="338">
         <v>10</v>
       </c>
-      <c r="C20" s="352" t="s">
+      <c r="C20" s="334" t="s">
         <v>384</v>
       </c>
       <c r="D20" s="289" t="s">
         <v>125</v>
       </c>
-      <c r="E20" s="354" t="s">
+      <c r="E20" s="336" t="s">
         <v>349</v>
       </c>
       <c r="F20" s="285" t="s">
@@ -21688,26 +21702,28 @@
       <c r="G20" s="321">
         <v>3</v>
       </c>
-      <c r="H20" s="321"/>
+      <c r="H20" s="321">
+        <v>0</v>
+      </c>
       <c r="I20" s="326"/>
       <c r="J20" s="326"/>
       <c r="K20" s="326"/>
       <c r="L20" s="326"/>
-      <c r="M20" s="351"/>
-      <c r="N20" s="350"/>
-      <c r="O20" s="350"/>
+      <c r="M20" s="333"/>
+      <c r="N20" s="332"/>
+      <c r="O20" s="332"/>
     </row>
     <row r="21" spans="2:15">
-      <c r="B21" s="353">
+      <c r="B21" s="335">
         <v>11</v>
       </c>
-      <c r="C21" s="352" t="s">
+      <c r="C21" s="334" t="s">
         <v>385</v>
       </c>
       <c r="D21" s="289" t="s">
         <v>125</v>
       </c>
-      <c r="E21" s="354" t="s">
+      <c r="E21" s="336" t="s">
         <v>349</v>
       </c>
       <c r="F21" s="285" t="s">
@@ -21716,46 +21732,48 @@
       <c r="G21" s="321">
         <v>3</v>
       </c>
-      <c r="H21" s="326"/>
+      <c r="H21" s="326">
+        <v>2</v>
+      </c>
       <c r="I21" s="326"/>
       <c r="J21" s="326"/>
       <c r="K21" s="326"/>
       <c r="L21" s="326"/>
-      <c r="M21" s="351"/>
-      <c r="N21" s="350"/>
-      <c r="O21" s="350"/>
+      <c r="M21" s="333"/>
+      <c r="N21" s="332"/>
+      <c r="O21" s="332"/>
     </row>
     <row r="22" spans="2:15">
-      <c r="B22" s="356">
+      <c r="B22" s="338">
         <v>12</v>
       </c>
-      <c r="C22" s="352" t="s">
+      <c r="C22" s="334" t="s">
         <v>367</v>
       </c>
       <c r="D22" s="289"/>
-      <c r="E22" s="354"/>
+      <c r="E22" s="336"/>
       <c r="F22" s="285"/>
       <c r="G22" s="321"/>
       <c r="H22" s="326"/>
-      <c r="I22" s="357"/>
-      <c r="J22" s="357"/>
-      <c r="K22" s="357"/>
-      <c r="L22" s="357"/>
-      <c r="M22" s="349"/>
-      <c r="N22" s="350"/>
-      <c r="O22" s="350"/>
+      <c r="I22" s="339"/>
+      <c r="J22" s="339"/>
+      <c r="K22" s="339"/>
+      <c r="L22" s="339"/>
+      <c r="M22" s="331"/>
+      <c r="N22" s="332"/>
+      <c r="O22" s="332"/>
     </row>
     <row r="23" spans="2:15">
-      <c r="B23" s="353">
+      <c r="B23" s="335">
         <v>13</v>
       </c>
-      <c r="C23" s="358" t="s">
+      <c r="C23" s="340" t="s">
         <v>368</v>
       </c>
       <c r="D23" s="289" t="s">
         <v>107</v>
       </c>
-      <c r="E23" s="354" t="s">
+      <c r="E23" s="336" t="s">
         <v>350</v>
       </c>
       <c r="F23" s="285" t="s">
@@ -21765,25 +21783,25 @@
         <v>5</v>
       </c>
       <c r="H23" s="326"/>
-      <c r="I23" s="357"/>
-      <c r="J23" s="357"/>
-      <c r="K23" s="357"/>
-      <c r="L23" s="357"/>
-      <c r="M23" s="349"/>
-      <c r="N23" s="350"/>
-      <c r="O23" s="350"/>
+      <c r="I23" s="339"/>
+      <c r="J23" s="339"/>
+      <c r="K23" s="339"/>
+      <c r="L23" s="339"/>
+      <c r="M23" s="331"/>
+      <c r="N23" s="332"/>
+      <c r="O23" s="332"/>
     </row>
     <row r="24" spans="2:15">
-      <c r="B24" s="356">
+      <c r="B24" s="338">
         <v>14</v>
       </c>
-      <c r="C24" s="359" t="s">
+      <c r="C24" s="341" t="s">
         <v>370</v>
       </c>
       <c r="D24" s="289" t="s">
         <v>107</v>
       </c>
-      <c r="E24" s="354" t="s">
+      <c r="E24" s="336" t="s">
         <v>350</v>
       </c>
       <c r="F24" s="285" t="s">
@@ -21793,25 +21811,25 @@
         <v>2</v>
       </c>
       <c r="H24" s="326"/>
-      <c r="I24" s="357"/>
-      <c r="J24" s="357"/>
-      <c r="K24" s="357"/>
-      <c r="L24" s="357"/>
-      <c r="M24" s="349"/>
-      <c r="N24" s="350"/>
-      <c r="O24" s="350"/>
+      <c r="I24" s="339"/>
+      <c r="J24" s="339"/>
+      <c r="K24" s="339"/>
+      <c r="L24" s="339"/>
+      <c r="M24" s="331"/>
+      <c r="N24" s="332"/>
+      <c r="O24" s="332"/>
     </row>
     <row r="25" spans="2:15">
-      <c r="B25" s="353">
+      <c r="B25" s="335">
         <v>15</v>
       </c>
-      <c r="C25" s="358" t="s">
+      <c r="C25" s="340" t="s">
         <v>369</v>
       </c>
       <c r="D25" s="289" t="s">
         <v>107</v>
       </c>
-      <c r="E25" s="354" t="s">
+      <c r="E25" s="336" t="s">
         <v>350</v>
       </c>
       <c r="F25" s="285" t="s">
@@ -21821,25 +21839,25 @@
         <v>5</v>
       </c>
       <c r="H25" s="326"/>
-      <c r="I25" s="357"/>
-      <c r="J25" s="357"/>
-      <c r="K25" s="357"/>
-      <c r="L25" s="357"/>
-      <c r="M25" s="349"/>
-      <c r="N25" s="350"/>
-      <c r="O25" s="350"/>
+      <c r="I25" s="339"/>
+      <c r="J25" s="339"/>
+      <c r="K25" s="339"/>
+      <c r="L25" s="339"/>
+      <c r="M25" s="331"/>
+      <c r="N25" s="332"/>
+      <c r="O25" s="332"/>
     </row>
     <row r="26" spans="2:15">
-      <c r="B26" s="356">
+      <c r="B26" s="338">
         <v>16</v>
       </c>
-      <c r="C26" s="359" t="s">
+      <c r="C26" s="341" t="s">
         <v>371</v>
       </c>
       <c r="D26" s="289" t="s">
         <v>107</v>
       </c>
-      <c r="E26" s="354" t="s">
+      <c r="E26" s="336" t="s">
         <v>350</v>
       </c>
       <c r="F26" s="285" t="s">
@@ -21849,45 +21867,45 @@
         <v>2</v>
       </c>
       <c r="H26" s="326"/>
-      <c r="I26" s="357"/>
-      <c r="J26" s="357"/>
-      <c r="K26" s="357"/>
-      <c r="L26" s="357"/>
-      <c r="M26" s="349"/>
-      <c r="N26" s="350"/>
-      <c r="O26" s="350"/>
+      <c r="I26" s="339"/>
+      <c r="J26" s="339"/>
+      <c r="K26" s="339"/>
+      <c r="L26" s="339"/>
+      <c r="M26" s="331"/>
+      <c r="N26" s="332"/>
+      <c r="O26" s="332"/>
     </row>
     <row r="27" spans="2:15">
-      <c r="B27" s="353">
+      <c r="B27" s="335">
         <v>17</v>
       </c>
-      <c r="C27" s="352" t="s">
+      <c r="C27" s="334" t="s">
         <v>359</v>
       </c>
       <c r="D27" s="289"/>
-      <c r="E27" s="354"/>
+      <c r="E27" s="336"/>
       <c r="F27" s="285"/>
       <c r="G27" s="321"/>
       <c r="H27" s="326"/>
-      <c r="I27" s="357"/>
-      <c r="J27" s="357"/>
-      <c r="K27" s="357"/>
-      <c r="L27" s="357"/>
-      <c r="M27" s="349"/>
-      <c r="N27" s="350"/>
-      <c r="O27" s="350"/>
+      <c r="I27" s="339"/>
+      <c r="J27" s="339"/>
+      <c r="K27" s="339"/>
+      <c r="L27" s="339"/>
+      <c r="M27" s="331"/>
+      <c r="N27" s="332"/>
+      <c r="O27" s="332"/>
     </row>
     <row r="28" spans="2:15">
-      <c r="B28" s="356">
+      <c r="B28" s="338">
         <v>18</v>
       </c>
-      <c r="C28" s="359" t="s">
+      <c r="C28" s="341" t="s">
         <v>386</v>
       </c>
       <c r="D28" s="289" t="s">
         <v>107</v>
       </c>
-      <c r="E28" s="354" t="s">
+      <c r="E28" s="336" t="s">
         <v>350</v>
       </c>
       <c r="F28" s="285" t="s">
@@ -21897,23 +21915,23 @@
         <v>4</v>
       </c>
       <c r="H28" s="326"/>
-      <c r="I28" s="357"/>
-      <c r="J28" s="357"/>
-      <c r="K28" s="357"/>
-      <c r="L28" s="357"/>
-      <c r="M28" s="349"/>
-      <c r="N28" s="350"/>
-      <c r="O28" s="350"/>
+      <c r="I28" s="339"/>
+      <c r="J28" s="339"/>
+      <c r="K28" s="339"/>
+      <c r="L28" s="339"/>
+      <c r="M28" s="331"/>
+      <c r="N28" s="332"/>
+      <c r="O28" s="332"/>
     </row>
     <row r="29" spans="2:15">
-      <c r="B29" s="353">
+      <c r="B29" s="335">
         <v>19</v>
       </c>
-      <c r="C29" s="352" t="s">
+      <c r="C29" s="334" t="s">
         <v>388</v>
       </c>
       <c r="D29" s="289"/>
-      <c r="E29" s="354"/>
+      <c r="E29" s="336"/>
       <c r="F29" s="285"/>
       <c r="G29" s="321"/>
       <c r="H29" s="326"/>
@@ -21921,21 +21939,21 @@
       <c r="J29" s="326"/>
       <c r="K29" s="326"/>
       <c r="L29" s="326"/>
-      <c r="M29" s="351"/>
-      <c r="N29" s="350"/>
-      <c r="O29" s="350"/>
+      <c r="M29" s="333"/>
+      <c r="N29" s="332"/>
+      <c r="O29" s="332"/>
     </row>
     <row r="30" spans="2:15">
-      <c r="B30" s="356">
+      <c r="B30" s="338">
         <v>20</v>
       </c>
-      <c r="C30" s="358" t="s">
+      <c r="C30" s="340" t="s">
         <v>387</v>
       </c>
       <c r="D30" s="289" t="s">
         <v>107</v>
       </c>
-      <c r="E30" s="354" t="s">
+      <c r="E30" s="336" t="s">
         <v>352</v>
       </c>
       <c r="F30" s="285" t="s">
@@ -21944,26 +21962,30 @@
       <c r="G30" s="321">
         <v>5</v>
       </c>
-      <c r="H30" s="326"/>
-      <c r="I30" s="326"/>
+      <c r="H30" s="326">
+        <v>3</v>
+      </c>
+      <c r="I30" s="326">
+        <v>0</v>
+      </c>
       <c r="J30" s="326"/>
       <c r="K30" s="326"/>
       <c r="L30" s="326"/>
-      <c r="M30" s="351"/>
-      <c r="N30" s="350"/>
-      <c r="O30" s="350"/>
+      <c r="M30" s="333"/>
+      <c r="N30" s="332"/>
+      <c r="O30" s="332"/>
     </row>
     <row r="31" spans="2:15">
-      <c r="B31" s="353">
+      <c r="B31" s="335">
         <v>21</v>
       </c>
-      <c r="C31" s="359" t="s">
+      <c r="C31" s="341" t="s">
         <v>391</v>
       </c>
       <c r="D31" s="289" t="s">
         <v>107</v>
       </c>
-      <c r="E31" s="354" t="s">
+      <c r="E31" s="336" t="s">
         <v>352</v>
       </c>
       <c r="F31" s="285" t="s">
@@ -21977,21 +21999,21 @@
       <c r="J31" s="326"/>
       <c r="K31" s="326"/>
       <c r="L31" s="326"/>
-      <c r="M31" s="351"/>
-      <c r="N31" s="350"/>
-      <c r="O31" s="350"/>
+      <c r="M31" s="333"/>
+      <c r="N31" s="332"/>
+      <c r="O31" s="332"/>
     </row>
     <row r="32" spans="2:15">
-      <c r="B32" s="356">
+      <c r="B32" s="338">
         <v>22</v>
       </c>
-      <c r="C32" s="358" t="s">
+      <c r="C32" s="340" t="s">
         <v>389</v>
       </c>
       <c r="D32" s="289" t="s">
         <v>107</v>
       </c>
-      <c r="E32" s="354" t="s">
+      <c r="E32" s="336" t="s">
         <v>352</v>
       </c>
       <c r="F32" s="285" t="s">
@@ -22005,21 +22027,21 @@
       <c r="J32" s="326"/>
       <c r="K32" s="326"/>
       <c r="L32" s="326"/>
-      <c r="M32" s="351"/>
-      <c r="N32" s="350"/>
-      <c r="O32" s="350"/>
+      <c r="M32" s="333"/>
+      <c r="N32" s="332"/>
+      <c r="O32" s="332"/>
     </row>
     <row r="33" spans="2:15">
-      <c r="B33" s="353">
+      <c r="B33" s="335">
         <v>23</v>
       </c>
-      <c r="C33" s="358" t="s">
+      <c r="C33" s="340" t="s">
         <v>390</v>
       </c>
       <c r="D33" s="289" t="s">
         <v>107</v>
       </c>
-      <c r="E33" s="354" t="s">
+      <c r="E33" s="336" t="s">
         <v>352</v>
       </c>
       <c r="F33" s="285" t="s">
@@ -22033,17 +22055,17 @@
       <c r="J33" s="326"/>
       <c r="K33" s="326"/>
       <c r="L33" s="326"/>
-      <c r="M33" s="351"/>
-      <c r="N33" s="350"/>
-      <c r="O33" s="350"/>
+      <c r="M33" s="333"/>
+      <c r="N33" s="332"/>
+      <c r="O33" s="332"/>
     </row>
     <row r="34" spans="2:15">
-      <c r="B34" s="356">
+      <c r="B34" s="338">
         <v>24</v>
       </c>
-      <c r="C34" s="360"/>
+      <c r="C34" s="342"/>
       <c r="D34" s="289"/>
-      <c r="E34" s="354"/>
+      <c r="E34" s="336"/>
       <c r="F34" s="285"/>
       <c r="G34" s="321"/>
       <c r="H34" s="326"/>
@@ -22051,17 +22073,17 @@
       <c r="J34" s="326"/>
       <c r="K34" s="326"/>
       <c r="L34" s="326"/>
-      <c r="M34" s="351"/>
-      <c r="N34" s="350"/>
-      <c r="O34" s="350"/>
+      <c r="M34" s="333"/>
+      <c r="N34" s="332"/>
+      <c r="O34" s="332"/>
     </row>
     <row r="35" spans="2:15">
-      <c r="B35" s="353">
+      <c r="B35" s="335">
         <v>25</v>
       </c>
-      <c r="C35" s="360"/>
+      <c r="C35" s="342"/>
       <c r="D35" s="289"/>
-      <c r="E35" s="354"/>
+      <c r="E35" s="336"/>
       <c r="F35" s="285"/>
       <c r="G35" s="321"/>
       <c r="H35" s="326"/>
@@ -22069,17 +22091,17 @@
       <c r="J35" s="326"/>
       <c r="K35" s="326"/>
       <c r="L35" s="326"/>
-      <c r="M35" s="351"/>
-      <c r="N35" s="350"/>
-      <c r="O35" s="350"/>
+      <c r="M35" s="333"/>
+      <c r="N35" s="332"/>
+      <c r="O35" s="332"/>
     </row>
     <row r="36" spans="2:15">
-      <c r="B36" s="356">
+      <c r="B36" s="338">
         <v>26</v>
       </c>
-      <c r="C36" s="354"/>
+      <c r="C36" s="336"/>
       <c r="D36" s="289"/>
-      <c r="E36" s="354"/>
+      <c r="E36" s="336"/>
       <c r="F36" s="285"/>
       <c r="G36" s="321"/>
       <c r="H36" s="326"/>
@@ -22087,17 +22109,17 @@
       <c r="J36" s="326"/>
       <c r="K36" s="326"/>
       <c r="L36" s="326"/>
-      <c r="M36" s="351"/>
-      <c r="N36" s="350"/>
-      <c r="O36" s="350"/>
+      <c r="M36" s="333"/>
+      <c r="N36" s="332"/>
+      <c r="O36" s="332"/>
     </row>
     <row r="37" spans="2:15">
-      <c r="B37" s="353">
+      <c r="B37" s="335">
         <v>27</v>
       </c>
-      <c r="C37" s="354"/>
+      <c r="C37" s="336"/>
       <c r="D37" s="289"/>
-      <c r="E37" s="354"/>
+      <c r="E37" s="336"/>
       <c r="F37" s="285"/>
       <c r="G37" s="321"/>
       <c r="H37" s="326"/>
@@ -22105,17 +22127,17 @@
       <c r="J37" s="326"/>
       <c r="K37" s="326"/>
       <c r="L37" s="326"/>
-      <c r="M37" s="351"/>
-      <c r="N37" s="350"/>
-      <c r="O37" s="350"/>
+      <c r="M37" s="333"/>
+      <c r="N37" s="332"/>
+      <c r="O37" s="332"/>
     </row>
     <row r="38" spans="2:15">
-      <c r="B38" s="356">
+      <c r="B38" s="338">
         <v>28</v>
       </c>
-      <c r="C38" s="354"/>
+      <c r="C38" s="336"/>
       <c r="D38" s="289"/>
-      <c r="E38" s="354"/>
+      <c r="E38" s="336"/>
       <c r="F38" s="285"/>
       <c r="G38" s="321"/>
       <c r="H38" s="326"/>
@@ -22123,17 +22145,17 @@
       <c r="J38" s="326"/>
       <c r="K38" s="326"/>
       <c r="L38" s="326"/>
-      <c r="M38" s="351"/>
-      <c r="N38" s="350"/>
-      <c r="O38" s="350"/>
+      <c r="M38" s="333"/>
+      <c r="N38" s="332"/>
+      <c r="O38" s="332"/>
     </row>
     <row r="39" spans="2:15">
-      <c r="B39" s="353">
+      <c r="B39" s="335">
         <v>29</v>
       </c>
-      <c r="C39" s="361"/>
+      <c r="C39" s="343"/>
       <c r="D39" s="289"/>
-      <c r="E39" s="354"/>
+      <c r="E39" s="336"/>
       <c r="F39" s="285"/>
       <c r="G39" s="321"/>
       <c r="H39" s="326"/>
@@ -22141,17 +22163,17 @@
       <c r="J39" s="326"/>
       <c r="K39" s="326"/>
       <c r="L39" s="326"/>
-      <c r="M39" s="351"/>
-      <c r="N39" s="350"/>
-      <c r="O39" s="350"/>
+      <c r="M39" s="333"/>
+      <c r="N39" s="332"/>
+      <c r="O39" s="332"/>
     </row>
     <row r="40" spans="2:15">
-      <c r="B40" s="356">
+      <c r="B40" s="338">
         <v>30</v>
       </c>
-      <c r="C40" s="361"/>
+      <c r="C40" s="343"/>
       <c r="D40" s="289"/>
-      <c r="E40" s="354"/>
+      <c r="E40" s="336"/>
       <c r="F40" s="285"/>
       <c r="G40" s="321"/>
       <c r="H40" s="326"/>
@@ -22159,17 +22181,17 @@
       <c r="J40" s="326"/>
       <c r="K40" s="326"/>
       <c r="L40" s="326"/>
-      <c r="M40" s="351"/>
-      <c r="N40" s="350"/>
-      <c r="O40" s="350"/>
+      <c r="M40" s="333"/>
+      <c r="N40" s="332"/>
+      <c r="O40" s="332"/>
     </row>
     <row r="41" spans="2:15">
-      <c r="B41" s="353">
+      <c r="B41" s="335">
         <v>31</v>
       </c>
-      <c r="C41" s="361"/>
+      <c r="C41" s="343"/>
       <c r="D41" s="289"/>
-      <c r="E41" s="354"/>
+      <c r="E41" s="336"/>
       <c r="F41" s="285"/>
       <c r="G41" s="321"/>
       <c r="H41" s="326"/>
@@ -22177,17 +22199,17 @@
       <c r="J41" s="326"/>
       <c r="K41" s="326"/>
       <c r="L41" s="326"/>
-      <c r="M41" s="351"/>
-      <c r="N41" s="350"/>
-      <c r="O41" s="350"/>
+      <c r="M41" s="333"/>
+      <c r="N41" s="332"/>
+      <c r="O41" s="332"/>
     </row>
     <row r="42" spans="2:15">
-      <c r="B42" s="356">
+      <c r="B42" s="338">
         <v>32</v>
       </c>
-      <c r="C42" s="361"/>
+      <c r="C42" s="343"/>
       <c r="D42" s="289"/>
-      <c r="E42" s="354"/>
+      <c r="E42" s="336"/>
       <c r="F42" s="285"/>
       <c r="G42" s="321"/>
       <c r="H42" s="326"/>
@@ -22195,17 +22217,17 @@
       <c r="J42" s="326"/>
       <c r="K42" s="326"/>
       <c r="L42" s="326"/>
-      <c r="M42" s="351"/>
-      <c r="N42" s="350"/>
-      <c r="O42" s="350"/>
+      <c r="M42" s="333"/>
+      <c r="N42" s="332"/>
+      <c r="O42" s="332"/>
     </row>
     <row r="43" spans="2:15">
-      <c r="B43" s="353">
+      <c r="B43" s="335">
         <v>33</v>
       </c>
-      <c r="C43" s="361"/>
+      <c r="C43" s="343"/>
       <c r="D43" s="289"/>
-      <c r="E43" s="354"/>
+      <c r="E43" s="336"/>
       <c r="F43" s="285"/>
       <c r="G43" s="321"/>
       <c r="H43" s="326"/>
@@ -22213,17 +22235,17 @@
       <c r="J43" s="326"/>
       <c r="K43" s="326"/>
       <c r="L43" s="326"/>
-      <c r="M43" s="351"/>
-      <c r="N43" s="350"/>
-      <c r="O43" s="350"/>
+      <c r="M43" s="333"/>
+      <c r="N43" s="332"/>
+      <c r="O43" s="332"/>
     </row>
     <row r="44" spans="2:15">
-      <c r="B44" s="356">
+      <c r="B44" s="338">
         <v>34</v>
       </c>
-      <c r="C44" s="358"/>
+      <c r="C44" s="340"/>
       <c r="D44" s="289"/>
-      <c r="E44" s="354"/>
+      <c r="E44" s="336"/>
       <c r="F44" s="285"/>
       <c r="G44" s="321"/>
       <c r="H44" s="326"/>
@@ -22231,17 +22253,17 @@
       <c r="J44" s="326"/>
       <c r="K44" s="326"/>
       <c r="L44" s="326"/>
-      <c r="M44" s="351"/>
-      <c r="N44" s="350"/>
-      <c r="O44" s="350"/>
+      <c r="M44" s="333"/>
+      <c r="N44" s="332"/>
+      <c r="O44" s="332"/>
     </row>
     <row r="45" spans="2:15">
-      <c r="B45" s="353">
+      <c r="B45" s="335">
         <v>35</v>
       </c>
-      <c r="C45" s="361"/>
+      <c r="C45" s="343"/>
       <c r="D45" s="289"/>
-      <c r="E45" s="354"/>
+      <c r="E45" s="336"/>
       <c r="F45" s="285"/>
       <c r="G45" s="321"/>
       <c r="H45" s="326"/>
@@ -22249,17 +22271,17 @@
       <c r="J45" s="326"/>
       <c r="K45" s="326"/>
       <c r="L45" s="326"/>
-      <c r="M45" s="351"/>
-      <c r="N45" s="350"/>
-      <c r="O45" s="350"/>
+      <c r="M45" s="333"/>
+      <c r="N45" s="332"/>
+      <c r="O45" s="332"/>
     </row>
     <row r="46" spans="2:15">
-      <c r="B46" s="356">
+      <c r="B46" s="338">
         <v>36</v>
       </c>
-      <c r="C46" s="361"/>
+      <c r="C46" s="343"/>
       <c r="D46" s="289"/>
-      <c r="E46" s="354"/>
+      <c r="E46" s="336"/>
       <c r="F46" s="285"/>
       <c r="G46" s="321"/>
       <c r="H46" s="326"/>
@@ -22267,17 +22289,17 @@
       <c r="J46" s="326"/>
       <c r="K46" s="326"/>
       <c r="L46" s="326"/>
-      <c r="M46" s="351"/>
-      <c r="N46" s="350"/>
-      <c r="O46" s="350"/>
+      <c r="M46" s="333"/>
+      <c r="N46" s="332"/>
+      <c r="O46" s="332"/>
     </row>
     <row r="47" spans="2:15">
-      <c r="B47" s="353">
+      <c r="B47" s="335">
         <v>37</v>
       </c>
-      <c r="C47" s="361"/>
+      <c r="C47" s="343"/>
       <c r="D47" s="289"/>
-      <c r="E47" s="354"/>
+      <c r="E47" s="336"/>
       <c r="F47" s="285"/>
       <c r="G47" s="321"/>
       <c r="H47" s="326"/>
@@ -22285,17 +22307,17 @@
       <c r="J47" s="326"/>
       <c r="K47" s="326"/>
       <c r="L47" s="326"/>
-      <c r="M47" s="351"/>
-      <c r="N47" s="350"/>
-      <c r="O47" s="350"/>
+      <c r="M47" s="333"/>
+      <c r="N47" s="332"/>
+      <c r="O47" s="332"/>
     </row>
     <row r="48" spans="2:15">
-      <c r="B48" s="356">
+      <c r="B48" s="338">
         <v>38</v>
       </c>
-      <c r="C48" s="361"/>
+      <c r="C48" s="343"/>
       <c r="D48" s="289"/>
-      <c r="E48" s="354"/>
+      <c r="E48" s="336"/>
       <c r="F48" s="285"/>
       <c r="G48" s="321"/>
       <c r="H48" s="326"/>
@@ -22303,17 +22325,17 @@
       <c r="J48" s="326"/>
       <c r="K48" s="326"/>
       <c r="L48" s="326"/>
-      <c r="M48" s="351"/>
-      <c r="N48" s="350"/>
-      <c r="O48" s="350"/>
+      <c r="M48" s="333"/>
+      <c r="N48" s="332"/>
+      <c r="O48" s="332"/>
     </row>
     <row r="49" spans="2:15">
-      <c r="B49" s="353">
+      <c r="B49" s="335">
         <v>39</v>
       </c>
-      <c r="C49" s="358"/>
+      <c r="C49" s="340"/>
       <c r="D49" s="289"/>
-      <c r="E49" s="354"/>
+      <c r="E49" s="336"/>
       <c r="F49" s="285"/>
       <c r="G49" s="321"/>
       <c r="H49" s="326"/>
@@ -22321,17 +22343,17 @@
       <c r="J49" s="326"/>
       <c r="K49" s="326"/>
       <c r="L49" s="326"/>
-      <c r="M49" s="351"/>
-      <c r="N49" s="350"/>
-      <c r="O49" s="350"/>
+      <c r="M49" s="333"/>
+      <c r="N49" s="332"/>
+      <c r="O49" s="332"/>
     </row>
     <row r="50" spans="2:15">
-      <c r="B50" s="356">
+      <c r="B50" s="338">
         <v>40</v>
       </c>
-      <c r="C50" s="358"/>
+      <c r="C50" s="340"/>
       <c r="D50" s="289"/>
-      <c r="E50" s="354"/>
+      <c r="E50" s="336"/>
       <c r="F50" s="285"/>
       <c r="G50" s="321"/>
       <c r="H50" s="326"/>
@@ -22339,17 +22361,17 @@
       <c r="J50" s="326"/>
       <c r="K50" s="326"/>
       <c r="L50" s="326"/>
-      <c r="M50" s="351"/>
-      <c r="N50" s="350"/>
-      <c r="O50" s="350"/>
+      <c r="M50" s="333"/>
+      <c r="N50" s="332"/>
+      <c r="O50" s="332"/>
     </row>
     <row r="51" spans="2:15">
-      <c r="B51" s="353">
+      <c r="B51" s="335">
         <v>41</v>
       </c>
-      <c r="C51" s="358"/>
+      <c r="C51" s="340"/>
       <c r="D51" s="289"/>
-      <c r="E51" s="354"/>
+      <c r="E51" s="336"/>
       <c r="F51" s="285"/>
       <c r="G51" s="321"/>
       <c r="H51" s="326"/>
@@ -22357,17 +22379,17 @@
       <c r="J51" s="326"/>
       <c r="K51" s="326"/>
       <c r="L51" s="326"/>
-      <c r="M51" s="351"/>
-      <c r="N51" s="350"/>
-      <c r="O51" s="350"/>
+      <c r="M51" s="333"/>
+      <c r="N51" s="332"/>
+      <c r="O51" s="332"/>
     </row>
     <row r="52" spans="2:15">
-      <c r="B52" s="356">
+      <c r="B52" s="338">
         <v>42</v>
       </c>
-      <c r="C52" s="358"/>
+      <c r="C52" s="340"/>
       <c r="D52" s="289"/>
-      <c r="E52" s="354"/>
+      <c r="E52" s="336"/>
       <c r="F52" s="285"/>
       <c r="G52" s="321"/>
       <c r="H52" s="326"/>
@@ -22375,17 +22397,17 @@
       <c r="J52" s="326"/>
       <c r="K52" s="326"/>
       <c r="L52" s="326"/>
-      <c r="M52" s="351"/>
-      <c r="N52" s="350"/>
-      <c r="O52" s="350"/>
+      <c r="M52" s="333"/>
+      <c r="N52" s="332"/>
+      <c r="O52" s="332"/>
     </row>
     <row r="53" spans="2:15">
-      <c r="B53" s="353">
+      <c r="B53" s="335">
         <v>43</v>
       </c>
-      <c r="C53" s="362"/>
+      <c r="C53" s="344"/>
       <c r="D53" s="289"/>
-      <c r="E53" s="354"/>
+      <c r="E53" s="336"/>
       <c r="F53" s="285"/>
       <c r="G53" s="321"/>
       <c r="H53" s="321"/>
@@ -22393,27 +22415,27 @@
       <c r="J53" s="321"/>
       <c r="K53" s="321"/>
       <c r="L53" s="321"/>
-      <c r="M53" s="363"/>
-      <c r="N53" s="350"/>
-      <c r="O53" s="350"/>
+      <c r="M53" s="345"/>
+      <c r="N53" s="332"/>
+      <c r="O53" s="332"/>
     </row>
     <row r="54" spans="2:15">
-      <c r="B54" s="364" t="s">
+      <c r="B54" s="346" t="s">
         <v>136</v>
       </c>
-      <c r="C54" s="365"/>
-      <c r="D54" s="366"/>
-      <c r="E54" s="367"/>
-      <c r="F54" s="368"/>
-      <c r="G54" s="369"/>
-      <c r="H54" s="369"/>
-      <c r="I54" s="369"/>
-      <c r="J54" s="369"/>
-      <c r="K54" s="369"/>
-      <c r="L54" s="369"/>
-      <c r="M54" s="370"/>
-      <c r="N54" s="371"/>
-      <c r="O54" s="371"/>
+      <c r="C54" s="347"/>
+      <c r="D54" s="348"/>
+      <c r="E54" s="349"/>
+      <c r="F54" s="350"/>
+      <c r="G54" s="351"/>
+      <c r="H54" s="351"/>
+      <c r="I54" s="351"/>
+      <c r="J54" s="351"/>
+      <c r="K54" s="351"/>
+      <c r="L54" s="351"/>
+      <c r="M54" s="352"/>
+      <c r="N54" s="353"/>
+      <c r="O54" s="353"/>
     </row>
     <row r="101" spans="2:15" s="97" customFormat="1">
       <c r="B101" t="s">

</xml_diff>

<commit_message>
Done IMPORT QUESTION function
</commit_message>
<xml_diff>
--- a/Documents/ProductBackLog/Capstone_Group6_ProductBackLog_SprintTaskList.xlsx
+++ b/Documents/ProductBackLog/Capstone_Group6_ProductBackLog_SprintTaskList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4680" firstSheet="6" activeTab="8"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4680" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="2" r:id="rId1"/>
@@ -311,17 +311,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Tu Huynh:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Sprint 2</t>
+          <t>Tu Huynh:May Span TWO Sprint</t>
         </r>
       </text>
     </comment>
@@ -333,7 +323,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>Tu Huynh:</t>
         </r>
@@ -342,10 +332,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Sprint 2</t>
+Sprint 3</t>
         </r>
       </text>
     </comment>
@@ -369,7 +359,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Sprint 2</t>
+Sprint 3</t>
         </r>
       </text>
     </comment>
@@ -381,7 +371,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>Tu Huynh:</t>
         </r>
@@ -390,10 +380,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Sprint 2</t>
+Sprint 3 of ThiBT</t>
         </r>
       </text>
     </comment>
@@ -417,7 +407,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Sprint 2</t>
+Sprint 3</t>
         </r>
       </text>
     </comment>
@@ -441,7 +431,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Sprint 2</t>
+Sprint 3</t>
         </r>
       </text>
     </comment>
@@ -465,7 +455,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Sprint 2</t>
+Sprint 3</t>
         </r>
       </text>
     </comment>
@@ -489,7 +479,79 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Sprint 2</t>
+Sprint 3</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G30" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tu Huynh:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Sprint 3</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G31" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tu Huynh:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Sprint 3</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G32" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tu Huynh:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Sprint 3</t>
         </r>
       </text>
     </comment>
@@ -498,7 +560,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="410">
   <si>
     <t>Introduction</t>
   </si>
@@ -1717,6 +1779,45 @@
   <si>
     <t>Report 3- User Requirement Specify</t>
   </si>
+  <si>
+    <t>Do Test</t>
+  </si>
+  <si>
+    <t>+Do Test Layout</t>
+  </si>
+  <si>
+    <t>27/05</t>
+  </si>
+  <si>
+    <t>28/05</t>
+  </si>
+  <si>
+    <t>29/05</t>
+  </si>
+  <si>
+    <t>30/05</t>
+  </si>
+  <si>
+    <t>31/05</t>
+  </si>
+  <si>
+    <t>01/06</t>
+  </si>
+  <si>
+    <t>02/05</t>
+  </si>
+  <si>
+    <t>+Do Test Function</t>
+  </si>
+  <si>
+    <t>List upcoming Tests</t>
+  </si>
+  <si>
+    <t>+Appointment UnAssign for teacher/student</t>
+  </si>
+  <si>
+    <t>+Invite User outside of system</t>
+  </si>
 </sst>
 </file>
 
@@ -1726,7 +1827,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="dd/mm"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1875,6 +1976,28 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="23">
@@ -2536,7 +2659,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="372">
+  <cellXfs count="386">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -3616,6 +3739,46 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="29" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="29" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="29" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="29" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9910,13 +10073,13 @@
     <tableColumn id="4" name="Assign To" dataDxfId="15"/>
     <tableColumn id="5" name="Status" dataDxfId="14"/>
     <tableColumn id="7" name="Estimate" dataDxfId="13"/>
-    <tableColumn id="8" name="20/05" dataDxfId="12"/>
-    <tableColumn id="9" name="21/05" dataDxfId="11"/>
-    <tableColumn id="10" name="22/05" dataDxfId="10"/>
-    <tableColumn id="11" name="23/05" dataDxfId="9"/>
-    <tableColumn id="12" name="24/05" dataDxfId="8"/>
-    <tableColumn id="13" name="25/05" dataDxfId="7"/>
-    <tableColumn id="14" name="26/05" dataDxfId="6"/>
+    <tableColumn id="8" name="27/05" dataDxfId="12"/>
+    <tableColumn id="9" name="28/05" dataDxfId="11"/>
+    <tableColumn id="10" name="29/05" dataDxfId="10"/>
+    <tableColumn id="11" name="30/05" dataDxfId="9"/>
+    <tableColumn id="12" name="31/05" dataDxfId="8"/>
+    <tableColumn id="13" name="01/06" dataDxfId="7"/>
+    <tableColumn id="14" name="02/05" dataDxfId="6"/>
     <tableColumn id="15" name="End" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -11015,8 +11178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:O119"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11081,25 +11244,25 @@
         <v>347</v>
       </c>
       <c r="H10" s="272" t="s">
-        <v>374</v>
+        <v>399</v>
       </c>
       <c r="I10" s="272" t="s">
-        <v>375</v>
+        <v>400</v>
       </c>
       <c r="J10" s="273" t="s">
-        <v>376</v>
+        <v>401</v>
       </c>
       <c r="K10" s="273" t="s">
-        <v>377</v>
+        <v>402</v>
       </c>
       <c r="L10" s="273" t="s">
-        <v>378</v>
+        <v>403</v>
       </c>
       <c r="M10" s="273" t="s">
-        <v>379</v>
+        <v>404</v>
       </c>
       <c r="N10" s="274" t="s">
-        <v>380</v>
+        <v>405</v>
       </c>
       <c r="O10" s="311" t="s">
         <v>284</v>
@@ -11122,88 +11285,56 @@
         <v>117</v>
       </c>
       <c r="G11" s="321">
-        <v>5</v>
-      </c>
-      <c r="H11" s="326">
-        <v>4</v>
-      </c>
-      <c r="I11" s="326">
-        <v>4</v>
-      </c>
-      <c r="J11" s="326">
-        <v>4</v>
-      </c>
-      <c r="K11" s="326">
-        <v>3</v>
-      </c>
-      <c r="L11" s="326">
-        <v>2</v>
-      </c>
-      <c r="M11" s="333">
-        <v>0</v>
-      </c>
-      <c r="N11" s="337">
-        <v>0</v>
-      </c>
-      <c r="O11" s="337">
-        <v>0</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="H11" s="326"/>
+      <c r="I11" s="326"/>
+      <c r="J11" s="326"/>
+      <c r="K11" s="326"/>
+      <c r="L11" s="326"/>
+      <c r="M11" s="333"/>
+      <c r="N11" s="337"/>
+      <c r="O11" s="337"/>
     </row>
     <row r="12" spans="2:15">
       <c r="B12" s="338">
         <v>2</v>
       </c>
       <c r="C12" s="334" t="s">
-        <v>381</v>
-      </c>
-      <c r="D12" s="289" t="s">
-        <v>125</v>
-      </c>
-      <c r="E12" s="336" t="s">
-        <v>351</v>
-      </c>
-      <c r="F12" s="285" t="s">
-        <v>117</v>
-      </c>
-      <c r="G12" s="321">
-        <v>5</v>
-      </c>
-      <c r="H12" s="326">
-        <v>4</v>
-      </c>
-      <c r="I12" s="339">
-        <v>3</v>
-      </c>
-      <c r="J12" s="339">
-        <v>3</v>
-      </c>
-      <c r="K12" s="339">
-        <v>2</v>
-      </c>
-      <c r="L12" s="339">
-        <v>0</v>
-      </c>
-      <c r="M12" s="331">
-        <v>0</v>
-      </c>
-      <c r="N12" s="332">
-        <v>0</v>
-      </c>
-      <c r="O12" s="332">
-        <v>0</v>
-      </c>
+        <v>397</v>
+      </c>
+      <c r="D12" s="289"/>
+      <c r="E12" s="336"/>
+      <c r="F12" s="285"/>
+      <c r="G12" s="321"/>
+      <c r="H12" s="326"/>
+      <c r="I12" s="339"/>
+      <c r="J12" s="339"/>
+      <c r="K12" s="339"/>
+      <c r="L12" s="339"/>
+      <c r="M12" s="331"/>
+      <c r="N12" s="332"/>
+      <c r="O12" s="332"/>
     </row>
     <row r="13" spans="2:15">
       <c r="B13" s="335">
         <v>3</v>
       </c>
-      <c r="C13" s="334" t="s">
-        <v>358</v>
-      </c>
-      <c r="D13" s="289"/>
-      <c r="E13" s="336"/>
-      <c r="F13" s="285"/>
-      <c r="G13" s="321"/>
+      <c r="C13" s="340" t="s">
+        <v>398</v>
+      </c>
+      <c r="D13" s="289" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="336" t="s">
+        <v>351</v>
+      </c>
+      <c r="F13" s="285" t="s">
+        <v>117</v>
+      </c>
+      <c r="G13" s="321">
+        <v>15</v>
+      </c>
       <c r="H13" s="326"/>
       <c r="I13" s="339"/>
       <c r="J13" s="339"/>
@@ -11218,7 +11349,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="340" t="s">
-        <v>382</v>
+        <v>406</v>
       </c>
       <c r="D14" s="289" t="s">
         <v>107</v>
@@ -11230,76 +11361,44 @@
         <v>117</v>
       </c>
       <c r="G14" s="321">
-        <v>20</v>
-      </c>
-      <c r="H14" s="326">
-        <v>18</v>
-      </c>
-      <c r="I14" s="339">
-        <v>15</v>
-      </c>
-      <c r="J14" s="339">
-        <v>12</v>
-      </c>
-      <c r="K14" s="339">
-        <v>10</v>
-      </c>
-      <c r="L14" s="339">
-        <v>7</v>
-      </c>
-      <c r="M14" s="331">
-        <v>4</v>
-      </c>
-      <c r="N14" s="332">
-        <v>0</v>
-      </c>
-      <c r="O14" s="332">
-        <v>0</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="H14" s="326"/>
+      <c r="I14" s="339"/>
+      <c r="J14" s="339"/>
+      <c r="K14" s="339"/>
+      <c r="L14" s="339"/>
+      <c r="M14" s="331"/>
+      <c r="N14" s="332"/>
+      <c r="O14" s="332"/>
     </row>
     <row r="15" spans="2:15">
       <c r="B15" s="335">
         <v>5</v>
       </c>
-      <c r="C15" s="340" t="s">
-        <v>383</v>
-      </c>
-      <c r="D15" s="289" t="s">
+      <c r="C15" s="384" t="s">
+        <v>407</v>
+      </c>
+      <c r="D15" s="375" t="s">
         <v>107</v>
       </c>
-      <c r="E15" s="336" t="s">
+      <c r="E15" s="373" t="s">
         <v>351</v>
       </c>
-      <c r="F15" s="285" t="s">
+      <c r="F15" s="375" t="s">
         <v>117</v>
       </c>
-      <c r="G15" s="321">
-        <v>20</v>
-      </c>
-      <c r="H15" s="326">
-        <v>18</v>
-      </c>
-      <c r="I15" s="339">
-        <v>15</v>
-      </c>
-      <c r="J15" s="339">
+      <c r="G15" s="378">
         <v>10</v>
       </c>
-      <c r="K15" s="339">
-        <v>8</v>
-      </c>
-      <c r="L15" s="326">
-        <v>5</v>
-      </c>
-      <c r="M15" s="333">
-        <v>3</v>
-      </c>
-      <c r="N15" s="332">
-        <v>0</v>
-      </c>
-      <c r="O15" s="332">
-        <v>0</v>
-      </c>
+      <c r="H15" s="326"/>
+      <c r="I15" s="339"/>
+      <c r="J15" s="339"/>
+      <c r="K15" s="339"/>
+      <c r="L15" s="326"/>
+      <c r="M15" s="333"/>
+      <c r="N15" s="332"/>
+      <c r="O15" s="332"/>
     </row>
     <row r="16" spans="2:15" s="197" customFormat="1">
       <c r="B16" s="338">
@@ -11325,8 +11424,8 @@
       <c r="B17" s="335">
         <v>7</v>
       </c>
-      <c r="C17" s="340" t="s">
-        <v>360</v>
+      <c r="C17" s="372" t="s">
+        <v>361</v>
       </c>
       <c r="D17" s="289" t="s">
         <v>107</v>
@@ -11338,120 +11437,72 @@
         <v>117</v>
       </c>
       <c r="G17" s="321">
-        <v>15</v>
-      </c>
-      <c r="H17" s="326">
-        <v>12</v>
-      </c>
-      <c r="I17" s="339">
         <v>10</v>
       </c>
-      <c r="J17" s="339">
-        <v>8</v>
-      </c>
-      <c r="K17" s="339">
-        <v>6</v>
-      </c>
-      <c r="L17" s="339">
-        <v>5</v>
-      </c>
-      <c r="M17" s="331">
-        <v>3</v>
-      </c>
-      <c r="N17" s="332">
-        <v>0</v>
-      </c>
-      <c r="O17" s="332">
-        <v>0</v>
-      </c>
+      <c r="H17" s="326"/>
+      <c r="I17" s="339"/>
+      <c r="J17" s="339"/>
+      <c r="K17" s="339"/>
+      <c r="L17" s="339"/>
+      <c r="M17" s="331"/>
+      <c r="N17" s="332"/>
+      <c r="O17" s="332"/>
     </row>
     <row r="18" spans="2:15" s="197" customFormat="1">
       <c r="B18" s="338">
         <v>8</v>
       </c>
-      <c r="C18" s="340" t="s">
-        <v>361</v>
-      </c>
-      <c r="D18" s="289" t="s">
+      <c r="C18" s="372" t="s">
+        <v>362</v>
+      </c>
+      <c r="D18" s="374" t="s">
         <v>107</v>
       </c>
-      <c r="E18" s="336" t="s">
+      <c r="E18" s="376" t="s">
         <v>349</v>
       </c>
-      <c r="F18" s="285" t="s">
+      <c r="F18" s="377" t="s">
         <v>117</v>
       </c>
       <c r="G18" s="321">
-        <v>10</v>
-      </c>
-      <c r="H18" s="326">
-        <v>10</v>
-      </c>
-      <c r="I18" s="339">
-        <v>10</v>
-      </c>
-      <c r="J18" s="339">
-        <v>10</v>
-      </c>
-      <c r="K18" s="339">
-        <v>10</v>
-      </c>
-      <c r="L18" s="339">
-        <v>10</v>
-      </c>
-      <c r="M18" s="331">
-        <v>10</v>
-      </c>
-      <c r="N18" s="332">
-        <v>10</v>
-      </c>
-      <c r="O18" s="332">
-        <v>10</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="H18" s="326"/>
+      <c r="I18" s="339"/>
+      <c r="J18" s="339"/>
+      <c r="K18" s="339"/>
+      <c r="L18" s="339"/>
+      <c r="M18" s="331"/>
+      <c r="N18" s="332"/>
+      <c r="O18" s="332"/>
     </row>
     <row r="19" spans="2:15" s="197" customFormat="1">
       <c r="B19" s="335">
         <v>9</v>
       </c>
-      <c r="C19" s="340" t="s">
-        <v>362</v>
-      </c>
-      <c r="D19" s="289" t="s">
+      <c r="C19" s="341" t="s">
+        <v>386</v>
+      </c>
+      <c r="D19" s="375" t="s">
         <v>107</v>
       </c>
-      <c r="E19" s="336" t="s">
+      <c r="E19" s="373" t="s">
         <v>349</v>
       </c>
-      <c r="F19" s="285" t="s">
+      <c r="F19" s="375" t="s">
         <v>117</v>
       </c>
-      <c r="G19" s="321">
-        <v>15</v>
-      </c>
-      <c r="H19" s="326">
-        <v>15</v>
-      </c>
-      <c r="I19" s="339">
-        <v>15</v>
-      </c>
-      <c r="J19" s="339">
-        <v>15</v>
-      </c>
-      <c r="K19" s="326">
-        <v>15</v>
-      </c>
-      <c r="L19" s="326">
-        <v>15</v>
-      </c>
-      <c r="M19" s="333">
-        <v>15</v>
-      </c>
-      <c r="N19" s="332">
-        <v>15</v>
-      </c>
-      <c r="O19" s="332">
-        <v>15</v>
-      </c>
+      <c r="G19" s="378">
+        <v>12</v>
+      </c>
+      <c r="H19" s="326"/>
+      <c r="I19" s="339"/>
+      <c r="J19" s="339"/>
+      <c r="K19" s="326"/>
+      <c r="L19" s="326"/>
+      <c r="M19" s="333"/>
+      <c r="N19" s="332"/>
+      <c r="O19" s="332"/>
     </row>
     <row r="20" spans="2:15">
       <c r="B20" s="338">
@@ -11460,42 +11511,26 @@
       <c r="C20" s="334" t="s">
         <v>395</v>
       </c>
-      <c r="D20" s="289" t="s">
+      <c r="D20" s="375" t="s">
         <v>125</v>
       </c>
-      <c r="E20" s="336" t="s">
+      <c r="E20" s="373" t="s">
         <v>349</v>
       </c>
-      <c r="F20" s="285" t="s">
+      <c r="F20" s="375" t="s">
         <v>117</v>
       </c>
       <c r="G20" s="321">
         <v>10</v>
       </c>
-      <c r="H20" s="321">
-        <v>8</v>
-      </c>
-      <c r="I20" s="326">
-        <v>6</v>
-      </c>
-      <c r="J20" s="326">
-        <v>4</v>
-      </c>
-      <c r="K20" s="326">
-        <v>3</v>
-      </c>
-      <c r="L20" s="326">
-        <v>0</v>
-      </c>
-      <c r="M20" s="333">
-        <v>0</v>
-      </c>
-      <c r="N20" s="332">
-        <v>0</v>
-      </c>
-      <c r="O20" s="332">
-        <v>0</v>
-      </c>
+      <c r="H20" s="321"/>
+      <c r="I20" s="326"/>
+      <c r="J20" s="326"/>
+      <c r="K20" s="326"/>
+      <c r="L20" s="326"/>
+      <c r="M20" s="333"/>
+      <c r="N20" s="332"/>
+      <c r="O20" s="332"/>
     </row>
     <row r="21" spans="2:15">
       <c r="B21" s="335">
@@ -11514,32 +11549,16 @@
         <v>117</v>
       </c>
       <c r="G21" s="321">
-        <v>10</v>
-      </c>
-      <c r="H21" s="326">
-        <v>8</v>
-      </c>
-      <c r="I21" s="326">
-        <v>6</v>
-      </c>
-      <c r="J21" s="326">
-        <v>3</v>
-      </c>
-      <c r="K21" s="326">
-        <v>2</v>
-      </c>
-      <c r="L21" s="326">
-        <v>0</v>
-      </c>
-      <c r="M21" s="333">
-        <v>0</v>
-      </c>
-      <c r="N21" s="332">
-        <v>0</v>
-      </c>
-      <c r="O21" s="332">
-        <v>0</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="H21" s="326"/>
+      <c r="I21" s="326"/>
+      <c r="J21" s="326"/>
+      <c r="K21" s="326"/>
+      <c r="L21" s="326"/>
+      <c r="M21" s="333"/>
+      <c r="N21" s="332"/>
+      <c r="O21" s="332"/>
     </row>
     <row r="22" spans="2:15">
       <c r="B22" s="338">
@@ -11548,10 +11567,10 @@
       <c r="C22" s="334" t="s">
         <v>367</v>
       </c>
-      <c r="D22" s="289"/>
-      <c r="E22" s="336"/>
-      <c r="F22" s="285"/>
-      <c r="G22" s="321"/>
+      <c r="D22" s="375"/>
+      <c r="E22" s="373"/>
+      <c r="F22" s="375"/>
+      <c r="G22" s="378"/>
       <c r="H22" s="326"/>
       <c r="I22" s="339"/>
       <c r="J22" s="339"/>
@@ -11578,176 +11597,120 @@
         <v>117</v>
       </c>
       <c r="G23" s="321">
-        <v>12</v>
-      </c>
-      <c r="H23" s="326">
-        <v>12</v>
-      </c>
-      <c r="I23" s="339">
-        <v>12</v>
-      </c>
-      <c r="J23" s="339">
-        <v>11</v>
-      </c>
-      <c r="K23" s="339">
-        <v>11</v>
-      </c>
-      <c r="L23" s="339">
         <v>10</v>
       </c>
-      <c r="M23" s="331">
-        <v>10</v>
-      </c>
-      <c r="N23" s="332">
-        <v>10</v>
-      </c>
-      <c r="O23" s="332">
-        <v>10</v>
-      </c>
+      <c r="H23" s="380"/>
+      <c r="I23" s="382"/>
+      <c r="J23" s="382"/>
+      <c r="K23" s="382"/>
+      <c r="L23" s="382"/>
+      <c r="M23" s="382"/>
+      <c r="N23" s="383"/>
+      <c r="O23" s="383"/>
     </row>
     <row r="24" spans="2:15">
       <c r="B24" s="338">
         <v>14</v>
       </c>
-      <c r="C24" s="341" t="s">
+      <c r="C24" s="379" t="s">
         <v>370</v>
       </c>
-      <c r="D24" s="289" t="s">
+      <c r="D24" s="374" t="s">
         <v>107</v>
       </c>
-      <c r="E24" s="336" t="s">
+      <c r="E24" s="376" t="s">
         <v>350</v>
       </c>
-      <c r="F24" s="285" t="s">
+      <c r="F24" s="377" t="s">
         <v>117</v>
       </c>
-      <c r="G24" s="321">
+      <c r="G24" s="378">
         <v>12</v>
       </c>
-      <c r="H24" s="326">
-        <v>12</v>
-      </c>
-      <c r="I24" s="339">
-        <v>12</v>
-      </c>
-      <c r="J24" s="339">
-        <v>12</v>
-      </c>
-      <c r="K24" s="339">
-        <v>12</v>
-      </c>
-      <c r="L24" s="339">
-        <v>12</v>
-      </c>
-      <c r="M24" s="331">
-        <v>12</v>
-      </c>
-      <c r="N24" s="332">
-        <v>12</v>
-      </c>
-      <c r="O24" s="332">
-        <v>12</v>
-      </c>
+      <c r="H24" s="380"/>
+      <c r="I24" s="382"/>
+      <c r="J24" s="382"/>
+      <c r="K24" s="382"/>
+      <c r="L24" s="382"/>
+      <c r="M24" s="382"/>
+      <c r="N24" s="383"/>
+      <c r="O24" s="383"/>
     </row>
     <row r="25" spans="2:15">
       <c r="B25" s="335">
         <v>15</v>
       </c>
-      <c r="C25" s="340" t="s">
+      <c r="C25" s="372" t="s">
         <v>369</v>
       </c>
-      <c r="D25" s="289" t="s">
+      <c r="D25" s="374" t="s">
         <v>107</v>
       </c>
-      <c r="E25" s="336" t="s">
+      <c r="E25" s="376" t="s">
         <v>350</v>
       </c>
-      <c r="F25" s="285" t="s">
+      <c r="F25" s="377" t="s">
         <v>117</v>
       </c>
-      <c r="G25" s="321">
-        <v>12</v>
-      </c>
-      <c r="H25" s="326">
-        <v>12</v>
-      </c>
-      <c r="I25" s="339">
-        <v>12</v>
-      </c>
-      <c r="J25" s="339">
-        <v>11</v>
-      </c>
-      <c r="K25" s="339">
-        <v>11</v>
-      </c>
-      <c r="L25" s="339">
+      <c r="G25" s="378">
         <v>10</v>
       </c>
-      <c r="M25" s="331">
-        <v>10</v>
-      </c>
-      <c r="N25" s="332">
-        <v>10</v>
-      </c>
-      <c r="O25" s="332">
-        <v>10</v>
-      </c>
+      <c r="H25" s="380"/>
+      <c r="I25" s="382"/>
+      <c r="J25" s="382"/>
+      <c r="K25" s="382"/>
+      <c r="L25" s="382"/>
+      <c r="M25" s="382"/>
+      <c r="N25" s="383"/>
+      <c r="O25" s="383"/>
     </row>
     <row r="26" spans="2:15">
       <c r="B26" s="338">
         <v>16</v>
       </c>
-      <c r="C26" s="341" t="s">
+      <c r="C26" s="379" t="s">
         <v>371</v>
       </c>
-      <c r="D26" s="289" t="s">
+      <c r="D26" s="374" t="s">
         <v>107</v>
       </c>
-      <c r="E26" s="336" t="s">
+      <c r="E26" s="376" t="s">
         <v>350</v>
       </c>
-      <c r="F26" s="285" t="s">
+      <c r="F26" s="377" t="s">
         <v>117</v>
       </c>
-      <c r="G26" s="321">
+      <c r="G26" s="378">
         <v>12</v>
       </c>
-      <c r="H26" s="326">
-        <v>12</v>
-      </c>
-      <c r="I26" s="339">
-        <v>12</v>
-      </c>
-      <c r="J26" s="339">
-        <v>12</v>
-      </c>
-      <c r="K26" s="339">
-        <v>12</v>
-      </c>
-      <c r="L26" s="339">
-        <v>12</v>
-      </c>
-      <c r="M26" s="331">
-        <v>12</v>
-      </c>
-      <c r="N26" s="332">
-        <v>12</v>
-      </c>
-      <c r="O26" s="332">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="2:15">
+      <c r="H26" s="381"/>
+      <c r="I26" s="381"/>
+      <c r="J26" s="381"/>
+      <c r="K26" s="381"/>
+      <c r="L26" s="381"/>
+      <c r="M26" s="381"/>
+      <c r="N26" s="383"/>
+      <c r="O26" s="383"/>
+    </row>
+    <row r="27" spans="2:15" ht="36" customHeight="1">
       <c r="B27" s="335">
         <v>17</v>
       </c>
-      <c r="C27" s="334" t="s">
-        <v>359</v>
-      </c>
-      <c r="D27" s="289"/>
-      <c r="E27" s="336"/>
-      <c r="F27" s="285"/>
-      <c r="G27" s="321"/>
+      <c r="C27" s="385" t="s">
+        <v>408</v>
+      </c>
+      <c r="D27" s="375" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27" s="376" t="s">
+        <v>350</v>
+      </c>
+      <c r="F27" s="377" t="s">
+        <v>117</v>
+      </c>
+      <c r="G27" s="378">
+        <v>10</v>
+      </c>
       <c r="H27" s="326"/>
       <c r="I27" s="339"/>
       <c r="J27" s="339"/>
@@ -11761,45 +11724,19 @@
       <c r="B28" s="338">
         <v>18</v>
       </c>
-      <c r="C28" s="341" t="s">
-        <v>386</v>
-      </c>
-      <c r="D28" s="289" t="s">
-        <v>107</v>
-      </c>
-      <c r="E28" s="336" t="s">
-        <v>350</v>
-      </c>
-      <c r="F28" s="285" t="s">
-        <v>117</v>
-      </c>
-      <c r="G28" s="321">
-        <v>12</v>
-      </c>
-      <c r="H28" s="326">
-        <v>12</v>
-      </c>
-      <c r="I28" s="339">
-        <v>12</v>
-      </c>
-      <c r="J28" s="339">
-        <v>12</v>
-      </c>
-      <c r="K28" s="339">
-        <v>12</v>
-      </c>
-      <c r="L28" s="339">
-        <v>12</v>
-      </c>
-      <c r="M28" s="331">
-        <v>12</v>
-      </c>
-      <c r="N28" s="332">
-        <v>12</v>
-      </c>
-      <c r="O28" s="332">
-        <v>12</v>
-      </c>
+      <c r="C28" s="334"/>
+      <c r="D28" s="289"/>
+      <c r="E28" s="336"/>
+      <c r="F28" s="285"/>
+      <c r="G28" s="321"/>
+      <c r="H28" s="326"/>
+      <c r="I28" s="339"/>
+      <c r="J28" s="339"/>
+      <c r="K28" s="339"/>
+      <c r="L28" s="339"/>
+      <c r="M28" s="331"/>
+      <c r="N28" s="332"/>
+      <c r="O28" s="332"/>
     </row>
     <row r="29" spans="2:15">
       <c r="B29" s="335">
@@ -11825,8 +11762,8 @@
       <c r="B30" s="338">
         <v>20</v>
       </c>
-      <c r="C30" s="340" t="s">
-        <v>387</v>
+      <c r="C30" s="341" t="s">
+        <v>391</v>
       </c>
       <c r="D30" s="289" t="s">
         <v>107</v>
@@ -11838,127 +11775,79 @@
         <v>117</v>
       </c>
       <c r="G30" s="321">
-        <v>20</v>
-      </c>
-      <c r="H30" s="326">
-        <v>18</v>
-      </c>
-      <c r="I30" s="326">
-        <v>15</v>
-      </c>
-      <c r="J30" s="326">
         <v>12</v>
       </c>
-      <c r="K30" s="326">
-        <v>8</v>
-      </c>
-      <c r="L30" s="326">
-        <v>5</v>
-      </c>
-      <c r="M30" s="333">
-        <v>3</v>
-      </c>
-      <c r="N30" s="332">
-        <v>0</v>
-      </c>
-      <c r="O30" s="332">
-        <v>0</v>
-      </c>
+      <c r="H30" s="326"/>
+      <c r="I30" s="326"/>
+      <c r="J30" s="326"/>
+      <c r="K30" s="326"/>
+      <c r="L30" s="326"/>
+      <c r="M30" s="333"/>
+      <c r="N30" s="332"/>
+      <c r="O30" s="332"/>
     </row>
     <row r="31" spans="2:15">
       <c r="B31" s="335">
         <v>21</v>
       </c>
-      <c r="C31" s="341" t="s">
-        <v>391</v>
-      </c>
-      <c r="D31" s="289" t="s">
+      <c r="C31" s="372" t="s">
+        <v>389</v>
+      </c>
+      <c r="D31" s="374" t="s">
         <v>107</v>
       </c>
-      <c r="E31" s="336" t="s">
+      <c r="E31" s="376" t="s">
         <v>352</v>
       </c>
-      <c r="F31" s="285" t="s">
+      <c r="F31" s="377" t="s">
         <v>117</v>
       </c>
-      <c r="G31" s="321">
+      <c r="G31" s="378">
         <v>12</v>
       </c>
-      <c r="H31" s="326">
-        <v>12</v>
-      </c>
-      <c r="I31" s="326">
-        <v>12</v>
-      </c>
-      <c r="J31" s="326">
-        <v>12</v>
-      </c>
-      <c r="K31" s="326">
-        <v>12</v>
-      </c>
-      <c r="L31" s="326">
-        <v>12</v>
-      </c>
-      <c r="M31" s="333">
-        <v>12</v>
-      </c>
-      <c r="N31" s="332">
-        <v>12</v>
-      </c>
-      <c r="O31" s="332">
-        <v>12</v>
-      </c>
+      <c r="H31" s="326"/>
+      <c r="I31" s="326"/>
+      <c r="J31" s="326"/>
+      <c r="K31" s="326"/>
+      <c r="L31" s="326"/>
+      <c r="M31" s="333"/>
+      <c r="N31" s="332"/>
+      <c r="O31" s="332"/>
     </row>
     <row r="32" spans="2:15">
       <c r="B32" s="338">
         <v>22</v>
       </c>
-      <c r="C32" s="340" t="s">
-        <v>389</v>
-      </c>
-      <c r="D32" s="289" t="s">
+      <c r="C32" s="372" t="s">
+        <v>390</v>
+      </c>
+      <c r="D32" s="374" t="s">
         <v>107</v>
       </c>
-      <c r="E32" s="336" t="s">
+      <c r="E32" s="376" t="s">
         <v>352</v>
       </c>
-      <c r="F32" s="285" t="s">
+      <c r="F32" s="377" t="s">
         <v>117</v>
       </c>
-      <c r="G32" s="321">
+      <c r="G32" s="378">
         <v>12</v>
       </c>
-      <c r="H32" s="326">
-        <v>12</v>
-      </c>
-      <c r="I32" s="326">
-        <v>12</v>
-      </c>
-      <c r="J32" s="326">
-        <v>12</v>
-      </c>
-      <c r="K32" s="326">
-        <v>12</v>
-      </c>
-      <c r="L32" s="326">
-        <v>12</v>
-      </c>
-      <c r="M32" s="333">
-        <v>12</v>
-      </c>
-      <c r="N32" s="332">
-        <v>12</v>
-      </c>
-      <c r="O32" s="332">
-        <v>12</v>
-      </c>
+      <c r="H32" s="326"/>
+      <c r="I32" s="326"/>
+      <c r="J32" s="326"/>
+      <c r="K32" s="326"/>
+      <c r="L32" s="326"/>
+      <c r="M32" s="333"/>
+      <c r="N32" s="332"/>
+      <c r="O32" s="332"/>
     </row>
     <row r="33" spans="2:15">
       <c r="B33" s="335">
         <v>23</v>
       </c>
       <c r="C33" s="340" t="s">
-        <v>390</v>
+        <v>409</v>
       </c>
       <c r="D33" s="289" t="s">
         <v>107</v>
@@ -11970,32 +11859,16 @@
         <v>117</v>
       </c>
       <c r="G33" s="321">
-        <v>12</v>
-      </c>
-      <c r="H33" s="326">
-        <v>12</v>
-      </c>
-      <c r="I33" s="326">
-        <v>12</v>
-      </c>
-      <c r="J33" s="326">
-        <v>12</v>
-      </c>
-      <c r="K33" s="326">
-        <v>12</v>
-      </c>
-      <c r="L33" s="326">
-        <v>12</v>
-      </c>
-      <c r="M33" s="333">
-        <v>12</v>
-      </c>
-      <c r="N33" s="332">
-        <v>12</v>
-      </c>
-      <c r="O33" s="332">
-        <v>12</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="H33" s="326"/>
+      <c r="I33" s="326"/>
+      <c r="J33" s="326"/>
+      <c r="K33" s="326"/>
+      <c r="L33" s="326"/>
+      <c r="M33" s="333"/>
+      <c r="N33" s="332"/>
+      <c r="O33" s="332"/>
     </row>
     <row r="34" spans="2:15">
       <c r="B34" s="338">
@@ -12019,11 +11892,11 @@
       <c r="B35" s="335">
         <v>25</v>
       </c>
-      <c r="C35" s="342"/>
-      <c r="D35" s="289"/>
-      <c r="E35" s="336"/>
-      <c r="F35" s="285"/>
-      <c r="G35" s="321"/>
+      <c r="C35" s="373"/>
+      <c r="D35" s="375"/>
+      <c r="E35" s="373"/>
+      <c r="F35" s="375"/>
+      <c r="G35" s="378"/>
       <c r="H35" s="326"/>
       <c r="I35" s="326"/>
       <c r="J35" s="326"/>
@@ -12037,11 +11910,11 @@
       <c r="B36" s="338">
         <v>26</v>
       </c>
-      <c r="C36" s="336"/>
-      <c r="D36" s="289"/>
-      <c r="E36" s="336"/>
-      <c r="F36" s="285"/>
-      <c r="G36" s="321"/>
+      <c r="C36" s="373"/>
+      <c r="D36" s="375"/>
+      <c r="E36" s="373"/>
+      <c r="F36" s="375"/>
+      <c r="G36" s="378"/>
       <c r="H36" s="326"/>
       <c r="I36" s="326"/>
       <c r="J36" s="326"/>
@@ -12055,11 +11928,11 @@
       <c r="B37" s="335">
         <v>27</v>
       </c>
-      <c r="C37" s="336"/>
-      <c r="D37" s="289"/>
-      <c r="E37" s="336"/>
-      <c r="F37" s="285"/>
-      <c r="G37" s="321"/>
+      <c r="C37" s="373"/>
+      <c r="D37" s="375"/>
+      <c r="E37" s="373"/>
+      <c r="F37" s="375"/>
+      <c r="G37" s="378"/>
       <c r="H37" s="326"/>
       <c r="I37" s="326"/>
       <c r="J37" s="326"/>
@@ -12073,11 +11946,11 @@
       <c r="B38" s="338">
         <v>28</v>
       </c>
-      <c r="C38" s="336"/>
-      <c r="D38" s="289"/>
-      <c r="E38" s="336"/>
-      <c r="F38" s="285"/>
-      <c r="G38" s="321"/>
+      <c r="C38" s="373"/>
+      <c r="D38" s="375"/>
+      <c r="E38" s="373"/>
+      <c r="F38" s="375"/>
+      <c r="G38" s="378"/>
       <c r="H38" s="326"/>
       <c r="I38" s="326"/>
       <c r="J38" s="326"/>
@@ -12091,11 +11964,11 @@
       <c r="B39" s="335">
         <v>29</v>
       </c>
-      <c r="C39" s="343"/>
-      <c r="D39" s="289"/>
-      <c r="E39" s="336"/>
-      <c r="F39" s="285"/>
-      <c r="G39" s="321"/>
+      <c r="C39" s="373"/>
+      <c r="D39" s="375"/>
+      <c r="E39" s="373"/>
+      <c r="F39" s="375"/>
+      <c r="G39" s="378"/>
       <c r="H39" s="326"/>
       <c r="I39" s="326"/>
       <c r="J39" s="326"/>
@@ -12109,11 +11982,11 @@
       <c r="B40" s="338">
         <v>30</v>
       </c>
-      <c r="C40" s="343"/>
-      <c r="D40" s="289"/>
-      <c r="E40" s="336"/>
-      <c r="F40" s="285"/>
-      <c r="G40" s="321"/>
+      <c r="C40" s="373"/>
+      <c r="D40" s="375"/>
+      <c r="E40" s="373"/>
+      <c r="F40" s="375"/>
+      <c r="G40" s="378"/>
       <c r="H40" s="326"/>
       <c r="I40" s="326"/>
       <c r="J40" s="326"/>
@@ -12127,11 +12000,11 @@
       <c r="B41" s="335">
         <v>31</v>
       </c>
-      <c r="C41" s="343"/>
-      <c r="D41" s="289"/>
-      <c r="E41" s="336"/>
-      <c r="F41" s="285"/>
-      <c r="G41" s="321"/>
+      <c r="C41" s="373"/>
+      <c r="D41" s="375"/>
+      <c r="E41" s="373"/>
+      <c r="F41" s="375"/>
+      <c r="G41" s="378"/>
       <c r="H41" s="326"/>
       <c r="I41" s="326"/>
       <c r="J41" s="326"/>
@@ -12145,11 +12018,11 @@
       <c r="B42" s="338">
         <v>32</v>
       </c>
-      <c r="C42" s="343"/>
-      <c r="D42" s="289"/>
-      <c r="E42" s="336"/>
-      <c r="F42" s="285"/>
-      <c r="G42" s="321"/>
+      <c r="C42" s="373"/>
+      <c r="D42" s="375"/>
+      <c r="E42" s="373"/>
+      <c r="F42" s="375"/>
+      <c r="G42" s="378"/>
       <c r="H42" s="326"/>
       <c r="I42" s="326"/>
       <c r="J42" s="326"/>
@@ -12163,11 +12036,11 @@
       <c r="B43" s="335">
         <v>33</v>
       </c>
-      <c r="C43" s="343"/>
-      <c r="D43" s="289"/>
-      <c r="E43" s="336"/>
-      <c r="F43" s="285"/>
-      <c r="G43" s="321"/>
+      <c r="C43" s="373"/>
+      <c r="D43" s="375"/>
+      <c r="E43" s="373"/>
+      <c r="F43" s="375"/>
+      <c r="G43" s="378"/>
       <c r="H43" s="326"/>
       <c r="I43" s="326"/>
       <c r="J43" s="326"/>
@@ -12181,11 +12054,11 @@
       <c r="B44" s="338">
         <v>34</v>
       </c>
-      <c r="C44" s="340"/>
-      <c r="D44" s="289"/>
-      <c r="E44" s="336"/>
-      <c r="F44" s="285"/>
-      <c r="G44" s="321"/>
+      <c r="C44" s="373"/>
+      <c r="D44" s="375"/>
+      <c r="E44" s="373"/>
+      <c r="F44" s="375"/>
+      <c r="G44" s="378"/>
       <c r="H44" s="326"/>
       <c r="I44" s="326"/>
       <c r="J44" s="326"/>
@@ -12199,11 +12072,11 @@
       <c r="B45" s="335">
         <v>35</v>
       </c>
-      <c r="C45" s="343"/>
-      <c r="D45" s="289"/>
-      <c r="E45" s="336"/>
-      <c r="F45" s="285"/>
-      <c r="G45" s="321"/>
+      <c r="C45" s="373"/>
+      <c r="D45" s="375"/>
+      <c r="E45" s="373"/>
+      <c r="F45" s="375"/>
+      <c r="G45" s="378"/>
       <c r="H45" s="326"/>
       <c r="I45" s="326"/>
       <c r="J45" s="326"/>
@@ -12217,11 +12090,11 @@
       <c r="B46" s="338">
         <v>36</v>
       </c>
-      <c r="C46" s="343"/>
-      <c r="D46" s="289"/>
-      <c r="E46" s="336"/>
-      <c r="F46" s="285"/>
-      <c r="G46" s="321"/>
+      <c r="C46" s="373"/>
+      <c r="D46" s="375"/>
+      <c r="E46" s="373"/>
+      <c r="F46" s="375"/>
+      <c r="G46" s="378"/>
       <c r="H46" s="326"/>
       <c r="I46" s="326"/>
       <c r="J46" s="326"/>
@@ -12235,11 +12108,11 @@
       <c r="B47" s="335">
         <v>37</v>
       </c>
-      <c r="C47" s="343"/>
-      <c r="D47" s="289"/>
-      <c r="E47" s="336"/>
-      <c r="F47" s="285"/>
-      <c r="G47" s="321"/>
+      <c r="C47" s="373"/>
+      <c r="D47" s="375"/>
+      <c r="E47" s="373"/>
+      <c r="F47" s="375"/>
+      <c r="G47" s="378"/>
       <c r="H47" s="326"/>
       <c r="I47" s="326"/>
       <c r="J47" s="326"/>
@@ -12253,11 +12126,11 @@
       <c r="B48" s="338">
         <v>38</v>
       </c>
-      <c r="C48" s="343"/>
-      <c r="D48" s="289"/>
-      <c r="E48" s="336"/>
-      <c r="F48" s="285"/>
-      <c r="G48" s="321"/>
+      <c r="C48" s="373"/>
+      <c r="D48" s="375"/>
+      <c r="E48" s="373"/>
+      <c r="F48" s="375"/>
+      <c r="G48" s="378"/>
       <c r="H48" s="326"/>
       <c r="I48" s="326"/>
       <c r="J48" s="326"/>
@@ -12271,11 +12144,11 @@
       <c r="B49" s="335">
         <v>39</v>
       </c>
-      <c r="C49" s="340"/>
-      <c r="D49" s="289"/>
-      <c r="E49" s="336"/>
-      <c r="F49" s="285"/>
-      <c r="G49" s="321"/>
+      <c r="C49" s="373"/>
+      <c r="D49" s="375"/>
+      <c r="E49" s="373"/>
+      <c r="F49" s="375"/>
+      <c r="G49" s="378"/>
       <c r="H49" s="326"/>
       <c r="I49" s="326"/>
       <c r="J49" s="326"/>
@@ -12289,11 +12162,11 @@
       <c r="B50" s="338">
         <v>40</v>
       </c>
-      <c r="C50" s="340"/>
-      <c r="D50" s="289"/>
-      <c r="E50" s="336"/>
-      <c r="F50" s="285"/>
-      <c r="G50" s="321"/>
+      <c r="C50" s="373"/>
+      <c r="D50" s="375"/>
+      <c r="E50" s="373"/>
+      <c r="F50" s="375"/>
+      <c r="G50" s="378"/>
       <c r="H50" s="326"/>
       <c r="I50" s="326"/>
       <c r="J50" s="326"/>
@@ -12307,11 +12180,11 @@
       <c r="B51" s="335">
         <v>41</v>
       </c>
-      <c r="C51" s="340"/>
-      <c r="D51" s="289"/>
-      <c r="E51" s="336"/>
-      <c r="F51" s="285"/>
-      <c r="G51" s="321"/>
+      <c r="C51" s="373"/>
+      <c r="D51" s="375"/>
+      <c r="E51" s="373"/>
+      <c r="F51" s="375"/>
+      <c r="G51" s="378"/>
       <c r="H51" s="326"/>
       <c r="I51" s="326"/>
       <c r="J51" s="326"/>
@@ -12651,24 +12524,18 @@
   <mergeCells count="1">
     <mergeCell ref="B7:E7"/>
   </mergeCells>
-  <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F11:F52">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F52:F54 F11:F14 F16:F34">
       <formula1>$C$114:$C$119</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="E11:E54">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="E52:E54 E11:E14 E16:E34">
       <formula1>$C$107:$C$111</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D35:D38">
-      <formula1>$C$108:$C$112</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F53:F91">
-      <formula1>$C$115:$C$119</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D53:D54 D39:D48 D11:D34">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D52:D54 D11:D14 D16:D26 D28:D34">
       <formula1>$C$101:$C$105</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D49:D52">
-      <formula1>$C$118:$C$122</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F55:F91">
+      <formula1>$C$115:$C$119</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23802,8 +23669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:O119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
update productbacklog task list
</commit_message>
<xml_diff>
--- a/Documents/ProductBackLog/Capstone_Group6_ProductBackLog_SprintTaskList.xlsx
+++ b/Documents/ProductBackLog/Capstone_Group6_ProductBackLog_SprintTaskList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4680" firstSheet="11" activeTab="14"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4680" firstSheet="12" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="2" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Sprint07_1706_2306 " sheetId="17" r:id="rId13"/>
     <sheet name="Sprint08_2406_3006" sheetId="16" r:id="rId14"/>
     <sheet name="Sprint09_0107_0707" sheetId="19" r:id="rId15"/>
+    <sheet name="Sprint10_0807_1407" sheetId="20" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Product Backlog'!$A$1:$G$106</definedName>
@@ -685,7 +686,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1623" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1701" uniqueCount="477">
   <si>
     <t>Introduction</t>
   </si>
@@ -2131,6 +2132,18 @@
   </si>
   <si>
     <t>+Sort name/date when teacher see feedback list</t>
+  </si>
+  <si>
+    <t>+Import question by file</t>
+  </si>
+  <si>
+    <t>+Search reuse with test tags</t>
+  </si>
+  <si>
+    <t>+Real time feedback using Signal-R</t>
+  </si>
+  <si>
+    <t>SPRINT 10 FROM 08/07 TO 14/07</t>
   </si>
 </sst>
 </file>
@@ -4203,6 +4216,21 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="10" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="10" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="10" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="27" fillId="10" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4256,42 +4284,468 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="23" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="10" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="10" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="10" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="27" fillId="10" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="257">
+  <dxfs count="276">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment vertical="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment vertical="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment vertical="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <border>
         <top style="thin">
           <color rgb="FF000000"/>
         </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
         <vertical/>
         <horizontal/>
       </border>
@@ -4345,6 +4799,15 @@
       </border>
     </dxf>
     <dxf>
+      <border>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -4831,15 +5294,6 @@
         <top style="thin">
           <color rgb="FF000000"/>
         </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
         <vertical/>
         <horizontal/>
       </border>
@@ -4893,6 +5347,15 @@
       </border>
     </dxf>
     <dxf>
+      <border>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -5372,6 +5835,104 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -13094,21 +13655,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B10:N30" totalsRowShown="0" headerRowDxfId="256" headerRowBorderDxfId="255" tableBorderDxfId="254">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B10:N30" totalsRowShown="0" headerRowDxfId="275" headerRowBorderDxfId="274" tableBorderDxfId="273">
   <autoFilter ref="B10:N30"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="No." dataDxfId="253"/>
-    <tableColumn id="2" name="Task description" dataDxfId="252"/>
-    <tableColumn id="3" name="Type" dataDxfId="251"/>
-    <tableColumn id="4" name="Assign To" dataDxfId="250"/>
-    <tableColumn id="5" name="Status" dataDxfId="249"/>
-    <tableColumn id="8" name="(W)23/5" dataDxfId="248"/>
-    <tableColumn id="9" name="(Th)24/5" dataDxfId="247"/>
-    <tableColumn id="10" name="(Fr)25/5" dataDxfId="246"/>
-    <tableColumn id="11" name="(Sa)26/5" dataDxfId="245"/>
-    <tableColumn id="12" name="(Su)27/5" dataDxfId="244"/>
+    <tableColumn id="1" name="No." dataDxfId="272"/>
+    <tableColumn id="2" name="Task description" dataDxfId="271"/>
+    <tableColumn id="3" name="Type" dataDxfId="270"/>
+    <tableColumn id="4" name="Assign To" dataDxfId="269"/>
+    <tableColumn id="5" name="Status" dataDxfId="268"/>
+    <tableColumn id="8" name="(W)23/5" dataDxfId="267"/>
+    <tableColumn id="9" name="(Th)24/5" dataDxfId="266"/>
+    <tableColumn id="10" name="(Fr)25/5" dataDxfId="265"/>
+    <tableColumn id="11" name="(Sa)26/5" dataDxfId="264"/>
+    <tableColumn id="12" name="(Su)27/5" dataDxfId="263"/>
     <tableColumn id="13" name="(Mo)28/5"/>
-    <tableColumn id="14" name="(Tu)29/5" dataDxfId="243"/>
+    <tableColumn id="14" name="(Tu)29/5" dataDxfId="262"/>
     <tableColumn id="7" name="End Sprint"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -13116,8 +13677,35 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table134567891011" displayName="Table134567891011" ref="B10:O54" totalsRowShown="0" headerRowDxfId="94" dataDxfId="92" headerRowBorderDxfId="93" tableBorderDxfId="91" totalsRowBorderDxfId="90">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table134567891011" displayName="Table134567891011" ref="B10:O54" totalsRowShown="0" headerRowDxfId="113" dataDxfId="111" headerRowBorderDxfId="112" tableBorderDxfId="110" totalsRowBorderDxfId="109">
   <autoFilter ref="B10:O54">
+    <filterColumn colId="5"/>
+    <filterColumn colId="12"/>
+    <filterColumn colId="13"/>
+  </autoFilter>
+  <tableColumns count="14">
+    <tableColumn id="1" name="No." dataDxfId="108"/>
+    <tableColumn id="2" name="Task description" dataDxfId="107"/>
+    <tableColumn id="3" name="Type" dataDxfId="106"/>
+    <tableColumn id="4" name="Assign To" dataDxfId="105"/>
+    <tableColumn id="5" name="Status" dataDxfId="104"/>
+    <tableColumn id="7" name="Estimate" dataDxfId="103"/>
+    <tableColumn id="8" name="03/06" dataDxfId="102"/>
+    <tableColumn id="9" name="04/06" dataDxfId="101"/>
+    <tableColumn id="10" name="05/06" dataDxfId="100"/>
+    <tableColumn id="11" name="06/06" dataDxfId="99"/>
+    <tableColumn id="12" name="07/06" dataDxfId="98"/>
+    <tableColumn id="13" name="08/06" dataDxfId="97"/>
+    <tableColumn id="14" name="09/06" dataDxfId="96"/>
+    <tableColumn id="15" name="End" dataDxfId="95"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table13456789101112" displayName="Table13456789101112" ref="B10:O56" totalsRowShown="0" headerRowDxfId="94" dataDxfId="92" headerRowBorderDxfId="93" tableBorderDxfId="91" totalsRowBorderDxfId="90">
+  <autoFilter ref="B10:O56">
     <filterColumn colId="5"/>
     <filterColumn colId="12"/>
     <filterColumn colId="13"/>
@@ -13129,21 +13717,21 @@
     <tableColumn id="4" name="Assign To" dataDxfId="86"/>
     <tableColumn id="5" name="Status" dataDxfId="85"/>
     <tableColumn id="7" name="Estimate" dataDxfId="84"/>
-    <tableColumn id="8" name="03/06" dataDxfId="83"/>
-    <tableColumn id="9" name="04/06" dataDxfId="82"/>
-    <tableColumn id="10" name="05/06" dataDxfId="81"/>
-    <tableColumn id="11" name="06/06" dataDxfId="80"/>
-    <tableColumn id="12" name="07/06" dataDxfId="79"/>
-    <tableColumn id="13" name="08/06" dataDxfId="78"/>
-    <tableColumn id="14" name="09/06" dataDxfId="77"/>
+    <tableColumn id="8" name="10/06" dataDxfId="83"/>
+    <tableColumn id="9" name="11/06" dataDxfId="82"/>
+    <tableColumn id="10" name="12/06" dataDxfId="81"/>
+    <tableColumn id="11" name="13/06" dataDxfId="80"/>
+    <tableColumn id="12" name="14/06" dataDxfId="79"/>
+    <tableColumn id="13" name="15/06" dataDxfId="78"/>
+    <tableColumn id="14" name="16/06" dataDxfId="77"/>
     <tableColumn id="15" name="End" dataDxfId="76"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table13456789101112" displayName="Table13456789101112" ref="B10:O56" totalsRowShown="0" headerRowDxfId="75" dataDxfId="73" headerRowBorderDxfId="74" tableBorderDxfId="72" totalsRowBorderDxfId="71">
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table134567891011121314" displayName="Table134567891011121314" ref="B10:O56" totalsRowShown="0" headerRowDxfId="75" dataDxfId="73" headerRowBorderDxfId="74" tableBorderDxfId="72" totalsRowBorderDxfId="71">
   <autoFilter ref="B10:O56">
     <filterColumn colId="5"/>
     <filterColumn colId="12"/>
@@ -13156,41 +13744,14 @@
     <tableColumn id="4" name="Assign To" dataDxfId="67"/>
     <tableColumn id="5" name="Status" dataDxfId="66"/>
     <tableColumn id="7" name="Estimate" dataDxfId="65"/>
-    <tableColumn id="8" name="10/06" dataDxfId="64"/>
-    <tableColumn id="9" name="11/06" dataDxfId="63"/>
-    <tableColumn id="10" name="12/06" dataDxfId="62"/>
-    <tableColumn id="11" name="13/06" dataDxfId="61"/>
-    <tableColumn id="12" name="14/06" dataDxfId="60"/>
-    <tableColumn id="13" name="15/06" dataDxfId="59"/>
-    <tableColumn id="14" name="16/06" dataDxfId="58"/>
+    <tableColumn id="8" name="17/06" dataDxfId="64"/>
+    <tableColumn id="9" name="18/06" dataDxfId="63"/>
+    <tableColumn id="10" name="19/06" dataDxfId="62"/>
+    <tableColumn id="11" name="20/06" dataDxfId="61"/>
+    <tableColumn id="12" name="21/06" dataDxfId="60"/>
+    <tableColumn id="13" name="22/06" dataDxfId="59"/>
+    <tableColumn id="14" name="23/06" dataDxfId="58"/>
     <tableColumn id="15" name="End" dataDxfId="57"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table134567891011121314" displayName="Table134567891011121314" ref="B10:O56" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" headerRowBorderDxfId="20" tableBorderDxfId="21" totalsRowBorderDxfId="19">
-  <autoFilter ref="B10:O56">
-    <filterColumn colId="5"/>
-    <filterColumn colId="12"/>
-    <filterColumn colId="13"/>
-  </autoFilter>
-  <tableColumns count="14">
-    <tableColumn id="1" name="No." dataDxfId="37"/>
-    <tableColumn id="2" name="Task description" dataDxfId="36"/>
-    <tableColumn id="3" name="Type" dataDxfId="35"/>
-    <tableColumn id="4" name="Assign To" dataDxfId="34"/>
-    <tableColumn id="5" name="Status" dataDxfId="33"/>
-    <tableColumn id="7" name="Estimate" dataDxfId="32"/>
-    <tableColumn id="8" name="17/06" dataDxfId="31"/>
-    <tableColumn id="9" name="18/06" dataDxfId="30"/>
-    <tableColumn id="10" name="19/06" dataDxfId="29"/>
-    <tableColumn id="11" name="20/06" dataDxfId="28"/>
-    <tableColumn id="12" name="21/06" dataDxfId="27"/>
-    <tableColumn id="13" name="22/06" dataDxfId="26"/>
-    <tableColumn id="14" name="23/06" dataDxfId="25"/>
-    <tableColumn id="15" name="End" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -13224,159 +13785,213 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table134567891011121315" displayName="Table134567891011121315" ref="B10:O56" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" headerRowBorderDxfId="1" tableBorderDxfId="2" totalsRowBorderDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table134567891011121315" displayName="Table134567891011121315" ref="B10:O57" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
+  <autoFilter ref="B10:O57">
+    <filterColumn colId="5"/>
+    <filterColumn colId="12"/>
+    <filterColumn colId="13"/>
+  </autoFilter>
+  <tableColumns count="14">
+    <tableColumn id="1" name="No." dataDxfId="32"/>
+    <tableColumn id="2" name="Task description" dataDxfId="31"/>
+    <tableColumn id="3" name="Type" dataDxfId="30"/>
+    <tableColumn id="4" name="Assign To" dataDxfId="29"/>
+    <tableColumn id="5" name="Status" dataDxfId="28"/>
+    <tableColumn id="7" name="Estimate" dataDxfId="27"/>
+    <tableColumn id="8" name="01/07" dataDxfId="26"/>
+    <tableColumn id="9" name="02/07" dataDxfId="25"/>
+    <tableColumn id="10" name="03/07" dataDxfId="24"/>
+    <tableColumn id="11" name="04/07" dataDxfId="23"/>
+    <tableColumn id="12" name="05/07" dataDxfId="22"/>
+    <tableColumn id="13" name="06/07" dataDxfId="21"/>
+    <tableColumn id="14" name="07/07" dataDxfId="20"/>
+    <tableColumn id="15" name="End" dataDxfId="19"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table13456789101112131516" displayName="Table13456789101112131516" ref="B10:O56" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="B10:O56">
     <filterColumn colId="5"/>
     <filterColumn colId="12"/>
     <filterColumn colId="13"/>
   </autoFilter>
   <tableColumns count="14">
-    <tableColumn id="1" name="No." dataDxfId="18"/>
-    <tableColumn id="2" name="Task description" dataDxfId="17"/>
-    <tableColumn id="3" name="Type" dataDxfId="16"/>
-    <tableColumn id="4" name="Assign To" dataDxfId="15"/>
-    <tableColumn id="5" name="Status" dataDxfId="14"/>
-    <tableColumn id="7" name="Estimate" dataDxfId="13"/>
-    <tableColumn id="8" name="01/07" dataDxfId="12"/>
-    <tableColumn id="9" name="02/07" dataDxfId="11"/>
-    <tableColumn id="10" name="03/07" dataDxfId="10"/>
-    <tableColumn id="11" name="04/07" dataDxfId="9"/>
-    <tableColumn id="12" name="05/07" dataDxfId="8"/>
-    <tableColumn id="13" name="06/07" dataDxfId="7"/>
-    <tableColumn id="14" name="07/07" dataDxfId="6"/>
-    <tableColumn id="15" name="End" dataDxfId="5"/>
+    <tableColumn id="1" name="No." dataDxfId="13"/>
+    <tableColumn id="2" name="Task description" dataDxfId="12"/>
+    <tableColumn id="3" name="Type" dataDxfId="11"/>
+    <tableColumn id="4" name="Assign To" dataDxfId="10"/>
+    <tableColumn id="5" name="Status" dataDxfId="9"/>
+    <tableColumn id="7" name="Estimate" dataDxfId="8"/>
+    <tableColumn id="8" name="01/07" dataDxfId="7"/>
+    <tableColumn id="9" name="02/07" dataDxfId="6"/>
+    <tableColumn id="10" name="03/07" dataDxfId="5"/>
+    <tableColumn id="11" name="04/07" dataDxfId="4"/>
+    <tableColumn id="12" name="05/07" dataDxfId="3"/>
+    <tableColumn id="13" name="06/07" dataDxfId="2"/>
+    <tableColumn id="14" name="07/07" dataDxfId="1"/>
+    <tableColumn id="15" name="End" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="B10:O28" totalsRowShown="0" headerRowDxfId="242" headerRowBorderDxfId="241" tableBorderDxfId="240">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="B10:O28" totalsRowShown="0" headerRowDxfId="261" headerRowBorderDxfId="260" tableBorderDxfId="259">
   <autoFilter ref="B10:O28"/>
   <tableColumns count="14">
-    <tableColumn id="1" name="No." dataDxfId="239"/>
-    <tableColumn id="2" name="Task description" dataDxfId="238"/>
-    <tableColumn id="3" name="Type" dataDxfId="237"/>
-    <tableColumn id="4" name="Assign To" dataDxfId="236"/>
-    <tableColumn id="5" name="Status" dataDxfId="235"/>
-    <tableColumn id="17" name="Percentage" dataDxfId="234"/>
-    <tableColumn id="8" name="(W)30/5" dataDxfId="233"/>
-    <tableColumn id="9" name="(Th)31/5" dataDxfId="232"/>
-    <tableColumn id="10" name="(Fr)1/6" dataDxfId="231"/>
-    <tableColumn id="11" name="(Sa)2/6" dataDxfId="230"/>
-    <tableColumn id="12" name="(Su)3/6" dataDxfId="229"/>
+    <tableColumn id="1" name="No." dataDxfId="258"/>
+    <tableColumn id="2" name="Task description" dataDxfId="257"/>
+    <tableColumn id="3" name="Type" dataDxfId="256"/>
+    <tableColumn id="4" name="Assign To" dataDxfId="255"/>
+    <tableColumn id="5" name="Status" dataDxfId="254"/>
+    <tableColumn id="17" name="Percentage" dataDxfId="253"/>
+    <tableColumn id="8" name="(W)30/5" dataDxfId="252"/>
+    <tableColumn id="9" name="(Th)31/5" dataDxfId="251"/>
+    <tableColumn id="10" name="(Fr)1/6" dataDxfId="250"/>
+    <tableColumn id="11" name="(Sa)2/6" dataDxfId="249"/>
+    <tableColumn id="12" name="(Su)3/6" dataDxfId="248"/>
     <tableColumn id="13" name="(Mo)4/6"/>
-    <tableColumn id="14" name="(Tu)5/6" dataDxfId="228"/>
-    <tableColumn id="7" name="End Sprint" dataDxfId="227"/>
+    <tableColumn id="14" name="(Tu)5/6" dataDxfId="247"/>
+    <tableColumn id="7" name="End Sprint" dataDxfId="246"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table134" displayName="Table134" ref="B10:N27" totalsRowShown="0" headerRowDxfId="226" headerRowBorderDxfId="225" tableBorderDxfId="224">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table134" displayName="Table134" ref="B10:N27" totalsRowShown="0" headerRowDxfId="245" headerRowBorderDxfId="244" tableBorderDxfId="243">
   <autoFilter ref="B10:N27"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="No." dataDxfId="223"/>
-    <tableColumn id="2" name="Task description" dataDxfId="222"/>
-    <tableColumn id="3" name="Type" dataDxfId="221"/>
-    <tableColumn id="4" name="Assign To" dataDxfId="220"/>
-    <tableColumn id="5" name="Status" dataDxfId="219"/>
-    <tableColumn id="8" name="(W)06/6" dataDxfId="218"/>
-    <tableColumn id="9" name="(Th)07/6" dataDxfId="217"/>
-    <tableColumn id="10" name="(Fr)08/6" dataDxfId="216"/>
-    <tableColumn id="11" name="(Sa)09/6" dataDxfId="215"/>
-    <tableColumn id="12" name="(Su)10/6" dataDxfId="214"/>
+    <tableColumn id="1" name="No." dataDxfId="242"/>
+    <tableColumn id="2" name="Task description" dataDxfId="241"/>
+    <tableColumn id="3" name="Type" dataDxfId="240"/>
+    <tableColumn id="4" name="Assign To" dataDxfId="239"/>
+    <tableColumn id="5" name="Status" dataDxfId="238"/>
+    <tableColumn id="8" name="(W)06/6" dataDxfId="237"/>
+    <tableColumn id="9" name="(Th)07/6" dataDxfId="236"/>
+    <tableColumn id="10" name="(Fr)08/6" dataDxfId="235"/>
+    <tableColumn id="11" name="(Sa)09/6" dataDxfId="234"/>
+    <tableColumn id="12" name="(Su)10/6" dataDxfId="233"/>
     <tableColumn id="13" name="(Mo)11/6"/>
-    <tableColumn id="14" name="(Tu)12/6" dataDxfId="213"/>
-    <tableColumn id="7" name="End Sprint" dataDxfId="212"/>
+    <tableColumn id="14" name="(Tu)12/6" dataDxfId="232"/>
+    <tableColumn id="7" name="End Sprint" dataDxfId="231"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table1345" displayName="Table1345" ref="B10:AA76" totalsRowShown="0" headerRowDxfId="211" headerRowBorderDxfId="210" tableBorderDxfId="209">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table1345" displayName="Table1345" ref="B10:AA76" totalsRowShown="0" headerRowDxfId="230" headerRowBorderDxfId="229" tableBorderDxfId="228">
   <autoFilter ref="B10:AA76"/>
   <tableColumns count="26">
-    <tableColumn id="1" name="No." dataDxfId="208"/>
-    <tableColumn id="2" name="Task description" dataDxfId="207"/>
-    <tableColumn id="3" name="Type" dataDxfId="206"/>
-    <tableColumn id="4" name="Assign To" dataDxfId="205"/>
-    <tableColumn id="5" name="Status" dataDxfId="204"/>
-    <tableColumn id="8" name="25/6" dataDxfId="203"/>
-    <tableColumn id="9" name="26/6" dataDxfId="202"/>
-    <tableColumn id="10" name="27/6" dataDxfId="201"/>
-    <tableColumn id="11" name="28/6" dataDxfId="200"/>
-    <tableColumn id="12" name="29/6" dataDxfId="199"/>
+    <tableColumn id="1" name="No." dataDxfId="227"/>
+    <tableColumn id="2" name="Task description" dataDxfId="226"/>
+    <tableColumn id="3" name="Type" dataDxfId="225"/>
+    <tableColumn id="4" name="Assign To" dataDxfId="224"/>
+    <tableColumn id="5" name="Status" dataDxfId="223"/>
+    <tableColumn id="8" name="25/6" dataDxfId="222"/>
+    <tableColumn id="9" name="26/6" dataDxfId="221"/>
+    <tableColumn id="10" name="27/6" dataDxfId="220"/>
+    <tableColumn id="11" name="28/6" dataDxfId="219"/>
+    <tableColumn id="12" name="29/6" dataDxfId="218"/>
     <tableColumn id="13" name="30/6"/>
-    <tableColumn id="14" name="1/7" dataDxfId="198"/>
-    <tableColumn id="6" name="2/7" dataDxfId="197"/>
-    <tableColumn id="7" name="3/7" dataDxfId="196"/>
-    <tableColumn id="15" name="4/7" dataDxfId="195"/>
-    <tableColumn id="16" name="5/7" dataDxfId="194"/>
-    <tableColumn id="17" name="6/7" dataDxfId="193"/>
-    <tableColumn id="24" name="7/7" dataDxfId="192"/>
-    <tableColumn id="23" name="8/7" dataDxfId="191"/>
-    <tableColumn id="22" name="9/7" dataDxfId="190"/>
-    <tableColumn id="21" name="10/7" dataDxfId="189"/>
-    <tableColumn id="20" name="11/7" dataDxfId="188"/>
-    <tableColumn id="18" name="12/7" dataDxfId="187"/>
-    <tableColumn id="25" name="13/7" dataDxfId="186"/>
-    <tableColumn id="26" name="14/7" dataDxfId="185"/>
-    <tableColumn id="19" name="End" dataDxfId="184"/>
+    <tableColumn id="14" name="1/7" dataDxfId="217"/>
+    <tableColumn id="6" name="2/7" dataDxfId="216"/>
+    <tableColumn id="7" name="3/7" dataDxfId="215"/>
+    <tableColumn id="15" name="4/7" dataDxfId="214"/>
+    <tableColumn id="16" name="5/7" dataDxfId="213"/>
+    <tableColumn id="17" name="6/7" dataDxfId="212"/>
+    <tableColumn id="24" name="7/7" dataDxfId="211"/>
+    <tableColumn id="23" name="8/7" dataDxfId="210"/>
+    <tableColumn id="22" name="9/7" dataDxfId="209"/>
+    <tableColumn id="21" name="10/7" dataDxfId="208"/>
+    <tableColumn id="20" name="11/7" dataDxfId="207"/>
+    <tableColumn id="18" name="12/7" dataDxfId="206"/>
+    <tableColumn id="25" name="13/7" dataDxfId="205"/>
+    <tableColumn id="26" name="14/7" dataDxfId="204"/>
+    <tableColumn id="19" name="End" dataDxfId="203"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13456" displayName="Table13456" ref="B10:N56" totalsRowShown="0" headerRowDxfId="183" headerRowBorderDxfId="182" tableBorderDxfId="181">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13456" displayName="Table13456" ref="B10:N56" totalsRowShown="0" headerRowDxfId="202" headerRowBorderDxfId="201" tableBorderDxfId="200">
   <autoFilter ref="B10:N56"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="No." dataDxfId="180"/>
-    <tableColumn id="2" name="Task description" dataDxfId="179"/>
-    <tableColumn id="3" name="Type" dataDxfId="178"/>
-    <tableColumn id="4" name="Assign To" dataDxfId="177"/>
-    <tableColumn id="5" name="Status" dataDxfId="176"/>
-    <tableColumn id="8" name="16/7" dataDxfId="175"/>
-    <tableColumn id="9" name="17/7" dataDxfId="174"/>
-    <tableColumn id="10" name="18/7" dataDxfId="173"/>
-    <tableColumn id="11" name="19/7" dataDxfId="172"/>
-    <tableColumn id="12" name="20/7" dataDxfId="171"/>
+    <tableColumn id="1" name="No." dataDxfId="199"/>
+    <tableColumn id="2" name="Task description" dataDxfId="198"/>
+    <tableColumn id="3" name="Type" dataDxfId="197"/>
+    <tableColumn id="4" name="Assign To" dataDxfId="196"/>
+    <tableColumn id="5" name="Status" dataDxfId="195"/>
+    <tableColumn id="8" name="16/7" dataDxfId="194"/>
+    <tableColumn id="9" name="17/7" dataDxfId="193"/>
+    <tableColumn id="10" name="18/7" dataDxfId="192"/>
+    <tableColumn id="11" name="19/7" dataDxfId="191"/>
+    <tableColumn id="12" name="20/7" dataDxfId="190"/>
     <tableColumn id="13" name="21/7"/>
-    <tableColumn id="14" name="22/7" dataDxfId="170"/>
-    <tableColumn id="19" name="End" dataDxfId="169"/>
+    <tableColumn id="14" name="22/7" dataDxfId="189"/>
+    <tableColumn id="19" name="End" dataDxfId="188"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table134567" displayName="Table134567" ref="B10:M54" totalsRowShown="0" headerRowDxfId="168" dataDxfId="166" headerRowBorderDxfId="167" tableBorderDxfId="165" totalsRowBorderDxfId="164">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table134567" displayName="Table134567" ref="B10:M54" totalsRowShown="0" headerRowDxfId="187" dataDxfId="185" headerRowBorderDxfId="186" tableBorderDxfId="184" totalsRowBorderDxfId="183">
   <autoFilter ref="B10:M54">
     <filterColumn colId="5"/>
   </autoFilter>
   <tableColumns count="12">
-    <tableColumn id="1" name="No." dataDxfId="163"/>
-    <tableColumn id="2" name="Task description" dataDxfId="162"/>
-    <tableColumn id="3" name="Type" dataDxfId="161"/>
-    <tableColumn id="4" name="Assign To" dataDxfId="160"/>
-    <tableColumn id="5" name="Status" dataDxfId="159"/>
-    <tableColumn id="7" name="Estimate" dataDxfId="158"/>
-    <tableColumn id="8" name="08/05" dataDxfId="157"/>
-    <tableColumn id="9" name="09/05" dataDxfId="156"/>
-    <tableColumn id="10" name="10/05" dataDxfId="155"/>
-    <tableColumn id="11" name="11/05" dataDxfId="154"/>
-    <tableColumn id="12" name="12/05" dataDxfId="153"/>
-    <tableColumn id="13" name="End" dataDxfId="152"/>
+    <tableColumn id="1" name="No." dataDxfId="182"/>
+    <tableColumn id="2" name="Task description" dataDxfId="181"/>
+    <tableColumn id="3" name="Type" dataDxfId="180"/>
+    <tableColumn id="4" name="Assign To" dataDxfId="179"/>
+    <tableColumn id="5" name="Status" dataDxfId="178"/>
+    <tableColumn id="7" name="Estimate" dataDxfId="177"/>
+    <tableColumn id="8" name="08/05" dataDxfId="176"/>
+    <tableColumn id="9" name="09/05" dataDxfId="175"/>
+    <tableColumn id="10" name="10/05" dataDxfId="174"/>
+    <tableColumn id="11" name="11/05" dataDxfId="173"/>
+    <tableColumn id="12" name="12/05" dataDxfId="172"/>
+    <tableColumn id="13" name="End" dataDxfId="171"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table1345678" displayName="Table1345678" ref="B10:O54" totalsRowShown="0" headerRowDxfId="151" dataDxfId="149" headerRowBorderDxfId="150" tableBorderDxfId="148" totalsRowBorderDxfId="147">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table1345678" displayName="Table1345678" ref="B10:O54" totalsRowShown="0" headerRowDxfId="170" dataDxfId="168" headerRowBorderDxfId="169" tableBorderDxfId="167" totalsRowBorderDxfId="166">
+  <autoFilter ref="B10:O54">
+    <filterColumn colId="5"/>
+    <filterColumn colId="12"/>
+    <filterColumn colId="13"/>
+  </autoFilter>
+  <tableColumns count="14">
+    <tableColumn id="1" name="No." dataDxfId="165"/>
+    <tableColumn id="2" name="Task description" dataDxfId="164"/>
+    <tableColumn id="3" name="Type" dataDxfId="163"/>
+    <tableColumn id="4" name="Assign To" dataDxfId="162"/>
+    <tableColumn id="5" name="Status" dataDxfId="161"/>
+    <tableColumn id="7" name="Estimate" dataDxfId="160"/>
+    <tableColumn id="8" name="13/05" dataDxfId="159"/>
+    <tableColumn id="9" name="14/05" dataDxfId="158"/>
+    <tableColumn id="10" name="15/05" dataDxfId="157"/>
+    <tableColumn id="11" name="16/05" dataDxfId="156"/>
+    <tableColumn id="12" name="17/05" dataDxfId="155"/>
+    <tableColumn id="13" name="18/05" dataDxfId="154"/>
+    <tableColumn id="14" name="19/05" dataDxfId="153"/>
+    <tableColumn id="15" name="End" dataDxfId="152"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table13456789" displayName="Table13456789" ref="B10:O54" totalsRowShown="0" headerRowDxfId="151" dataDxfId="149" headerRowBorderDxfId="150" tableBorderDxfId="148" totalsRowBorderDxfId="147">
   <autoFilter ref="B10:O54">
     <filterColumn colId="5"/>
     <filterColumn colId="12"/>
@@ -13389,21 +14004,21 @@
     <tableColumn id="4" name="Assign To" dataDxfId="143"/>
     <tableColumn id="5" name="Status" dataDxfId="142"/>
     <tableColumn id="7" name="Estimate" dataDxfId="141"/>
-    <tableColumn id="8" name="13/05" dataDxfId="140"/>
-    <tableColumn id="9" name="14/05" dataDxfId="139"/>
-    <tableColumn id="10" name="15/05" dataDxfId="138"/>
-    <tableColumn id="11" name="16/05" dataDxfId="137"/>
-    <tableColumn id="12" name="17/05" dataDxfId="136"/>
-    <tableColumn id="13" name="18/05" dataDxfId="135"/>
-    <tableColumn id="14" name="19/05" dataDxfId="134"/>
+    <tableColumn id="8" name="20/05" dataDxfId="140"/>
+    <tableColumn id="9" name="21/05" dataDxfId="139"/>
+    <tableColumn id="10" name="22/05" dataDxfId="138"/>
+    <tableColumn id="11" name="23/05" dataDxfId="137"/>
+    <tableColumn id="12" name="24/05" dataDxfId="136"/>
+    <tableColumn id="13" name="25/05" dataDxfId="135"/>
+    <tableColumn id="14" name="26/05" dataDxfId="134"/>
     <tableColumn id="15" name="End" dataDxfId="133"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table13456789" displayName="Table13456789" ref="B10:O54" totalsRowShown="0" headerRowDxfId="132" dataDxfId="130" headerRowBorderDxfId="131" tableBorderDxfId="129" totalsRowBorderDxfId="128">
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table1345678910" displayName="Table1345678910" ref="B10:O54" totalsRowShown="0" headerRowDxfId="132" dataDxfId="130" headerRowBorderDxfId="131" tableBorderDxfId="129" totalsRowBorderDxfId="128">
   <autoFilter ref="B10:O54">
     <filterColumn colId="5"/>
     <filterColumn colId="12"/>
@@ -13416,41 +14031,14 @@
     <tableColumn id="4" name="Assign To" dataDxfId="124"/>
     <tableColumn id="5" name="Status" dataDxfId="123"/>
     <tableColumn id="7" name="Estimate" dataDxfId="122"/>
-    <tableColumn id="8" name="20/05" dataDxfId="121"/>
-    <tableColumn id="9" name="21/05" dataDxfId="120"/>
-    <tableColumn id="10" name="22/05" dataDxfId="119"/>
-    <tableColumn id="11" name="23/05" dataDxfId="118"/>
-    <tableColumn id="12" name="24/05" dataDxfId="117"/>
-    <tableColumn id="13" name="25/05" dataDxfId="116"/>
-    <tableColumn id="14" name="26/05" dataDxfId="115"/>
+    <tableColumn id="8" name="27/05" dataDxfId="121"/>
+    <tableColumn id="9" name="28/05" dataDxfId="120"/>
+    <tableColumn id="10" name="29/05" dataDxfId="119"/>
+    <tableColumn id="11" name="30/05" dataDxfId="118"/>
+    <tableColumn id="12" name="31/05" dataDxfId="117"/>
+    <tableColumn id="13" name="01/06" dataDxfId="116"/>
+    <tableColumn id="14" name="02/06" dataDxfId="115"/>
     <tableColumn id="15" name="End" dataDxfId="114"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table1345678910" displayName="Table1345678910" ref="B10:O54" totalsRowShown="0" headerRowDxfId="113" dataDxfId="111" headerRowBorderDxfId="112" tableBorderDxfId="110" totalsRowBorderDxfId="109">
-  <autoFilter ref="B10:O54">
-    <filterColumn colId="5"/>
-    <filterColumn colId="12"/>
-    <filterColumn colId="13"/>
-  </autoFilter>
-  <tableColumns count="14">
-    <tableColumn id="1" name="No." dataDxfId="108"/>
-    <tableColumn id="2" name="Task description" dataDxfId="107"/>
-    <tableColumn id="3" name="Type" dataDxfId="106"/>
-    <tableColumn id="4" name="Assign To" dataDxfId="105"/>
-    <tableColumn id="5" name="Status" dataDxfId="104"/>
-    <tableColumn id="7" name="Estimate" dataDxfId="103"/>
-    <tableColumn id="8" name="27/05" dataDxfId="102"/>
-    <tableColumn id="9" name="28/05" dataDxfId="101"/>
-    <tableColumn id="10" name="29/05" dataDxfId="100"/>
-    <tableColumn id="11" name="30/05" dataDxfId="99"/>
-    <tableColumn id="12" name="31/05" dataDxfId="98"/>
-    <tableColumn id="13" name="01/06" dataDxfId="97"/>
-    <tableColumn id="14" name="02/06" dataDxfId="96"/>
-    <tableColumn id="15" name="End" dataDxfId="95"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -13831,7 +14419,7 @@
       </c>
     </row>
     <row r="14" spans="2:7">
-      <c r="C14" s="400">
+      <c r="C14" s="405">
         <v>2</v>
       </c>
       <c r="D14" s="17" t="s">
@@ -13842,7 +14430,7 @@
       </c>
     </row>
     <row r="15" spans="2:7">
-      <c r="C15" s="401"/>
+      <c r="C15" s="406"/>
       <c r="D15" s="3" t="s">
         <v>2</v>
       </c>
@@ -13850,28 +14438,28 @@
       <c r="G15" s="26"/>
     </row>
     <row r="16" spans="2:7">
-      <c r="C16" s="401"/>
+      <c r="C16" s="406"/>
       <c r="D16" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E16" s="19"/>
     </row>
     <row r="17" spans="3:8">
-      <c r="C17" s="401"/>
+      <c r="C17" s="406"/>
       <c r="D17" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E17" s="19"/>
     </row>
     <row r="18" spans="3:8">
-      <c r="C18" s="407"/>
+      <c r="C18" s="412"/>
       <c r="D18" s="20" t="s">
         <v>5</v>
       </c>
       <c r="E18" s="21"/>
     </row>
     <row r="19" spans="3:8">
-      <c r="C19" s="414">
+      <c r="C19" s="419">
         <v>3</v>
       </c>
       <c r="D19" s="51" t="s">
@@ -13882,7 +14470,7 @@
       </c>
     </row>
     <row r="20" spans="3:8">
-      <c r="C20" s="415"/>
+      <c r="C20" s="420"/>
       <c r="D20" s="4" t="s">
         <v>7</v>
       </c>
@@ -13892,7 +14480,7 @@
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="3:8">
-      <c r="C21" s="415"/>
+      <c r="C21" s="420"/>
       <c r="D21" s="3" t="s">
         <v>8</v>
       </c>
@@ -13902,42 +14490,42 @@
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="3:8">
-      <c r="C22" s="415"/>
+      <c r="C22" s="420"/>
       <c r="D22" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E22" s="50"/>
     </row>
     <row r="23" spans="3:8">
-      <c r="C23" s="415"/>
+      <c r="C23" s="420"/>
       <c r="D23" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E23" s="50"/>
     </row>
     <row r="24" spans="3:8">
-      <c r="C24" s="415"/>
+      <c r="C24" s="420"/>
       <c r="D24" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E24" s="50"/>
     </row>
     <row r="25" spans="3:8">
-      <c r="C25" s="415"/>
+      <c r="C25" s="420"/>
       <c r="D25" s="6" t="s">
         <v>12</v>
       </c>
       <c r="E25" s="50"/>
     </row>
     <row r="26" spans="3:8">
-      <c r="C26" s="416"/>
+      <c r="C26" s="421"/>
       <c r="D26" s="20" t="s">
         <v>31</v>
       </c>
       <c r="E26" s="53"/>
     </row>
     <row r="27" spans="3:8">
-      <c r="C27" s="400">
+      <c r="C27" s="405">
         <v>4</v>
       </c>
       <c r="D27" s="22" t="s">
@@ -13948,56 +14536,56 @@
       </c>
     </row>
     <row r="28" spans="3:8">
-      <c r="C28" s="401"/>
+      <c r="C28" s="406"/>
       <c r="D28" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E28" s="19"/>
     </row>
     <row r="29" spans="3:8">
-      <c r="C29" s="401"/>
+      <c r="C29" s="406"/>
       <c r="D29" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E29" s="19"/>
     </row>
     <row r="30" spans="3:8">
-      <c r="C30" s="401"/>
+      <c r="C30" s="406"/>
       <c r="D30" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E30" s="19"/>
     </row>
     <row r="31" spans="3:8">
-      <c r="C31" s="401"/>
+      <c r="C31" s="406"/>
       <c r="D31" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E31" s="19"/>
     </row>
     <row r="32" spans="3:8">
-      <c r="C32" s="401"/>
+      <c r="C32" s="406"/>
       <c r="D32" s="8" t="s">
         <v>18</v>
       </c>
       <c r="E32" s="19"/>
     </row>
     <row r="33" spans="2:7">
-      <c r="C33" s="401"/>
+      <c r="C33" s="406"/>
       <c r="D33" s="9" t="s">
         <v>19</v>
       </c>
       <c r="E33" s="19"/>
     </row>
     <row r="34" spans="2:7">
-      <c r="C34" s="407"/>
+      <c r="C34" s="412"/>
       <c r="D34" s="20" t="s">
         <v>32</v>
       </c>
       <c r="E34" s="21"/>
     </row>
     <row r="35" spans="2:7">
-      <c r="C35" s="406">
+      <c r="C35" s="411">
         <v>5</v>
       </c>
       <c r="D35" s="46" t="s">
@@ -14008,14 +14596,14 @@
       </c>
     </row>
     <row r="36" spans="2:7">
-      <c r="C36" s="404"/>
+      <c r="C36" s="409"/>
       <c r="D36" s="27" t="s">
         <v>21</v>
       </c>
       <c r="E36" s="48"/>
     </row>
     <row r="37" spans="2:7">
-      <c r="C37" s="404"/>
+      <c r="C37" s="409"/>
       <c r="D37" s="28" t="s">
         <v>22</v>
       </c>
@@ -14023,14 +14611,14 @@
       <c r="G37" s="30"/>
     </row>
     <row r="38" spans="2:7">
-      <c r="C38" s="411"/>
+      <c r="C38" s="416"/>
       <c r="D38" s="29" t="s">
         <v>23</v>
       </c>
       <c r="E38" s="49"/>
     </row>
     <row r="39" spans="2:7">
-      <c r="C39" s="400">
+      <c r="C39" s="405">
         <v>6</v>
       </c>
       <c r="D39" s="22" t="s">
@@ -14041,21 +14629,21 @@
       </c>
     </row>
     <row r="40" spans="2:7">
-      <c r="C40" s="401"/>
+      <c r="C40" s="406"/>
       <c r="D40" s="8" t="s">
         <v>25</v>
       </c>
       <c r="E40" s="19"/>
     </row>
     <row r="41" spans="2:7">
-      <c r="C41" s="407"/>
+      <c r="C41" s="412"/>
       <c r="D41" s="23" t="s">
         <v>26</v>
       </c>
       <c r="E41" s="21"/>
     </row>
     <row r="42" spans="2:7">
-      <c r="C42" s="412" t="s">
+      <c r="C42" s="417" t="s">
         <v>42</v>
       </c>
       <c r="D42" s="24" t="s">
@@ -14066,7 +14654,7 @@
       </c>
     </row>
     <row r="43" spans="2:7">
-      <c r="C43" s="413"/>
+      <c r="C43" s="418"/>
       <c r="D43" s="25" t="s">
         <v>44</v>
       </c>
@@ -14106,10 +14694,10 @@
       </c>
     </row>
     <row r="52" spans="2:5">
-      <c r="C52" s="410" t="s">
+      <c r="C52" s="415" t="s">
         <v>53</v>
       </c>
-      <c r="D52" s="410"/>
+      <c r="D52" s="415"/>
       <c r="E52" s="42"/>
     </row>
     <row r="53" spans="2:5">
@@ -14131,10 +14719,10 @@
       <c r="E54" s="40"/>
     </row>
     <row r="55" spans="2:5">
-      <c r="C55" s="408" t="s">
+      <c r="C55" s="413" t="s">
         <v>27</v>
       </c>
-      <c r="D55" s="409"/>
+      <c r="D55" s="414"/>
       <c r="E55" s="36"/>
     </row>
     <row r="56" spans="2:5">
@@ -14156,10 +14744,10 @@
       <c r="E57" s="40"/>
     </row>
     <row r="58" spans="2:5">
-      <c r="C58" s="408" t="s">
+      <c r="C58" s="413" t="s">
         <v>58</v>
       </c>
-      <c r="D58" s="409"/>
+      <c r="D58" s="414"/>
       <c r="E58" s="36"/>
     </row>
     <row r="59" spans="2:5">
@@ -14172,7 +14760,7 @@
       <c r="E59" s="37"/>
     </row>
     <row r="60" spans="2:5">
-      <c r="C60" s="401">
+      <c r="C60" s="406">
         <v>1</v>
       </c>
       <c r="D60" s="31" t="s">
@@ -14181,70 +14769,70 @@
       <c r="E60" s="19"/>
     </row>
     <row r="61" spans="2:5">
-      <c r="C61" s="401"/>
+      <c r="C61" s="406"/>
       <c r="D61" s="32" t="s">
         <v>60</v>
       </c>
       <c r="E61" s="19"/>
     </row>
     <row r="62" spans="2:5">
-      <c r="C62" s="401"/>
+      <c r="C62" s="406"/>
       <c r="D62" s="33" t="s">
         <v>61</v>
       </c>
       <c r="E62" s="21"/>
     </row>
     <row r="63" spans="2:5">
-      <c r="C63" s="401"/>
+      <c r="C63" s="406"/>
       <c r="D63" s="32" t="s">
         <v>62</v>
       </c>
       <c r="E63" s="18"/>
     </row>
     <row r="64" spans="2:5">
-      <c r="C64" s="401"/>
+      <c r="C64" s="406"/>
       <c r="D64" s="33" t="s">
         <v>28</v>
       </c>
       <c r="E64" s="19"/>
     </row>
     <row r="65" spans="3:5">
-      <c r="C65" s="401"/>
+      <c r="C65" s="406"/>
       <c r="D65" s="34" t="s">
         <v>63</v>
       </c>
       <c r="E65" s="21"/>
     </row>
     <row r="66" spans="3:5">
-      <c r="C66" s="401"/>
+      <c r="C66" s="406"/>
       <c r="D66" s="35" t="s">
         <v>64</v>
       </c>
       <c r="E66" s="18"/>
     </row>
     <row r="67" spans="3:5">
-      <c r="C67" s="401"/>
+      <c r="C67" s="406"/>
       <c r="D67" s="32" t="s">
         <v>65</v>
       </c>
       <c r="E67" s="19"/>
     </row>
     <row r="68" spans="3:5">
-      <c r="C68" s="401"/>
+      <c r="C68" s="406"/>
       <c r="D68" s="35" t="s">
         <v>66</v>
       </c>
       <c r="E68" s="21"/>
     </row>
     <row r="69" spans="3:5">
-      <c r="C69" s="407"/>
+      <c r="C69" s="412"/>
       <c r="D69" s="34" t="s">
         <v>29</v>
       </c>
       <c r="E69" s="18"/>
     </row>
     <row r="70" spans="3:5">
-      <c r="C70" s="406">
+      <c r="C70" s="411">
         <v>2</v>
       </c>
       <c r="D70" s="57" t="s">
@@ -14253,35 +14841,35 @@
       <c r="E70" s="47"/>
     </row>
     <row r="71" spans="3:5">
-      <c r="C71" s="404"/>
+      <c r="C71" s="409"/>
       <c r="D71" s="32" t="s">
         <v>67</v>
       </c>
       <c r="E71" s="48"/>
     </row>
     <row r="72" spans="3:5">
-      <c r="C72" s="404"/>
+      <c r="C72" s="409"/>
       <c r="D72" s="33" t="s">
         <v>68</v>
       </c>
       <c r="E72" s="48"/>
     </row>
     <row r="73" spans="3:5">
-      <c r="C73" s="404"/>
+      <c r="C73" s="409"/>
       <c r="D73" s="32" t="s">
         <v>69</v>
       </c>
       <c r="E73" s="48"/>
     </row>
     <row r="74" spans="3:5">
-      <c r="C74" s="404"/>
+      <c r="C74" s="409"/>
       <c r="D74" s="32" t="s">
         <v>134</v>
       </c>
       <c r="E74" s="49"/>
     </row>
     <row r="75" spans="3:5">
-      <c r="C75" s="400">
+      <c r="C75" s="405">
         <v>3</v>
       </c>
       <c r="D75" s="44" t="s">
@@ -14290,42 +14878,42 @@
       <c r="E75" s="18"/>
     </row>
     <row r="76" spans="3:5">
-      <c r="C76" s="401"/>
+      <c r="C76" s="406"/>
       <c r="D76" s="32" t="s">
         <v>71</v>
       </c>
       <c r="E76" s="19"/>
     </row>
     <row r="77" spans="3:5">
-      <c r="C77" s="401"/>
+      <c r="C77" s="406"/>
       <c r="D77" s="33" t="s">
         <v>72</v>
       </c>
       <c r="E77" s="21"/>
     </row>
     <row r="78" spans="3:5">
-      <c r="C78" s="401"/>
+      <c r="C78" s="406"/>
       <c r="D78" s="32" t="s">
         <v>73</v>
       </c>
       <c r="E78" s="18"/>
     </row>
     <row r="79" spans="3:5">
-      <c r="C79" s="401"/>
+      <c r="C79" s="406"/>
       <c r="D79" s="33" t="s">
         <v>74</v>
       </c>
       <c r="E79" s="19"/>
     </row>
     <row r="80" spans="3:5" ht="15.75" thickBot="1">
-      <c r="C80" s="402"/>
+      <c r="C80" s="407"/>
       <c r="D80" s="32" t="s">
         <v>75</v>
       </c>
       <c r="E80" s="21"/>
     </row>
     <row r="81" spans="3:5">
-      <c r="C81" s="403">
+      <c r="C81" s="408">
         <v>4</v>
       </c>
       <c r="D81" s="57" t="s">
@@ -14334,63 +14922,63 @@
       <c r="E81" s="48"/>
     </row>
     <row r="82" spans="3:5">
-      <c r="C82" s="404"/>
+      <c r="C82" s="409"/>
       <c r="D82" s="32" t="s">
         <v>77</v>
       </c>
       <c r="E82" s="48"/>
     </row>
     <row r="83" spans="3:5">
-      <c r="C83" s="404"/>
+      <c r="C83" s="409"/>
       <c r="D83" s="33" t="s">
         <v>78</v>
       </c>
       <c r="E83" s="48"/>
     </row>
     <row r="84" spans="3:5">
-      <c r="C84" s="404"/>
+      <c r="C84" s="409"/>
       <c r="D84" s="32" t="s">
         <v>79</v>
       </c>
       <c r="E84" s="48"/>
     </row>
     <row r="85" spans="3:5">
-      <c r="C85" s="404"/>
+      <c r="C85" s="409"/>
       <c r="D85" s="33" t="s">
         <v>80</v>
       </c>
       <c r="E85" s="48"/>
     </row>
     <row r="86" spans="3:5">
-      <c r="C86" s="404"/>
+      <c r="C86" s="409"/>
       <c r="D86" s="32" t="s">
         <v>137</v>
       </c>
       <c r="E86" s="48"/>
     </row>
     <row r="87" spans="3:5">
-      <c r="C87" s="404"/>
+      <c r="C87" s="409"/>
       <c r="D87" s="35" t="s">
         <v>81</v>
       </c>
       <c r="E87" s="48"/>
     </row>
     <row r="88" spans="3:5">
-      <c r="C88" s="404"/>
+      <c r="C88" s="409"/>
       <c r="D88" s="34" t="s">
         <v>82</v>
       </c>
       <c r="E88" s="48"/>
     </row>
     <row r="89" spans="3:5" ht="15.75" thickBot="1">
-      <c r="C89" s="405"/>
+      <c r="C89" s="410"/>
       <c r="D89" s="35" t="s">
         <v>83</v>
       </c>
       <c r="E89" s="48"/>
     </row>
     <row r="90" spans="3:5">
-      <c r="C90" s="400">
+      <c r="C90" s="405">
         <v>5</v>
       </c>
       <c r="D90" s="44" t="s">
@@ -14399,28 +14987,28 @@
       <c r="E90" s="18"/>
     </row>
     <row r="91" spans="3:5">
-      <c r="C91" s="401"/>
+      <c r="C91" s="406"/>
       <c r="D91" s="33" t="s">
         <v>85</v>
       </c>
       <c r="E91" s="19"/>
     </row>
     <row r="92" spans="3:5">
-      <c r="C92" s="401"/>
+      <c r="C92" s="406"/>
       <c r="D92" s="32" t="s">
         <v>86</v>
       </c>
       <c r="E92" s="21"/>
     </row>
     <row r="93" spans="3:5">
-      <c r="C93" s="401"/>
+      <c r="C93" s="406"/>
       <c r="D93" s="33" t="s">
         <v>87</v>
       </c>
       <c r="E93" s="18"/>
     </row>
     <row r="94" spans="3:5">
-      <c r="C94" s="406">
+      <c r="C94" s="411">
         <v>6</v>
       </c>
       <c r="D94" s="57" t="s">
@@ -14429,21 +15017,21 @@
       <c r="E94" s="48"/>
     </row>
     <row r="95" spans="3:5">
-      <c r="C95" s="404"/>
+      <c r="C95" s="409"/>
       <c r="D95" s="33" t="s">
         <v>89</v>
       </c>
       <c r="E95" s="48"/>
     </row>
     <row r="96" spans="3:5">
-      <c r="C96" s="404"/>
+      <c r="C96" s="409"/>
       <c r="D96" s="32" t="s">
         <v>90</v>
       </c>
       <c r="E96" s="48"/>
     </row>
     <row r="97" spans="3:5">
-      <c r="C97" s="400">
+      <c r="C97" s="405">
         <v>7</v>
       </c>
       <c r="D97" s="44" t="s">
@@ -14452,35 +15040,35 @@
       <c r="E97" s="18"/>
     </row>
     <row r="98" spans="3:5">
-      <c r="C98" s="401"/>
+      <c r="C98" s="406"/>
       <c r="D98" s="32" t="s">
         <v>92</v>
       </c>
       <c r="E98" s="18"/>
     </row>
     <row r="99" spans="3:5">
-      <c r="C99" s="401"/>
+      <c r="C99" s="406"/>
       <c r="D99" s="33" t="s">
         <v>93</v>
       </c>
       <c r="E99" s="18"/>
     </row>
     <row r="100" spans="3:5">
-      <c r="C100" s="401"/>
+      <c r="C100" s="406"/>
       <c r="D100" s="32" t="s">
         <v>94</v>
       </c>
       <c r="E100" s="18"/>
     </row>
     <row r="101" spans="3:5">
-      <c r="C101" s="407"/>
+      <c r="C101" s="412"/>
       <c r="D101" s="33" t="s">
         <v>95</v>
       </c>
       <c r="E101" s="18"/>
     </row>
     <row r="102" spans="3:5">
-      <c r="C102" s="406">
+      <c r="C102" s="411">
         <v>8</v>
       </c>
       <c r="D102" s="57" t="s">
@@ -14489,21 +15077,21 @@
       <c r="E102" s="48"/>
     </row>
     <row r="103" spans="3:5">
-      <c r="C103" s="404"/>
+      <c r="C103" s="409"/>
       <c r="D103" s="33" t="s">
         <v>97</v>
       </c>
       <c r="E103" s="48"/>
     </row>
     <row r="104" spans="3:5">
-      <c r="C104" s="404"/>
+      <c r="C104" s="409"/>
       <c r="D104" s="32" t="s">
         <v>98</v>
       </c>
       <c r="E104" s="48"/>
     </row>
     <row r="105" spans="3:5">
-      <c r="C105" s="400" t="s">
+      <c r="C105" s="405" t="s">
         <v>99</v>
       </c>
       <c r="D105" s="58" t="s">
@@ -14514,7 +15102,7 @@
       </c>
     </row>
     <row r="106" spans="3:5">
-      <c r="C106" s="401"/>
+      <c r="C106" s="406"/>
       <c r="D106" s="38"/>
       <c r="E106" s="18"/>
     </row>
@@ -14587,12 +15175,12 @@
       <c r="C6" s="14"/>
     </row>
     <row r="7" spans="2:15" ht="18">
-      <c r="B7" s="417" t="s">
+      <c r="B7" s="422" t="s">
         <v>393</v>
       </c>
-      <c r="C7" s="417"/>
-      <c r="D7" s="417"/>
-      <c r="E7" s="417"/>
+      <c r="C7" s="422"/>
+      <c r="D7" s="422"/>
+      <c r="E7" s="422"/>
     </row>
     <row r="10" spans="2:15" s="107" customFormat="1" ht="12" customHeight="1">
       <c r="B10" s="275" t="s">
@@ -16248,12 +16836,12 @@
       <c r="C6" s="14"/>
     </row>
     <row r="7" spans="2:15" ht="18">
-      <c r="B7" s="417" t="s">
+      <c r="B7" s="422" t="s">
         <v>410</v>
       </c>
-      <c r="C7" s="417"/>
-      <c r="D7" s="417"/>
-      <c r="E7" s="417"/>
+      <c r="C7" s="422"/>
+      <c r="D7" s="422"/>
+      <c r="E7" s="422"/>
     </row>
     <row r="10" spans="2:15" s="107" customFormat="1" ht="12" customHeight="1">
       <c r="B10" s="275" t="s">
@@ -17779,12 +18367,12 @@
       <c r="C6" s="14"/>
     </row>
     <row r="7" spans="2:15" ht="18">
-      <c r="B7" s="417" t="s">
+      <c r="B7" s="422" t="s">
         <v>413</v>
       </c>
-      <c r="C7" s="417"/>
-      <c r="D7" s="417"/>
-      <c r="E7" s="417"/>
+      <c r="C7" s="422"/>
+      <c r="D7" s="422"/>
+      <c r="E7" s="422"/>
     </row>
     <row r="10" spans="2:15" s="107" customFormat="1" ht="12" customHeight="1">
       <c r="B10" s="275" t="s">
@@ -19348,12 +19936,12 @@
       <c r="C6" s="14"/>
     </row>
     <row r="7" spans="2:15" ht="18">
-      <c r="B7" s="417" t="s">
+      <c r="B7" s="422" t="s">
         <v>458</v>
       </c>
-      <c r="C7" s="417"/>
-      <c r="D7" s="417"/>
-      <c r="E7" s="417"/>
+      <c r="C7" s="422"/>
+      <c r="D7" s="422"/>
+      <c r="E7" s="422"/>
     </row>
     <row r="10" spans="2:15" s="107" customFormat="1" ht="12" customHeight="1">
       <c r="B10" s="275" t="s">
@@ -19374,28 +19962,28 @@
       <c r="G10" s="310" t="s">
         <v>347</v>
       </c>
-      <c r="H10" s="419" t="s">
+      <c r="H10" s="401" t="s">
         <v>434</v>
       </c>
-      <c r="I10" s="419" t="s">
+      <c r="I10" s="401" t="s">
         <v>435</v>
       </c>
-      <c r="J10" s="420" t="s">
+      <c r="J10" s="402" t="s">
         <v>436</v>
       </c>
-      <c r="K10" s="420" t="s">
+      <c r="K10" s="402" t="s">
         <v>437</v>
       </c>
-      <c r="L10" s="420" t="s">
+      <c r="L10" s="402" t="s">
         <v>438</v>
       </c>
-      <c r="M10" s="420" t="s">
+      <c r="M10" s="402" t="s">
         <v>439</v>
       </c>
-      <c r="N10" s="421" t="s">
+      <c r="N10" s="403" t="s">
         <v>440</v>
       </c>
-      <c r="O10" s="422" t="s">
+      <c r="O10" s="404" t="s">
         <v>284</v>
       </c>
     </row>
@@ -20785,12 +21373,12 @@
       <c r="C6" s="14"/>
     </row>
     <row r="7" spans="2:15" ht="18">
-      <c r="B7" s="417" t="s">
+      <c r="B7" s="422" t="s">
         <v>448</v>
       </c>
-      <c r="C7" s="417"/>
-      <c r="D7" s="417"/>
-      <c r="E7" s="417"/>
+      <c r="C7" s="422"/>
+      <c r="D7" s="422"/>
+      <c r="E7" s="422"/>
     </row>
     <row r="10" spans="2:15" s="107" customFormat="1" ht="12" customHeight="1">
       <c r="B10" s="275" t="s">
@@ -21110,7 +21698,7 @@
       <c r="D17" s="369" t="s">
         <v>107</v>
       </c>
-      <c r="E17" s="418" t="s">
+      <c r="E17" s="400" t="s">
         <v>352</v>
       </c>
       <c r="F17" s="369" t="s">
@@ -22199,10 +22787,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:O121"/>
+  <dimension ref="B2:O122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22240,12 +22828,12 @@
       <c r="C6" s="14"/>
     </row>
     <row r="7" spans="2:15" ht="18">
-      <c r="B7" s="417" t="s">
+      <c r="B7" s="422" t="s">
         <v>459</v>
       </c>
-      <c r="C7" s="417"/>
-      <c r="D7" s="417"/>
-      <c r="E7" s="417"/>
+      <c r="C7" s="422"/>
+      <c r="D7" s="422"/>
+      <c r="E7" s="422"/>
     </row>
     <row r="10" spans="2:15" s="107" customFormat="1" ht="12" customHeight="1">
       <c r="B10" s="275" t="s">
@@ -22309,6 +22897,1505 @@
       </c>
       <c r="G11" s="367">
         <v>25</v>
+      </c>
+      <c r="H11" s="356">
+        <v>23</v>
+      </c>
+      <c r="I11" s="357">
+        <v>20</v>
+      </c>
+      <c r="J11" s="357">
+        <v>18</v>
+      </c>
+      <c r="K11" s="357">
+        <v>17</v>
+      </c>
+      <c r="L11" s="357">
+        <v>16</v>
+      </c>
+      <c r="M11" s="357">
+        <v>15</v>
+      </c>
+      <c r="N11" s="371">
+        <v>15</v>
+      </c>
+      <c r="O11" s="371">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15">
+      <c r="B12" s="335">
+        <v>2</v>
+      </c>
+      <c r="C12" s="372" t="s">
+        <v>414</v>
+      </c>
+      <c r="D12" s="365" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="366" t="s">
+        <v>351</v>
+      </c>
+      <c r="F12" s="365" t="s">
+        <v>117</v>
+      </c>
+      <c r="G12" s="367">
+        <v>20</v>
+      </c>
+      <c r="H12" s="356">
+        <v>20</v>
+      </c>
+      <c r="I12" s="357">
+        <v>20</v>
+      </c>
+      <c r="J12" s="357">
+        <v>20</v>
+      </c>
+      <c r="K12" s="357">
+        <v>20</v>
+      </c>
+      <c r="L12" s="356">
+        <v>20</v>
+      </c>
+      <c r="M12" s="356">
+        <v>20</v>
+      </c>
+      <c r="N12" s="371">
+        <v>20</v>
+      </c>
+      <c r="O12" s="371">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15">
+      <c r="B13" s="338">
+        <v>3</v>
+      </c>
+      <c r="C13" s="368" t="s">
+        <v>469</v>
+      </c>
+      <c r="D13" s="289" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="336" t="s">
+        <v>349</v>
+      </c>
+      <c r="F13" s="359" t="s">
+        <v>117</v>
+      </c>
+      <c r="G13" s="360">
+        <v>20</v>
+      </c>
+      <c r="H13" s="373">
+        <v>20</v>
+      </c>
+      <c r="I13" s="373">
+        <v>20</v>
+      </c>
+      <c r="J13" s="373">
+        <v>20</v>
+      </c>
+      <c r="K13" s="373">
+        <v>20</v>
+      </c>
+      <c r="L13" s="373">
+        <v>20</v>
+      </c>
+      <c r="M13" s="373">
+        <v>20</v>
+      </c>
+      <c r="N13" s="371">
+        <v>20</v>
+      </c>
+      <c r="O13" s="371">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15">
+      <c r="B14" s="338">
+        <v>4</v>
+      </c>
+      <c r="C14" s="368" t="s">
+        <v>467</v>
+      </c>
+      <c r="D14" s="354" t="s">
+        <v>107</v>
+      </c>
+      <c r="E14" s="366" t="s">
+        <v>349</v>
+      </c>
+      <c r="F14" s="369" t="s">
+        <v>117</v>
+      </c>
+      <c r="G14" s="367">
+        <v>10</v>
+      </c>
+      <c r="H14" s="373">
+        <v>10</v>
+      </c>
+      <c r="I14" s="373">
+        <v>10</v>
+      </c>
+      <c r="J14" s="373">
+        <v>10</v>
+      </c>
+      <c r="K14" s="373">
+        <v>10</v>
+      </c>
+      <c r="L14" s="373">
+        <v>10</v>
+      </c>
+      <c r="M14" s="373">
+        <v>10</v>
+      </c>
+      <c r="N14" s="371">
+        <v>10</v>
+      </c>
+      <c r="O14" s="371">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15">
+      <c r="B15" s="335">
+        <v>5</v>
+      </c>
+      <c r="C15" s="368" t="s">
+        <v>473</v>
+      </c>
+      <c r="D15" s="354" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="366" t="s">
+        <v>349</v>
+      </c>
+      <c r="F15" s="369" t="s">
+        <v>119</v>
+      </c>
+      <c r="G15" s="367">
+        <v>8</v>
+      </c>
+      <c r="H15" s="373">
+        <v>6</v>
+      </c>
+      <c r="I15" s="373">
+        <v>4</v>
+      </c>
+      <c r="J15" s="373">
+        <v>3</v>
+      </c>
+      <c r="K15" s="373">
+        <v>2</v>
+      </c>
+      <c r="L15" s="373">
+        <v>0</v>
+      </c>
+      <c r="M15" s="373">
+        <v>0</v>
+      </c>
+      <c r="N15" s="371">
+        <v>0</v>
+      </c>
+      <c r="O15" s="371">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15">
+      <c r="B16" s="338">
+        <v>6</v>
+      </c>
+      <c r="C16" s="368" t="s">
+        <v>468</v>
+      </c>
+      <c r="D16" s="354" t="s">
+        <v>107</v>
+      </c>
+      <c r="E16" s="366" t="s">
+        <v>349</v>
+      </c>
+      <c r="F16" s="369" t="s">
+        <v>119</v>
+      </c>
+      <c r="G16" s="367">
+        <v>20</v>
+      </c>
+      <c r="H16" s="326">
+        <v>15</v>
+      </c>
+      <c r="I16" s="339">
+        <v>12</v>
+      </c>
+      <c r="J16" s="339">
+        <v>9</v>
+      </c>
+      <c r="K16" s="339">
+        <v>7</v>
+      </c>
+      <c r="L16" s="339">
+        <v>5</v>
+      </c>
+      <c r="M16" s="331">
+        <v>3</v>
+      </c>
+      <c r="N16" s="362">
+        <v>0</v>
+      </c>
+      <c r="O16" s="362">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" s="197" customFormat="1">
+      <c r="B17" s="338">
+        <v>7</v>
+      </c>
+      <c r="C17" s="385" t="s">
+        <v>470</v>
+      </c>
+      <c r="D17" s="365" t="s">
+        <v>107</v>
+      </c>
+      <c r="E17" s="366" t="s">
+        <v>352</v>
+      </c>
+      <c r="F17" s="365" t="s">
+        <v>117</v>
+      </c>
+      <c r="G17" s="367">
+        <v>15</v>
+      </c>
+      <c r="H17" s="356">
+        <v>15</v>
+      </c>
+      <c r="I17" s="357">
+        <v>15</v>
+      </c>
+      <c r="J17" s="357">
+        <v>15</v>
+      </c>
+      <c r="K17" s="357">
+        <v>15</v>
+      </c>
+      <c r="L17" s="357">
+        <v>15</v>
+      </c>
+      <c r="M17" s="357">
+        <v>15</v>
+      </c>
+      <c r="N17" s="371">
+        <v>15</v>
+      </c>
+      <c r="O17" s="371">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" s="197" customFormat="1">
+      <c r="B18" s="335">
+        <v>8</v>
+      </c>
+      <c r="C18" s="368" t="s">
+        <v>471</v>
+      </c>
+      <c r="D18" s="369" t="s">
+        <v>107</v>
+      </c>
+      <c r="E18" s="400" t="s">
+        <v>352</v>
+      </c>
+      <c r="F18" s="369" t="s">
+        <v>117</v>
+      </c>
+      <c r="G18" s="367">
+        <v>15</v>
+      </c>
+      <c r="H18" s="356">
+        <v>15</v>
+      </c>
+      <c r="I18" s="357">
+        <v>15</v>
+      </c>
+      <c r="J18" s="357">
+        <v>15</v>
+      </c>
+      <c r="K18" s="357">
+        <v>15</v>
+      </c>
+      <c r="L18" s="357">
+        <v>15</v>
+      </c>
+      <c r="M18" s="357">
+        <v>15</v>
+      </c>
+      <c r="N18" s="399">
+        <v>15</v>
+      </c>
+      <c r="O18" s="399">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" s="197" customFormat="1">
+      <c r="B19" s="338">
+        <v>9</v>
+      </c>
+      <c r="C19" s="385" t="s">
+        <v>446</v>
+      </c>
+      <c r="D19" s="365" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" s="366" t="s">
+        <v>350</v>
+      </c>
+      <c r="F19" s="365" t="s">
+        <v>117</v>
+      </c>
+      <c r="G19" s="367">
+        <v>20</v>
+      </c>
+      <c r="H19" s="356">
+        <v>18</v>
+      </c>
+      <c r="I19" s="357">
+        <v>15</v>
+      </c>
+      <c r="J19" s="357">
+        <v>13</v>
+      </c>
+      <c r="K19" s="356">
+        <v>10</v>
+      </c>
+      <c r="L19" s="356">
+        <v>10</v>
+      </c>
+      <c r="M19" s="356">
+        <v>10</v>
+      </c>
+      <c r="N19" s="371">
+        <v>10</v>
+      </c>
+      <c r="O19" s="371">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" s="197" customFormat="1" ht="36" customHeight="1">
+      <c r="B20" s="338">
+        <v>10</v>
+      </c>
+      <c r="C20" s="374" t="s">
+        <v>472</v>
+      </c>
+      <c r="D20" s="354" t="s">
+        <v>107</v>
+      </c>
+      <c r="E20" s="355" t="s">
+        <v>350</v>
+      </c>
+      <c r="F20" s="369" t="s">
+        <v>119</v>
+      </c>
+      <c r="G20" s="367">
+        <v>10</v>
+      </c>
+      <c r="H20" s="326">
+        <v>8</v>
+      </c>
+      <c r="I20" s="339">
+        <v>5</v>
+      </c>
+      <c r="J20" s="339">
+        <v>3</v>
+      </c>
+      <c r="K20" s="339">
+        <v>1</v>
+      </c>
+      <c r="L20" s="339">
+        <v>0</v>
+      </c>
+      <c r="M20" s="331">
+        <v>0</v>
+      </c>
+      <c r="N20" s="398">
+        <v>0</v>
+      </c>
+      <c r="O20" s="398">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15">
+      <c r="B21" s="335">
+        <v>11</v>
+      </c>
+      <c r="C21" s="368"/>
+      <c r="D21" s="354"/>
+      <c r="E21" s="355"/>
+      <c r="F21" s="369"/>
+      <c r="G21" s="367"/>
+      <c r="H21" s="356"/>
+      <c r="I21" s="357"/>
+      <c r="J21" s="357"/>
+      <c r="K21" s="357"/>
+      <c r="L21" s="357"/>
+      <c r="M21" s="357"/>
+      <c r="N21" s="399"/>
+      <c r="O21" s="399"/>
+    </row>
+    <row r="22" spans="2:15">
+      <c r="B22" s="338">
+        <v>12</v>
+      </c>
+      <c r="C22" s="372"/>
+      <c r="D22" s="354"/>
+      <c r="E22" s="355"/>
+      <c r="F22" s="369"/>
+      <c r="G22" s="367"/>
+      <c r="H22" s="356"/>
+      <c r="I22" s="357"/>
+      <c r="J22" s="357"/>
+      <c r="K22" s="357"/>
+      <c r="L22" s="357"/>
+      <c r="M22" s="357"/>
+      <c r="N22" s="399"/>
+      <c r="O22" s="399"/>
+    </row>
+    <row r="23" spans="2:15">
+      <c r="B23" s="338">
+        <v>13</v>
+      </c>
+      <c r="C23" s="374"/>
+      <c r="D23" s="365"/>
+      <c r="E23" s="355"/>
+      <c r="F23" s="369"/>
+      <c r="G23" s="367"/>
+      <c r="H23" s="367"/>
+      <c r="I23" s="367"/>
+      <c r="J23" s="367"/>
+      <c r="K23" s="367"/>
+      <c r="L23" s="367"/>
+      <c r="M23" s="367"/>
+      <c r="N23" s="399"/>
+      <c r="O23" s="399"/>
+    </row>
+    <row r="24" spans="2:15">
+      <c r="B24" s="335">
+        <v>14</v>
+      </c>
+      <c r="C24" s="385"/>
+      <c r="D24" s="365"/>
+      <c r="E24" s="355"/>
+      <c r="F24" s="369"/>
+      <c r="G24" s="367"/>
+      <c r="H24" s="367"/>
+      <c r="I24" s="367"/>
+      <c r="J24" s="367"/>
+      <c r="K24" s="367"/>
+      <c r="L24" s="367"/>
+      <c r="M24" s="367"/>
+      <c r="N24" s="399"/>
+      <c r="O24" s="399"/>
+    </row>
+    <row r="25" spans="2:15">
+      <c r="B25" s="338">
+        <v>15</v>
+      </c>
+      <c r="C25" s="386"/>
+      <c r="D25" s="354"/>
+      <c r="E25" s="355"/>
+      <c r="F25" s="369"/>
+      <c r="G25" s="367"/>
+      <c r="H25" s="356"/>
+      <c r="I25" s="357"/>
+      <c r="J25" s="357"/>
+      <c r="K25" s="357"/>
+      <c r="L25" s="357"/>
+      <c r="M25" s="357"/>
+      <c r="N25" s="399"/>
+      <c r="O25" s="399"/>
+    </row>
+    <row r="26" spans="2:15">
+      <c r="B26" s="338">
+        <v>16</v>
+      </c>
+      <c r="C26" s="385"/>
+      <c r="D26" s="354"/>
+      <c r="E26" s="355"/>
+      <c r="F26" s="369"/>
+      <c r="G26" s="367"/>
+      <c r="H26" s="356"/>
+      <c r="I26" s="357"/>
+      <c r="J26" s="357"/>
+      <c r="K26" s="357"/>
+      <c r="L26" s="357"/>
+      <c r="M26" s="357"/>
+      <c r="N26" s="399"/>
+      <c r="O26" s="399"/>
+    </row>
+    <row r="27" spans="2:15">
+      <c r="B27" s="335">
+        <v>17</v>
+      </c>
+      <c r="C27" s="372"/>
+      <c r="D27" s="354"/>
+      <c r="E27" s="355"/>
+      <c r="F27" s="369"/>
+      <c r="G27" s="367"/>
+      <c r="H27" s="326"/>
+      <c r="I27" s="339"/>
+      <c r="J27" s="339"/>
+      <c r="K27" s="339"/>
+      <c r="L27" s="339"/>
+      <c r="M27" s="331"/>
+      <c r="N27" s="398"/>
+      <c r="O27" s="398"/>
+    </row>
+    <row r="28" spans="2:15">
+      <c r="B28" s="338">
+        <v>18</v>
+      </c>
+      <c r="C28" s="368"/>
+      <c r="D28" s="354"/>
+      <c r="E28" s="355"/>
+      <c r="F28" s="369"/>
+      <c r="G28" s="367"/>
+      <c r="H28" s="326"/>
+      <c r="I28" s="326"/>
+      <c r="J28" s="326"/>
+      <c r="K28" s="326"/>
+      <c r="L28" s="326"/>
+      <c r="M28" s="333"/>
+      <c r="N28" s="398"/>
+      <c r="O28" s="398"/>
+    </row>
+    <row r="29" spans="2:15">
+      <c r="B29" s="338">
+        <v>19</v>
+      </c>
+      <c r="C29" s="368"/>
+      <c r="D29" s="354"/>
+      <c r="E29" s="355"/>
+      <c r="F29" s="369"/>
+      <c r="G29" s="367"/>
+      <c r="H29" s="326"/>
+      <c r="I29" s="326"/>
+      <c r="J29" s="326"/>
+      <c r="K29" s="326"/>
+      <c r="L29" s="326"/>
+      <c r="M29" s="333"/>
+      <c r="N29" s="398"/>
+      <c r="O29" s="398"/>
+    </row>
+    <row r="30" spans="2:15" ht="21.75" customHeight="1">
+      <c r="B30" s="335">
+        <v>20</v>
+      </c>
+      <c r="C30" s="366"/>
+      <c r="D30" s="365"/>
+      <c r="E30" s="366"/>
+      <c r="F30" s="365"/>
+      <c r="G30" s="367"/>
+      <c r="H30" s="356"/>
+      <c r="I30" s="356"/>
+      <c r="J30" s="356"/>
+      <c r="K30" s="356"/>
+      <c r="L30" s="356"/>
+      <c r="M30" s="356"/>
+      <c r="N30" s="371"/>
+      <c r="O30" s="371"/>
+    </row>
+    <row r="31" spans="2:15">
+      <c r="B31" s="338">
+        <v>21</v>
+      </c>
+      <c r="C31" s="366"/>
+      <c r="D31" s="365"/>
+      <c r="E31" s="366"/>
+      <c r="F31" s="365"/>
+      <c r="G31" s="367"/>
+      <c r="H31" s="373"/>
+      <c r="I31" s="373"/>
+      <c r="J31" s="373"/>
+      <c r="K31" s="373"/>
+      <c r="L31" s="373"/>
+      <c r="M31" s="373"/>
+      <c r="N31" s="371"/>
+      <c r="O31" s="371"/>
+    </row>
+    <row r="32" spans="2:15">
+      <c r="B32" s="338">
+        <v>22</v>
+      </c>
+      <c r="C32" s="366"/>
+      <c r="D32" s="365"/>
+      <c r="E32" s="366"/>
+      <c r="F32" s="365"/>
+      <c r="G32" s="367"/>
+      <c r="H32" s="373"/>
+      <c r="I32" s="373"/>
+      <c r="J32" s="373"/>
+      <c r="K32" s="373"/>
+      <c r="L32" s="373"/>
+      <c r="M32" s="373"/>
+      <c r="N32" s="371"/>
+      <c r="O32" s="371"/>
+    </row>
+    <row r="33" spans="2:15">
+      <c r="B33" s="335">
+        <v>23</v>
+      </c>
+      <c r="C33" s="366"/>
+      <c r="D33" s="365"/>
+      <c r="E33" s="366"/>
+      <c r="F33" s="365"/>
+      <c r="G33" s="367"/>
+      <c r="H33" s="373"/>
+      <c r="I33" s="373"/>
+      <c r="J33" s="373"/>
+      <c r="K33" s="373"/>
+      <c r="L33" s="373"/>
+      <c r="M33" s="373"/>
+      <c r="N33" s="371"/>
+      <c r="O33" s="371"/>
+    </row>
+    <row r="34" spans="2:15">
+      <c r="B34" s="338">
+        <v>24</v>
+      </c>
+      <c r="C34" s="366"/>
+      <c r="D34" s="365"/>
+      <c r="E34" s="366"/>
+      <c r="F34" s="365"/>
+      <c r="G34" s="367"/>
+      <c r="H34" s="373"/>
+      <c r="I34" s="373"/>
+      <c r="J34" s="373"/>
+      <c r="K34" s="373"/>
+      <c r="L34" s="373"/>
+      <c r="M34" s="373"/>
+      <c r="N34" s="371"/>
+      <c r="O34" s="371"/>
+    </row>
+    <row r="35" spans="2:15">
+      <c r="B35" s="338">
+        <v>25</v>
+      </c>
+      <c r="C35" s="366"/>
+      <c r="D35" s="365"/>
+      <c r="E35" s="366"/>
+      <c r="F35" s="365"/>
+      <c r="G35" s="367"/>
+      <c r="H35" s="373"/>
+      <c r="I35" s="373"/>
+      <c r="J35" s="373"/>
+      <c r="K35" s="373"/>
+      <c r="L35" s="373"/>
+      <c r="M35" s="373"/>
+      <c r="N35" s="371"/>
+      <c r="O35" s="371"/>
+    </row>
+    <row r="36" spans="2:15">
+      <c r="B36" s="335">
+        <v>26</v>
+      </c>
+      <c r="C36" s="366"/>
+      <c r="D36" s="365"/>
+      <c r="E36" s="366"/>
+      <c r="F36" s="365"/>
+      <c r="G36" s="367"/>
+      <c r="H36" s="326"/>
+      <c r="I36" s="326"/>
+      <c r="J36" s="326"/>
+      <c r="K36" s="326"/>
+      <c r="L36" s="326"/>
+      <c r="M36" s="333"/>
+      <c r="N36" s="362"/>
+      <c r="O36" s="362"/>
+    </row>
+    <row r="37" spans="2:15">
+      <c r="B37" s="338">
+        <v>27</v>
+      </c>
+      <c r="C37" s="375"/>
+      <c r="D37" s="289"/>
+      <c r="E37" s="336"/>
+      <c r="F37" s="359"/>
+      <c r="G37" s="360"/>
+      <c r="H37" s="326"/>
+      <c r="I37" s="326"/>
+      <c r="J37" s="326"/>
+      <c r="K37" s="326"/>
+      <c r="L37" s="326"/>
+      <c r="M37" s="333"/>
+      <c r="N37" s="362"/>
+      <c r="O37" s="362"/>
+    </row>
+    <row r="38" spans="2:15">
+      <c r="B38" s="338">
+        <v>28</v>
+      </c>
+      <c r="C38" s="366"/>
+      <c r="D38" s="365"/>
+      <c r="E38" s="366"/>
+      <c r="F38" s="365"/>
+      <c r="G38" s="367"/>
+      <c r="H38" s="326"/>
+      <c r="I38" s="326"/>
+      <c r="J38" s="326"/>
+      <c r="K38" s="326"/>
+      <c r="L38" s="326"/>
+      <c r="M38" s="333"/>
+      <c r="N38" s="362"/>
+      <c r="O38" s="362"/>
+    </row>
+    <row r="39" spans="2:15">
+      <c r="B39" s="335">
+        <v>29</v>
+      </c>
+      <c r="C39" s="366"/>
+      <c r="D39" s="365"/>
+      <c r="E39" s="366"/>
+      <c r="F39" s="365"/>
+      <c r="G39" s="367"/>
+      <c r="H39" s="326"/>
+      <c r="I39" s="326"/>
+      <c r="J39" s="326"/>
+      <c r="K39" s="326"/>
+      <c r="L39" s="326"/>
+      <c r="M39" s="333"/>
+      <c r="N39" s="362"/>
+      <c r="O39" s="362"/>
+    </row>
+    <row r="40" spans="2:15">
+      <c r="B40" s="338">
+        <v>30</v>
+      </c>
+      <c r="C40" s="366"/>
+      <c r="D40" s="365"/>
+      <c r="E40" s="366"/>
+      <c r="F40" s="365"/>
+      <c r="G40" s="367"/>
+      <c r="H40" s="326"/>
+      <c r="I40" s="326"/>
+      <c r="J40" s="326"/>
+      <c r="K40" s="326"/>
+      <c r="L40" s="326"/>
+      <c r="M40" s="333"/>
+      <c r="N40" s="362"/>
+      <c r="O40" s="362"/>
+    </row>
+    <row r="41" spans="2:15">
+      <c r="B41" s="338">
+        <v>31</v>
+      </c>
+      <c r="C41" s="366"/>
+      <c r="D41" s="365"/>
+      <c r="E41" s="366"/>
+      <c r="F41" s="365"/>
+      <c r="G41" s="367"/>
+      <c r="H41" s="326"/>
+      <c r="I41" s="326"/>
+      <c r="J41" s="326"/>
+      <c r="K41" s="326"/>
+      <c r="L41" s="326"/>
+      <c r="M41" s="333"/>
+      <c r="N41" s="362"/>
+      <c r="O41" s="362"/>
+    </row>
+    <row r="42" spans="2:15">
+      <c r="B42" s="335">
+        <v>32</v>
+      </c>
+      <c r="C42" s="366"/>
+      <c r="D42" s="365"/>
+      <c r="E42" s="366"/>
+      <c r="F42" s="365"/>
+      <c r="G42" s="367"/>
+      <c r="H42" s="326"/>
+      <c r="I42" s="326"/>
+      <c r="J42" s="326"/>
+      <c r="K42" s="326"/>
+      <c r="L42" s="326"/>
+      <c r="M42" s="333"/>
+      <c r="N42" s="362"/>
+      <c r="O42" s="362"/>
+    </row>
+    <row r="43" spans="2:15">
+      <c r="B43" s="338">
+        <v>33</v>
+      </c>
+      <c r="C43" s="366"/>
+      <c r="D43" s="365"/>
+      <c r="E43" s="366"/>
+      <c r="F43" s="365"/>
+      <c r="G43" s="367"/>
+      <c r="H43" s="326"/>
+      <c r="I43" s="326"/>
+      <c r="J43" s="326"/>
+      <c r="K43" s="326"/>
+      <c r="L43" s="326"/>
+      <c r="M43" s="333"/>
+      <c r="N43" s="362"/>
+      <c r="O43" s="362"/>
+    </row>
+    <row r="44" spans="2:15">
+      <c r="B44" s="338">
+        <v>34</v>
+      </c>
+      <c r="C44" s="366"/>
+      <c r="D44" s="365"/>
+      <c r="E44" s="366"/>
+      <c r="F44" s="365"/>
+      <c r="G44" s="367"/>
+      <c r="H44" s="326"/>
+      <c r="I44" s="326"/>
+      <c r="J44" s="326"/>
+      <c r="K44" s="326"/>
+      <c r="L44" s="326"/>
+      <c r="M44" s="333"/>
+      <c r="N44" s="362"/>
+      <c r="O44" s="362"/>
+    </row>
+    <row r="45" spans="2:15">
+      <c r="B45" s="335">
+        <v>35</v>
+      </c>
+      <c r="C45" s="366"/>
+      <c r="D45" s="365"/>
+      <c r="E45" s="366"/>
+      <c r="F45" s="365"/>
+      <c r="G45" s="367"/>
+      <c r="H45" s="326"/>
+      <c r="I45" s="326"/>
+      <c r="J45" s="326"/>
+      <c r="K45" s="326"/>
+      <c r="L45" s="326"/>
+      <c r="M45" s="333"/>
+      <c r="N45" s="362"/>
+      <c r="O45" s="362"/>
+    </row>
+    <row r="46" spans="2:15">
+      <c r="B46" s="338">
+        <v>36</v>
+      </c>
+      <c r="C46" s="366"/>
+      <c r="D46" s="365"/>
+      <c r="E46" s="366"/>
+      <c r="F46" s="365"/>
+      <c r="G46" s="367"/>
+      <c r="H46" s="326"/>
+      <c r="I46" s="326"/>
+      <c r="J46" s="326"/>
+      <c r="K46" s="326"/>
+      <c r="L46" s="326"/>
+      <c r="M46" s="333"/>
+      <c r="N46" s="362"/>
+      <c r="O46" s="362"/>
+    </row>
+    <row r="47" spans="2:15">
+      <c r="B47" s="338">
+        <v>37</v>
+      </c>
+      <c r="C47" s="366"/>
+      <c r="D47" s="365"/>
+      <c r="E47" s="366"/>
+      <c r="F47" s="365"/>
+      <c r="G47" s="367"/>
+      <c r="H47" s="326"/>
+      <c r="I47" s="326"/>
+      <c r="J47" s="326"/>
+      <c r="K47" s="326"/>
+      <c r="L47" s="326"/>
+      <c r="M47" s="333"/>
+      <c r="N47" s="362"/>
+      <c r="O47" s="362"/>
+    </row>
+    <row r="48" spans="2:15">
+      <c r="B48" s="335">
+        <v>38</v>
+      </c>
+      <c r="C48" s="366"/>
+      <c r="D48" s="365"/>
+      <c r="E48" s="366"/>
+      <c r="F48" s="365"/>
+      <c r="G48" s="367"/>
+      <c r="H48" s="326"/>
+      <c r="I48" s="326"/>
+      <c r="J48" s="326"/>
+      <c r="K48" s="326"/>
+      <c r="L48" s="326"/>
+      <c r="M48" s="333"/>
+      <c r="N48" s="362"/>
+      <c r="O48" s="362"/>
+    </row>
+    <row r="49" spans="2:15">
+      <c r="B49" s="338">
+        <v>39</v>
+      </c>
+      <c r="C49" s="366"/>
+      <c r="D49" s="365"/>
+      <c r="E49" s="366"/>
+      <c r="F49" s="365"/>
+      <c r="G49" s="367"/>
+      <c r="H49" s="326"/>
+      <c r="I49" s="326"/>
+      <c r="J49" s="326"/>
+      <c r="K49" s="326"/>
+      <c r="L49" s="326"/>
+      <c r="M49" s="333"/>
+      <c r="N49" s="362"/>
+      <c r="O49" s="362"/>
+    </row>
+    <row r="50" spans="2:15">
+      <c r="B50" s="338">
+        <v>40</v>
+      </c>
+      <c r="C50" s="366"/>
+      <c r="D50" s="365"/>
+      <c r="E50" s="366"/>
+      <c r="F50" s="365"/>
+      <c r="G50" s="367"/>
+      <c r="H50" s="326"/>
+      <c r="I50" s="326"/>
+      <c r="J50" s="326"/>
+      <c r="K50" s="326"/>
+      <c r="L50" s="326"/>
+      <c r="M50" s="333"/>
+      <c r="N50" s="362"/>
+      <c r="O50" s="362"/>
+    </row>
+    <row r="51" spans="2:15">
+      <c r="B51" s="335">
+        <v>41</v>
+      </c>
+      <c r="C51" s="366"/>
+      <c r="D51" s="365"/>
+      <c r="E51" s="366"/>
+      <c r="F51" s="365"/>
+      <c r="G51" s="367"/>
+      <c r="H51" s="326"/>
+      <c r="I51" s="326"/>
+      <c r="J51" s="326"/>
+      <c r="K51" s="326"/>
+      <c r="L51" s="326"/>
+      <c r="M51" s="333"/>
+      <c r="N51" s="362"/>
+      <c r="O51" s="362"/>
+    </row>
+    <row r="52" spans="2:15">
+      <c r="B52" s="338">
+        <v>42</v>
+      </c>
+      <c r="C52" s="366"/>
+      <c r="D52" s="365"/>
+      <c r="E52" s="366"/>
+      <c r="F52" s="365"/>
+      <c r="G52" s="367"/>
+      <c r="H52" s="326"/>
+      <c r="I52" s="326"/>
+      <c r="J52" s="326"/>
+      <c r="K52" s="326"/>
+      <c r="L52" s="326"/>
+      <c r="M52" s="333"/>
+      <c r="N52" s="362"/>
+      <c r="O52" s="362"/>
+    </row>
+    <row r="53" spans="2:15">
+      <c r="B53" s="338">
+        <v>43</v>
+      </c>
+      <c r="C53" s="366"/>
+      <c r="D53" s="365"/>
+      <c r="E53" s="366"/>
+      <c r="F53" s="365"/>
+      <c r="G53" s="367"/>
+      <c r="H53" s="326"/>
+      <c r="I53" s="326"/>
+      <c r="J53" s="326"/>
+      <c r="K53" s="326"/>
+      <c r="L53" s="326"/>
+      <c r="M53" s="333"/>
+      <c r="N53" s="362"/>
+      <c r="O53" s="362"/>
+    </row>
+    <row r="54" spans="2:15">
+      <c r="B54" s="335">
+        <v>44</v>
+      </c>
+      <c r="C54" s="366"/>
+      <c r="D54" s="365"/>
+      <c r="E54" s="366"/>
+      <c r="F54" s="365"/>
+      <c r="G54" s="367"/>
+      <c r="H54" s="326"/>
+      <c r="I54" s="326"/>
+      <c r="J54" s="326"/>
+      <c r="K54" s="326"/>
+      <c r="L54" s="326"/>
+      <c r="M54" s="333"/>
+      <c r="N54" s="362"/>
+      <c r="O54" s="362"/>
+    </row>
+    <row r="55" spans="2:15">
+      <c r="B55" s="338">
+        <v>45</v>
+      </c>
+      <c r="C55" s="363"/>
+      <c r="D55" s="289"/>
+      <c r="E55" s="336"/>
+      <c r="F55" s="359"/>
+      <c r="G55" s="360"/>
+      <c r="H55" s="326"/>
+      <c r="I55" s="326"/>
+      <c r="J55" s="326"/>
+      <c r="K55" s="326"/>
+      <c r="L55" s="326"/>
+      <c r="M55" s="333"/>
+      <c r="N55" s="362"/>
+      <c r="O55" s="362"/>
+    </row>
+    <row r="56" spans="2:15">
+      <c r="B56" s="338">
+        <v>46</v>
+      </c>
+      <c r="C56" s="376"/>
+      <c r="D56" s="289"/>
+      <c r="E56" s="336"/>
+      <c r="F56" s="359"/>
+      <c r="G56" s="360"/>
+      <c r="H56" s="360"/>
+      <c r="I56" s="360"/>
+      <c r="J56" s="360"/>
+      <c r="K56" s="360"/>
+      <c r="L56" s="360"/>
+      <c r="M56" s="377"/>
+      <c r="N56" s="362"/>
+      <c r="O56" s="362"/>
+    </row>
+    <row r="57" spans="2:15">
+      <c r="B57" s="378" t="s">
+        <v>136</v>
+      </c>
+      <c r="C57" s="379"/>
+      <c r="D57" s="348"/>
+      <c r="E57" s="380"/>
+      <c r="F57" s="381"/>
+      <c r="G57" s="382"/>
+      <c r="H57" s="382"/>
+      <c r="I57" s="382"/>
+      <c r="J57" s="382"/>
+      <c r="K57" s="382"/>
+      <c r="L57" s="382"/>
+      <c r="M57" s="383"/>
+      <c r="N57" s="384"/>
+      <c r="O57" s="384"/>
+    </row>
+    <row r="104" spans="2:15" s="97" customFormat="1">
+      <c r="B104" t="s">
+        <v>104</v>
+      </c>
+      <c r="C104" s="63" t="s">
+        <v>107</v>
+      </c>
+      <c r="E104"/>
+      <c r="H104"/>
+      <c r="I104"/>
+      <c r="J104"/>
+      <c r="K104"/>
+      <c r="L104"/>
+      <c r="M104"/>
+      <c r="N104"/>
+      <c r="O104"/>
+    </row>
+    <row r="105" spans="2:15" s="97" customFormat="1">
+      <c r="B105"/>
+      <c r="C105" s="63" t="s">
+        <v>108</v>
+      </c>
+      <c r="E105"/>
+      <c r="H105"/>
+      <c r="I105"/>
+      <c r="J105"/>
+      <c r="K105"/>
+      <c r="L105"/>
+      <c r="M105"/>
+      <c r="N105"/>
+      <c r="O105"/>
+    </row>
+    <row r="106" spans="2:15" s="97" customFormat="1">
+      <c r="B106"/>
+      <c r="C106" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="E106"/>
+      <c r="H106"/>
+      <c r="I106"/>
+      <c r="J106"/>
+      <c r="K106"/>
+      <c r="L106"/>
+      <c r="M106"/>
+      <c r="N106"/>
+      <c r="O106"/>
+    </row>
+    <row r="107" spans="2:15" s="97" customFormat="1">
+      <c r="B107"/>
+      <c r="C107" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="E107"/>
+      <c r="H107"/>
+      <c r="I107"/>
+      <c r="J107"/>
+      <c r="K107"/>
+      <c r="L107"/>
+      <c r="M107"/>
+      <c r="N107"/>
+      <c r="O107"/>
+    </row>
+    <row r="108" spans="2:15" s="97" customFormat="1">
+      <c r="B108"/>
+      <c r="C108" s="64" t="s">
+        <v>125</v>
+      </c>
+      <c r="E108"/>
+      <c r="H108"/>
+      <c r="I108"/>
+      <c r="J108"/>
+      <c r="K108"/>
+      <c r="L108"/>
+      <c r="M108"/>
+      <c r="N108"/>
+      <c r="O108"/>
+    </row>
+    <row r="109" spans="2:15" s="97" customFormat="1">
+      <c r="B109" t="s">
+        <v>111</v>
+      </c>
+      <c r="C109"/>
+      <c r="E109"/>
+      <c r="H109"/>
+      <c r="I109"/>
+      <c r="J109"/>
+      <c r="K109"/>
+      <c r="L109"/>
+      <c r="M109"/>
+      <c r="N109"/>
+      <c r="O109"/>
+    </row>
+    <row r="110" spans="2:15" s="97" customFormat="1">
+      <c r="B110"/>
+      <c r="C110" s="64" t="s">
+        <v>349</v>
+      </c>
+      <c r="E110"/>
+      <c r="H110"/>
+      <c r="I110"/>
+      <c r="J110"/>
+      <c r="K110"/>
+      <c r="L110"/>
+      <c r="M110"/>
+      <c r="N110"/>
+      <c r="O110"/>
+    </row>
+    <row r="111" spans="2:15" s="97" customFormat="1">
+      <c r="B111"/>
+      <c r="C111" s="64" t="s">
+        <v>350</v>
+      </c>
+      <c r="E111"/>
+      <c r="H111"/>
+      <c r="I111"/>
+      <c r="J111"/>
+      <c r="K111"/>
+      <c r="L111"/>
+      <c r="M111"/>
+      <c r="N111"/>
+      <c r="O111"/>
+    </row>
+    <row r="112" spans="2:15" s="97" customFormat="1">
+      <c r="B112"/>
+      <c r="C112" s="64" t="s">
+        <v>351</v>
+      </c>
+      <c r="E112"/>
+      <c r="H112"/>
+      <c r="I112"/>
+      <c r="J112"/>
+      <c r="K112"/>
+      <c r="L112"/>
+      <c r="M112"/>
+      <c r="N112"/>
+      <c r="O112"/>
+    </row>
+    <row r="113" spans="2:15" s="97" customFormat="1">
+      <c r="B113"/>
+      <c r="C113" s="64" t="s">
+        <v>352</v>
+      </c>
+      <c r="E113"/>
+      <c r="H113"/>
+      <c r="I113"/>
+      <c r="J113"/>
+      <c r="K113"/>
+      <c r="L113"/>
+      <c r="M113"/>
+      <c r="N113"/>
+      <c r="O113"/>
+    </row>
+    <row r="114" spans="2:15" s="97" customFormat="1">
+      <c r="B114"/>
+      <c r="C114" s="64" t="s">
+        <v>116</v>
+      </c>
+      <c r="E114"/>
+      <c r="H114"/>
+      <c r="I114"/>
+      <c r="J114"/>
+      <c r="K114"/>
+      <c r="L114"/>
+      <c r="M114"/>
+      <c r="N114"/>
+      <c r="O114"/>
+    </row>
+    <row r="116" spans="2:15" s="97" customFormat="1">
+      <c r="B116" t="s">
+        <v>106</v>
+      </c>
+      <c r="C116"/>
+      <c r="E116"/>
+      <c r="H116"/>
+      <c r="I116"/>
+      <c r="J116"/>
+      <c r="K116"/>
+      <c r="L116"/>
+      <c r="M116"/>
+      <c r="N116"/>
+      <c r="O116"/>
+    </row>
+    <row r="117" spans="2:15" s="97" customFormat="1">
+      <c r="B117"/>
+      <c r="C117" s="64" t="s">
+        <v>339</v>
+      </c>
+      <c r="E117"/>
+      <c r="H117"/>
+      <c r="I117"/>
+      <c r="J117"/>
+      <c r="K117"/>
+      <c r="L117"/>
+      <c r="M117"/>
+      <c r="N117"/>
+      <c r="O117"/>
+    </row>
+    <row r="118" spans="2:15" s="97" customFormat="1">
+      <c r="B118"/>
+      <c r="C118" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="E118"/>
+      <c r="H118"/>
+      <c r="I118"/>
+      <c r="J118"/>
+      <c r="K118"/>
+      <c r="L118"/>
+      <c r="M118"/>
+      <c r="N118"/>
+      <c r="O118"/>
+    </row>
+    <row r="119" spans="2:15" s="97" customFormat="1">
+      <c r="B119"/>
+      <c r="C119" s="64" t="s">
+        <v>118</v>
+      </c>
+      <c r="E119"/>
+      <c r="H119"/>
+      <c r="I119"/>
+      <c r="J119"/>
+      <c r="K119"/>
+      <c r="L119"/>
+      <c r="M119"/>
+      <c r="N119"/>
+      <c r="O119"/>
+    </row>
+    <row r="120" spans="2:15" s="97" customFormat="1">
+      <c r="B120"/>
+      <c r="C120" s="64" t="s">
+        <v>119</v>
+      </c>
+      <c r="E120"/>
+      <c r="H120"/>
+      <c r="I120"/>
+      <c r="J120"/>
+      <c r="K120"/>
+      <c r="L120"/>
+      <c r="M120"/>
+      <c r="N120"/>
+      <c r="O120"/>
+    </row>
+    <row r="121" spans="2:15" s="97" customFormat="1">
+      <c r="B121"/>
+      <c r="C121" s="64" t="s">
+        <v>120</v>
+      </c>
+      <c r="E121"/>
+      <c r="H121"/>
+      <c r="I121"/>
+      <c r="J121"/>
+      <c r="K121"/>
+      <c r="L121"/>
+      <c r="M121"/>
+      <c r="N121"/>
+      <c r="O121"/>
+    </row>
+    <row r="122" spans="2:15" s="97" customFormat="1">
+      <c r="B122"/>
+      <c r="C122" s="64" t="s">
+        <v>121</v>
+      </c>
+      <c r="E122"/>
+      <c r="H122"/>
+      <c r="I122"/>
+      <c r="J122"/>
+      <c r="K122"/>
+      <c r="L122"/>
+      <c r="M122"/>
+      <c r="N122"/>
+      <c r="O122"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B7:E7"/>
+  </mergeCells>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F55:F57 F20:F40 F11:F18">
+      <formula1>$C$117:$C$122</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="E55:E57 E11:E34 E37">
+      <formula1>$C$110:$C$114</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D55:D57 D11:D32 D37">
+      <formula1>$C$104:$C$108</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F58:F94">
+      <formula1>$C$118:$C$122</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="28" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:O121"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" customWidth="1"/>
+    <col min="3" max="3" width="45.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="97" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.5703125" style="97" customWidth="1"/>
+    <col min="8" max="15" width="9.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:15" ht="18">
+      <c r="B2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="156"/>
+    </row>
+    <row r="3" spans="2:15" ht="18">
+      <c r="B3" s="13"/>
+    </row>
+    <row r="4" spans="2:15">
+      <c r="C4" s="14" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15">
+      <c r="C5" s="14" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15">
+      <c r="C6" s="14"/>
+    </row>
+    <row r="7" spans="2:15" ht="18">
+      <c r="B7" s="422" t="s">
+        <v>476</v>
+      </c>
+      <c r="C7" s="422"/>
+      <c r="D7" s="422"/>
+      <c r="E7" s="422"/>
+    </row>
+    <row r="10" spans="2:15" s="107" customFormat="1" ht="12" customHeight="1">
+      <c r="B10" s="275" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="276" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="276" t="s">
+        <v>104</v>
+      </c>
+      <c r="E10" s="276" t="s">
+        <v>105</v>
+      </c>
+      <c r="F10" s="276" t="s">
+        <v>106</v>
+      </c>
+      <c r="G10" s="310" t="s">
+        <v>347</v>
+      </c>
+      <c r="H10" s="272" t="s">
+        <v>460</v>
+      </c>
+      <c r="I10" s="272" t="s">
+        <v>461</v>
+      </c>
+      <c r="J10" s="273" t="s">
+        <v>462</v>
+      </c>
+      <c r="K10" s="273" t="s">
+        <v>463</v>
+      </c>
+      <c r="L10" s="273" t="s">
+        <v>464</v>
+      </c>
+      <c r="M10" s="273" t="s">
+        <v>465</v>
+      </c>
+      <c r="N10" s="274" t="s">
+        <v>466</v>
+      </c>
+      <c r="O10" s="311" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15">
+      <c r="B11" s="338">
+        <v>1</v>
+      </c>
+      <c r="C11" s="368" t="s">
+        <v>443</v>
+      </c>
+      <c r="D11" s="354" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" s="355" t="s">
+        <v>351</v>
+      </c>
+      <c r="F11" s="369" t="s">
+        <v>117</v>
+      </c>
+      <c r="G11" s="367">
+        <v>15</v>
       </c>
       <c r="H11" s="356"/>
       <c r="I11" s="357"/>
@@ -22408,7 +24495,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="368" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="D15" s="354" t="s">
         <v>107</v>
@@ -22420,7 +24507,7 @@
         <v>117</v>
       </c>
       <c r="G15" s="367">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H15" s="326"/>
       <c r="I15" s="339"/>
@@ -22469,7 +24556,7 @@
       <c r="D17" s="369" t="s">
         <v>107</v>
       </c>
-      <c r="E17" s="418" t="s">
+      <c r="E17" s="400" t="s">
         <v>352</v>
       </c>
       <c r="F17" s="369" t="s">
@@ -22504,7 +24591,7 @@
         <v>117</v>
       </c>
       <c r="G18" s="367">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H18" s="356"/>
       <c r="I18" s="357"/>
@@ -22520,7 +24607,7 @@
         <v>9</v>
       </c>
       <c r="C19" s="374" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="D19" s="354" t="s">
         <v>107</v>
@@ -22529,10 +24616,10 @@
         <v>350</v>
       </c>
       <c r="F19" s="369" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G19" s="367">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H19" s="326"/>
       <c r="I19" s="339"/>
@@ -23486,24 +25573,23 @@
     <mergeCell ref="B7:E7"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F54:F56 F11:F17 F19:F39">
-      <formula1>$C$116:$C$121</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F57:F93">
+      <formula1>$C$117:$C$121</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D54:D56 D36 D11:D31">
+      <formula1>$C$103:$C$107</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="E54:E56 E36 E11:E33">
       <formula1>$C$109:$C$113</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D54:D56 D36 D11:D31">
-      <formula1>$C$103:$C$107</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F57:F93">
-      <formula1>$C$117:$C$121</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F54:F56 F11:F17 F19:F39">
+      <formula1>$C$116:$C$121</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="28" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -26035,12 +28121,12 @@
       <c r="C6" s="14"/>
     </row>
     <row r="7" spans="2:27" ht="18">
-      <c r="B7" s="417" t="s">
+      <c r="B7" s="422" t="s">
         <v>285</v>
       </c>
-      <c r="C7" s="417"/>
-      <c r="D7" s="417"/>
-      <c r="E7" s="417"/>
+      <c r="C7" s="422"/>
+      <c r="D7" s="422"/>
+      <c r="E7" s="422"/>
     </row>
     <row r="10" spans="2:27" s="107" customFormat="1" ht="12" customHeight="1">
       <c r="B10" s="117" t="s">
@@ -30216,12 +32302,12 @@
       <c r="C6" s="14"/>
     </row>
     <row r="7" spans="2:14" ht="18">
-      <c r="B7" s="417" t="s">
+      <c r="B7" s="422" t="s">
         <v>317</v>
       </c>
-      <c r="C7" s="417"/>
-      <c r="D7" s="417"/>
-      <c r="E7" s="417"/>
+      <c r="C7" s="422"/>
+      <c r="D7" s="422"/>
+      <c r="E7" s="422"/>
     </row>
     <row r="10" spans="2:14" s="107" customFormat="1" ht="12" customHeight="1">
       <c r="B10" s="117" t="s">
@@ -31837,12 +33923,12 @@
       <c r="C6" s="14"/>
     </row>
     <row r="7" spans="2:13" ht="18">
-      <c r="B7" s="417" t="s">
+      <c r="B7" s="422" t="s">
         <v>348</v>
       </c>
-      <c r="C7" s="417"/>
-      <c r="D7" s="417"/>
-      <c r="E7" s="417"/>
+      <c r="C7" s="422"/>
+      <c r="D7" s="422"/>
+      <c r="E7" s="422"/>
     </row>
     <row r="10" spans="2:13" s="107" customFormat="1" ht="12" customHeight="1">
       <c r="B10" s="275" t="s">
@@ -33106,12 +35192,12 @@
       <c r="C6" s="14"/>
     </row>
     <row r="7" spans="2:15" ht="18">
-      <c r="B7" s="417" t="s">
+      <c r="B7" s="422" t="s">
         <v>372</v>
       </c>
-      <c r="C7" s="417"/>
-      <c r="D7" s="417"/>
-      <c r="E7" s="417"/>
+      <c r="C7" s="422"/>
+      <c r="D7" s="422"/>
+      <c r="E7" s="422"/>
     </row>
     <row r="10" spans="2:15" s="107" customFormat="1" ht="12" customHeight="1">
       <c r="B10" s="275" t="s">
@@ -34669,12 +36755,12 @@
       <c r="C6" s="14"/>
     </row>
     <row r="7" spans="2:15" ht="18">
-      <c r="B7" s="417" t="s">
+      <c r="B7" s="422" t="s">
         <v>392</v>
       </c>
-      <c r="C7" s="417"/>
-      <c r="D7" s="417"/>
-      <c r="E7" s="417"/>
+      <c r="C7" s="422"/>
+      <c r="D7" s="422"/>
+      <c r="E7" s="422"/>
     </row>
     <row r="10" spans="2:15" s="107" customFormat="1" ht="12" customHeight="1">
       <c r="B10" s="275" t="s">

</xml_diff>

<commit_message>
check SVN for exls extension - inprogress
</commit_message>
<xml_diff>
--- a/Documents/ProductBackLog/Capstone_Group6_ProductBackLog_SprintTaskList.xlsx
+++ b/Documents/ProductBackLog/Capstone_Group6_ProductBackLog_SprintTaskList.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4680" firstSheet="10" activeTab="12"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4680" tabRatio="949" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint01_0805_1205" sheetId="9" r:id="rId1"/>
@@ -402,55 +402,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G24" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tu Huynh:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Sprint 3</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G25" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tu Huynh:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Sprint 3</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G28" authorId="0">
+    <comment ref="G26" authorId="0">
       <text>
         <r>
           <rPr>
@@ -474,7 +426,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G29" authorId="0">
+    <comment ref="G27" authorId="0">
       <text>
         <r>
           <rPr>
@@ -498,7 +450,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G30" authorId="0">
+    <comment ref="G28" authorId="0">
       <text>
         <r>
           <rPr>
@@ -647,7 +599,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1220" uniqueCount="254">
   <si>
     <t>CAPSTONE PROJECT</t>
   </si>
@@ -9962,8 +9914,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table1345678910" displayName="Table1345678910" ref="B10:O53" totalsRowShown="0" headerRowDxfId="208" dataDxfId="206" headerRowBorderDxfId="207" tableBorderDxfId="205" totalsRowBorderDxfId="204">
-  <autoFilter ref="B10:O53"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table1345678910" displayName="Table1345678910" ref="B10:O51" totalsRowShown="0" headerRowDxfId="208" dataDxfId="206" headerRowBorderDxfId="207" tableBorderDxfId="205" totalsRowBorderDxfId="204">
+  <autoFilter ref="B10:O51"/>
   <tableColumns count="14">
     <tableColumn id="1" name="No." dataDxfId="203"/>
     <tableColumn id="2" name="Task description" dataDxfId="202"/>
@@ -15999,7 +15951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:O121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
@@ -18802,7 +18754,7 @@
   <dimension ref="B2:O119"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25:C28"/>
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19428,10 +19380,10 @@
         <v>12</v>
       </c>
       <c r="G25" s="50">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H25" s="51">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I25" s="54">
         <v>15</v>
@@ -19443,16 +19395,16 @@
         <v>13</v>
       </c>
       <c r="L25" s="54">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="M25" s="55">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="N25" s="65">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="O25" s="65">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="2:15">
@@ -19472,7 +19424,7 @@
         <v>12</v>
       </c>
       <c r="G26" s="50">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H26" s="51">
         <v>12</v>
@@ -19516,7 +19468,7 @@
         <v>12</v>
       </c>
       <c r="G27" s="50">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H27" s="51">
         <v>15</v>
@@ -19540,7 +19492,7 @@
         <v>12</v>
       </c>
       <c r="O27" s="65">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="2:15">
@@ -19560,7 +19512,7 @@
         <v>12</v>
       </c>
       <c r="G28" s="50">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H28" s="51">
         <v>12</v>
@@ -20364,8 +20316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:O119"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31:C33"/>
+    <sheetView topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20924,34 +20876,34 @@
         <v>51</v>
       </c>
       <c r="F23" s="22" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G23" s="58">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H23" s="63">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="I23" s="76">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="J23" s="76">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="K23" s="76">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="L23" s="76">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="M23" s="68">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="N23" s="69">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="O23" s="69">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:15">
@@ -20977,25 +20929,25 @@
         <v>12</v>
       </c>
       <c r="I24" s="76">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J24" s="76">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="K24" s="76">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="L24" s="76">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="M24" s="68">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="N24" s="69">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="O24" s="69">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="2:15">
@@ -21012,34 +20964,34 @@
         <v>51</v>
       </c>
       <c r="F25" s="22" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G25" s="58">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H25" s="63">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="I25" s="76">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="J25" s="76">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="K25" s="76">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="L25" s="76">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="M25" s="68">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="N25" s="69">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="O25" s="69">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:15">
@@ -21062,28 +21014,28 @@
         <v>12</v>
       </c>
       <c r="H26" s="63">
-        <v>12</v>
-      </c>
-      <c r="I26" s="76">
-        <v>12</v>
-      </c>
-      <c r="J26" s="76">
-        <v>12</v>
-      </c>
-      <c r="K26" s="76">
-        <v>12</v>
-      </c>
-      <c r="L26" s="76">
-        <v>12</v>
-      </c>
-      <c r="M26" s="68">
-        <v>12</v>
-      </c>
-      <c r="N26" s="69">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="I26" s="63">
+        <v>10</v>
+      </c>
+      <c r="J26" s="63">
+        <v>10</v>
+      </c>
+      <c r="K26" s="63">
+        <v>10</v>
+      </c>
+      <c r="L26" s="63">
+        <v>10</v>
+      </c>
+      <c r="M26" s="63">
+        <v>6</v>
+      </c>
+      <c r="N26" s="63">
+        <v>6</v>
       </c>
       <c r="O26" s="69">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="2:15">
@@ -21123,7 +21075,7 @@
         <v>12</v>
       </c>
       <c r="G28" s="58">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H28" s="63">
         <v>12</v>
@@ -21144,10 +21096,10 @@
         <v>12</v>
       </c>
       <c r="N28" s="69">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="O28" s="69">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="2:15">
@@ -22031,10 +21983,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:O118"/>
+  <dimension ref="B2:O116"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22537,37 +22489,37 @@
     </row>
     <row r="22" spans="2:15">
       <c r="B22" s="75">
-        <v>12</v>
-      </c>
-      <c r="C22" s="100" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="109" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="73" t="s">
+      <c r="E22" s="92" t="s">
         <v>51</v>
       </c>
-      <c r="F22" s="96" t="s">
+      <c r="F22" s="106" t="s">
         <v>14</v>
       </c>
-      <c r="G22" s="97">
-        <v>10</v>
+      <c r="G22" s="104">
+        <v>4</v>
       </c>
       <c r="H22" s="93">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I22" s="94">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J22" s="94">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K22" s="94">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L22" s="94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M22" s="94">
         <v>0</v>
@@ -22581,10 +22533,10 @@
     </row>
     <row r="23" spans="2:15">
       <c r="B23" s="75">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C23" s="109" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D23" s="91" t="s">
         <v>6</v>
@@ -22593,44 +22545,44 @@
         <v>51</v>
       </c>
       <c r="F23" s="106" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G23" s="104">
-        <v>12</v>
-      </c>
-      <c r="H23" s="93">
-        <v>12</v>
-      </c>
-      <c r="I23" s="94">
-        <v>12</v>
-      </c>
-      <c r="J23" s="94">
-        <v>12</v>
-      </c>
-      <c r="K23" s="94">
-        <v>12</v>
-      </c>
-      <c r="L23" s="94">
-        <v>12</v>
-      </c>
-      <c r="M23" s="94">
-        <v>12</v>
+        <v>4</v>
+      </c>
+      <c r="H23" s="110">
+        <v>4</v>
+      </c>
+      <c r="I23" s="110">
+        <v>3</v>
+      </c>
+      <c r="J23" s="110">
+        <v>0</v>
+      </c>
+      <c r="K23" s="110">
+        <v>0</v>
+      </c>
+      <c r="L23" s="110">
+        <v>0</v>
+      </c>
+      <c r="M23" s="110">
+        <v>0</v>
       </c>
       <c r="N23" s="108">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="O23" s="108">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="2:15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" ht="36" customHeight="1">
       <c r="B24" s="75">
-        <v>14</v>
-      </c>
-      <c r="C24" s="105" t="s">
-        <v>70</v>
-      </c>
-      <c r="D24" s="91" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="111" t="s">
+        <v>108</v>
+      </c>
+      <c r="D24" s="102" t="s">
         <v>6</v>
       </c>
       <c r="E24" s="92" t="s">
@@ -22642,145 +22594,145 @@
       <c r="G24" s="104">
         <v>10</v>
       </c>
-      <c r="H24" s="93">
+      <c r="H24" s="63">
         <v>10</v>
       </c>
-      <c r="I24" s="94">
+      <c r="I24" s="76">
         <v>10</v>
       </c>
-      <c r="J24" s="94">
+      <c r="J24" s="76">
         <v>10</v>
       </c>
-      <c r="K24" s="94">
+      <c r="K24" s="76">
         <v>10</v>
       </c>
-      <c r="L24" s="94">
+      <c r="L24" s="76">
         <v>10</v>
       </c>
-      <c r="M24" s="94">
+      <c r="M24" s="68">
         <v>10</v>
       </c>
-      <c r="N24" s="108">
+      <c r="N24" s="99">
         <v>10</v>
       </c>
-      <c r="O24" s="108">
+      <c r="O24" s="99">
         <v>10</v>
       </c>
     </row>
     <row r="25" spans="2:15">
       <c r="B25" s="75">
-        <v>15</v>
-      </c>
-      <c r="C25" s="109" t="s">
-        <v>72</v>
-      </c>
-      <c r="D25" s="91" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="95" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="26"/>
+      <c r="E25" s="73"/>
+      <c r="F25" s="96"/>
+      <c r="G25" s="97"/>
+      <c r="H25" s="63"/>
+      <c r="I25" s="76"/>
+      <c r="J25" s="76"/>
+      <c r="K25" s="76"/>
+      <c r="L25" s="76"/>
+      <c r="M25" s="68"/>
+      <c r="N25" s="99"/>
+      <c r="O25" s="99"/>
+    </row>
+    <row r="26" spans="2:15">
+      <c r="B26" s="75">
+        <v>18</v>
+      </c>
+      <c r="C26" s="109" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="92" t="s">
-        <v>51</v>
-      </c>
-      <c r="F25" s="106" t="s">
-        <v>12</v>
-      </c>
-      <c r="G25" s="104">
-        <v>12</v>
-      </c>
-      <c r="H25" s="110">
-        <v>12</v>
-      </c>
-      <c r="I25" s="110">
-        <v>12</v>
-      </c>
-      <c r="J25" s="110">
-        <v>12</v>
-      </c>
-      <c r="K25" s="110">
-        <v>12</v>
-      </c>
-      <c r="L25" s="110">
-        <v>12</v>
-      </c>
-      <c r="M25" s="110">
-        <v>12</v>
-      </c>
-      <c r="N25" s="108">
-        <v>12</v>
-      </c>
-      <c r="O25" s="108">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="2:15" ht="36" customHeight="1">
-      <c r="B26" s="75">
-        <v>16</v>
-      </c>
-      <c r="C26" s="111" t="s">
-        <v>108</v>
-      </c>
-      <c r="D26" s="102" t="s">
-        <v>6</v>
-      </c>
       <c r="E26" s="92" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F26" s="106" t="s">
         <v>12</v>
       </c>
       <c r="G26" s="104">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H26" s="63">
         <v>10</v>
       </c>
-      <c r="I26" s="76">
-        <v>10</v>
-      </c>
-      <c r="J26" s="76">
-        <v>10</v>
-      </c>
-      <c r="K26" s="76">
-        <v>10</v>
-      </c>
-      <c r="L26" s="76">
-        <v>10</v>
-      </c>
-      <c r="M26" s="68">
-        <v>10</v>
+      <c r="I26" s="63">
+        <v>8</v>
+      </c>
+      <c r="J26" s="63">
+        <v>7</v>
+      </c>
+      <c r="K26" s="63">
+        <v>6</v>
+      </c>
+      <c r="L26" s="63">
+        <v>5</v>
+      </c>
+      <c r="M26" s="70">
+        <v>5</v>
       </c>
       <c r="N26" s="99">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="O26" s="99">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="2:15">
       <c r="B27" s="75">
-        <v>17</v>
-      </c>
-      <c r="C27" s="95" t="s">
-        <v>89</v>
-      </c>
-      <c r="D27" s="26"/>
-      <c r="E27" s="73"/>
-      <c r="F27" s="96"/>
-      <c r="G27" s="97"/>
-      <c r="H27" s="63"/>
-      <c r="I27" s="76"/>
-      <c r="J27" s="76"/>
-      <c r="K27" s="76"/>
-      <c r="L27" s="76"/>
-      <c r="M27" s="68"/>
-      <c r="N27" s="99"/>
-      <c r="O27" s="99"/>
+        <v>19</v>
+      </c>
+      <c r="C27" s="105" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" s="91" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="92" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="106" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" s="104">
+        <v>12</v>
+      </c>
+      <c r="H27" s="63">
+        <v>10</v>
+      </c>
+      <c r="I27" s="63">
+        <v>8</v>
+      </c>
+      <c r="J27" s="63">
+        <v>7</v>
+      </c>
+      <c r="K27" s="63">
+        <v>6</v>
+      </c>
+      <c r="L27" s="63">
+        <v>4</v>
+      </c>
+      <c r="M27" s="70">
+        <v>2</v>
+      </c>
+      <c r="N27" s="99">
+        <v>0</v>
+      </c>
+      <c r="O27" s="99">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="2:15">
       <c r="B28" s="75">
-        <v>18</v>
-      </c>
-      <c r="C28" s="109" t="s">
-        <v>92</v>
+        <v>20</v>
+      </c>
+      <c r="C28" s="105" t="s">
+        <v>91</v>
       </c>
       <c r="D28" s="91" t="s">
         <v>6</v>
@@ -22795,36 +22747,36 @@
         <v>12</v>
       </c>
       <c r="H28" s="63">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I28" s="63">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="J28" s="63">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="K28" s="63">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="L28" s="63">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="M28" s="70">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="N28" s="99">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="O28" s="99">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="2:15">
       <c r="B29" s="75">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C29" s="105" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="D29" s="91" t="s">
         <v>6</v>
@@ -22836,124 +22788,72 @@
         <v>12</v>
       </c>
       <c r="G29" s="104">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H29" s="63">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="I29" s="63">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="J29" s="63">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="K29" s="63">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="L29" s="63">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="M29" s="70">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="N29" s="99">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O29" s="99">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="2:15">
       <c r="B30" s="75">
-        <v>20</v>
-      </c>
-      <c r="C30" s="105" t="s">
-        <v>91</v>
-      </c>
-      <c r="D30" s="91" t="s">
-        <v>6</v>
-      </c>
-      <c r="E30" s="92" t="s">
-        <v>53</v>
-      </c>
-      <c r="F30" s="106" t="s">
-        <v>12</v>
-      </c>
-      <c r="G30" s="104">
-        <v>12</v>
-      </c>
-      <c r="H30" s="63">
-        <v>12</v>
-      </c>
-      <c r="I30" s="63">
-        <v>12</v>
-      </c>
-      <c r="J30" s="63">
-        <v>12</v>
-      </c>
-      <c r="K30" s="63">
-        <v>12</v>
-      </c>
-      <c r="L30" s="63">
-        <v>12</v>
-      </c>
-      <c r="M30" s="70">
-        <v>12</v>
-      </c>
-      <c r="N30" s="99">
-        <v>12</v>
-      </c>
-      <c r="O30" s="99">
-        <v>12</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="C30" s="103"/>
+      <c r="D30" s="102"/>
+      <c r="E30" s="103"/>
+      <c r="F30" s="102"/>
+      <c r="G30" s="104"/>
+      <c r="H30" s="63"/>
+      <c r="I30" s="63"/>
+      <c r="J30" s="63"/>
+      <c r="K30" s="63"/>
+      <c r="L30" s="63"/>
+      <c r="M30" s="70"/>
+      <c r="N30" s="99"/>
+      <c r="O30" s="99"/>
     </row>
     <row r="31" spans="2:15">
       <c r="B31" s="75">
-        <v>21</v>
-      </c>
-      <c r="C31" s="105" t="s">
-        <v>109</v>
-      </c>
-      <c r="D31" s="91" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" s="92" t="s">
-        <v>53</v>
-      </c>
-      <c r="F31" s="106" t="s">
-        <v>12</v>
-      </c>
-      <c r="G31" s="104">
-        <v>20</v>
-      </c>
-      <c r="H31" s="63">
-        <v>20</v>
-      </c>
-      <c r="I31" s="63">
-        <v>20</v>
-      </c>
-      <c r="J31" s="63">
-        <v>20</v>
-      </c>
-      <c r="K31" s="63">
-        <v>20</v>
-      </c>
-      <c r="L31" s="63">
-        <v>20</v>
-      </c>
-      <c r="M31" s="70">
-        <v>20</v>
-      </c>
-      <c r="N31" s="99">
-        <v>20</v>
-      </c>
-      <c r="O31" s="99">
-        <v>20</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C31" s="112"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="73"/>
+      <c r="F31" s="96"/>
+      <c r="G31" s="97"/>
+      <c r="H31" s="63"/>
+      <c r="I31" s="63"/>
+      <c r="J31" s="63"/>
+      <c r="K31" s="63"/>
+      <c r="L31" s="63"/>
+      <c r="M31" s="70"/>
+      <c r="N31" s="99"/>
+      <c r="O31" s="99"/>
     </row>
     <row r="32" spans="2:15">
       <c r="B32" s="75">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C32" s="103"/>
       <c r="D32" s="102"/>
@@ -22971,13 +22871,13 @@
     </row>
     <row r="33" spans="2:15">
       <c r="B33" s="75">
-        <v>23</v>
-      </c>
-      <c r="C33" s="112"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="73"/>
-      <c r="F33" s="96"/>
-      <c r="G33" s="97"/>
+        <v>25</v>
+      </c>
+      <c r="C33" s="103"/>
+      <c r="D33" s="102"/>
+      <c r="E33" s="103"/>
+      <c r="F33" s="102"/>
+      <c r="G33" s="104"/>
       <c r="H33" s="63"/>
       <c r="I33" s="63"/>
       <c r="J33" s="63"/>
@@ -22989,7 +22889,7 @@
     </row>
     <row r="34" spans="2:15">
       <c r="B34" s="75">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C34" s="103"/>
       <c r="D34" s="102"/>
@@ -23007,7 +22907,7 @@
     </row>
     <row r="35" spans="2:15">
       <c r="B35" s="75">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C35" s="103"/>
       <c r="D35" s="102"/>
@@ -23025,7 +22925,7 @@
     </row>
     <row r="36" spans="2:15">
       <c r="B36" s="75">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C36" s="103"/>
       <c r="D36" s="102"/>
@@ -23043,7 +22943,7 @@
     </row>
     <row r="37" spans="2:15">
       <c r="B37" s="75">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C37" s="103"/>
       <c r="D37" s="102"/>
@@ -23061,7 +22961,7 @@
     </row>
     <row r="38" spans="2:15">
       <c r="B38" s="75">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C38" s="103"/>
       <c r="D38" s="102"/>
@@ -23079,7 +22979,7 @@
     </row>
     <row r="39" spans="2:15">
       <c r="B39" s="75">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C39" s="103"/>
       <c r="D39" s="102"/>
@@ -23097,7 +22997,7 @@
     </row>
     <row r="40" spans="2:15">
       <c r="B40" s="75">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C40" s="103"/>
       <c r="D40" s="102"/>
@@ -23115,7 +23015,7 @@
     </row>
     <row r="41" spans="2:15">
       <c r="B41" s="75">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C41" s="103"/>
       <c r="D41" s="102"/>
@@ -23133,7 +23033,7 @@
     </row>
     <row r="42" spans="2:15">
       <c r="B42" s="75">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C42" s="103"/>
       <c r="D42" s="102"/>
@@ -23151,7 +23051,7 @@
     </row>
     <row r="43" spans="2:15">
       <c r="B43" s="75">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C43" s="103"/>
       <c r="D43" s="102"/>
@@ -23169,7 +23069,7 @@
     </row>
     <row r="44" spans="2:15">
       <c r="B44" s="75">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C44" s="103"/>
       <c r="D44" s="102"/>
@@ -23187,7 +23087,7 @@
     </row>
     <row r="45" spans="2:15">
       <c r="B45" s="75">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C45" s="103"/>
       <c r="D45" s="102"/>
@@ -23205,7 +23105,7 @@
     </row>
     <row r="46" spans="2:15">
       <c r="B46" s="75">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C46" s="103"/>
       <c r="D46" s="102"/>
@@ -23223,7 +23123,7 @@
     </row>
     <row r="47" spans="2:15">
       <c r="B47" s="75">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C47" s="103"/>
       <c r="D47" s="102"/>
@@ -23241,7 +23141,7 @@
     </row>
     <row r="48" spans="2:15">
       <c r="B48" s="75">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C48" s="103"/>
       <c r="D48" s="102"/>
@@ -23259,13 +23159,13 @@
     </row>
     <row r="49" spans="2:15">
       <c r="B49" s="75">
-        <v>39</v>
-      </c>
-      <c r="C49" s="103"/>
-      <c r="D49" s="102"/>
-      <c r="E49" s="103"/>
-      <c r="F49" s="102"/>
-      <c r="G49" s="104"/>
+        <v>41</v>
+      </c>
+      <c r="C49" s="100"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="73"/>
+      <c r="F49" s="96"/>
+      <c r="G49" s="97"/>
       <c r="H49" s="63"/>
       <c r="I49" s="63"/>
       <c r="J49" s="63"/>
@@ -23277,82 +23177,76 @@
     </row>
     <row r="50" spans="2:15">
       <c r="B50" s="75">
-        <v>40</v>
-      </c>
-      <c r="C50" s="103"/>
-      <c r="D50" s="102"/>
-      <c r="E50" s="103"/>
-      <c r="F50" s="102"/>
-      <c r="G50" s="104"/>
-      <c r="H50" s="63"/>
-      <c r="I50" s="63"/>
-      <c r="J50" s="63"/>
-      <c r="K50" s="63"/>
-      <c r="L50" s="63"/>
-      <c r="M50" s="70"/>
+        <v>42</v>
+      </c>
+      <c r="C50" s="113"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="73"/>
+      <c r="F50" s="96"/>
+      <c r="G50" s="97"/>
+      <c r="H50" s="97"/>
+      <c r="I50" s="97"/>
+      <c r="J50" s="97"/>
+      <c r="K50" s="97"/>
+      <c r="L50" s="97"/>
+      <c r="M50" s="114"/>
       <c r="N50" s="99"/>
       <c r="O50" s="99"/>
     </row>
     <row r="51" spans="2:15">
-      <c r="B51" s="75">
-        <v>41</v>
-      </c>
-      <c r="C51" s="100"/>
-      <c r="D51" s="26"/>
-      <c r="E51" s="73"/>
-      <c r="F51" s="96"/>
-      <c r="G51" s="97"/>
-      <c r="H51" s="63"/>
-      <c r="I51" s="63"/>
-      <c r="J51" s="63"/>
-      <c r="K51" s="63"/>
-      <c r="L51" s="63"/>
-      <c r="M51" s="70"/>
-      <c r="N51" s="99"/>
-      <c r="O51" s="99"/>
-    </row>
-    <row r="52" spans="2:15">
-      <c r="B52" s="75">
-        <v>42</v>
-      </c>
-      <c r="C52" s="113"/>
-      <c r="D52" s="26"/>
-      <c r="E52" s="73"/>
-      <c r="F52" s="96"/>
-      <c r="G52" s="97"/>
-      <c r="H52" s="97"/>
-      <c r="I52" s="97"/>
-      <c r="J52" s="97"/>
-      <c r="K52" s="97"/>
-      <c r="L52" s="97"/>
-      <c r="M52" s="114"/>
-      <c r="N52" s="99"/>
-      <c r="O52" s="99"/>
-    </row>
-    <row r="53" spans="2:15">
-      <c r="B53" s="115" t="s">
+      <c r="B51" s="115" t="s">
         <v>18</v>
       </c>
-      <c r="C53" s="116"/>
-      <c r="D53" s="85"/>
-      <c r="E53" s="117"/>
-      <c r="F53" s="118"/>
-      <c r="G53" s="119"/>
-      <c r="H53" s="119"/>
-      <c r="I53" s="119"/>
-      <c r="J53" s="119"/>
-      <c r="K53" s="119"/>
-      <c r="L53" s="119"/>
-      <c r="M53" s="120"/>
-      <c r="N53" s="121"/>
-      <c r="O53" s="121"/>
+      <c r="C51" s="116"/>
+      <c r="D51" s="85"/>
+      <c r="E51" s="117"/>
+      <c r="F51" s="118"/>
+      <c r="G51" s="119"/>
+      <c r="H51" s="119"/>
+      <c r="I51" s="119"/>
+      <c r="J51" s="119"/>
+      <c r="K51" s="119"/>
+      <c r="L51" s="119"/>
+      <c r="M51" s="120"/>
+      <c r="N51" s="121"/>
+      <c r="O51" s="121"/>
+    </row>
+    <row r="98" spans="2:15" s="5" customFormat="1">
+      <c r="B98" t="s">
+        <v>3</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E98"/>
+      <c r="H98"/>
+      <c r="I98"/>
+      <c r="J98"/>
+      <c r="K98"/>
+      <c r="L98"/>
+      <c r="M98"/>
+      <c r="N98"/>
+      <c r="O98"/>
+    </row>
+    <row r="99" spans="2:15" s="5" customFormat="1">
+      <c r="B99"/>
+      <c r="C99" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E99"/>
+      <c r="H99"/>
+      <c r="I99"/>
+      <c r="J99"/>
+      <c r="K99"/>
+      <c r="L99"/>
+      <c r="M99"/>
+      <c r="N99"/>
+      <c r="O99"/>
     </row>
     <row r="100" spans="2:15" s="5" customFormat="1">
-      <c r="B100" t="s">
-        <v>3</v>
-      </c>
+      <c r="B100"/>
       <c r="C100" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E100"/>
       <c r="H100"/>
@@ -23367,7 +23261,7 @@
     <row r="101" spans="2:15" s="5" customFormat="1">
       <c r="B101"/>
       <c r="C101" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E101"/>
       <c r="H101"/>
@@ -23381,8 +23275,8 @@
     </row>
     <row r="102" spans="2:15" s="5" customFormat="1">
       <c r="B102"/>
-      <c r="C102" s="3" t="s">
-        <v>8</v>
+      <c r="C102" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="E102"/>
       <c r="H102"/>
@@ -23395,10 +23289,10 @@
       <c r="O102"/>
     </row>
     <row r="103" spans="2:15" s="5" customFormat="1">
-      <c r="B103"/>
-      <c r="C103" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="B103" t="s">
+        <v>10</v>
+      </c>
+      <c r="C103"/>
       <c r="E103"/>
       <c r="H103"/>
       <c r="I103"/>
@@ -23412,7 +23306,7 @@
     <row r="104" spans="2:15" s="5" customFormat="1">
       <c r="B104"/>
       <c r="C104" s="4" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="E104"/>
       <c r="H104"/>
@@ -23425,10 +23319,10 @@
       <c r="O104"/>
     </row>
     <row r="105" spans="2:15" s="5" customFormat="1">
-      <c r="B105" t="s">
-        <v>10</v>
-      </c>
-      <c r="C105"/>
+      <c r="B105"/>
+      <c r="C105" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="E105"/>
       <c r="H105"/>
       <c r="I105"/>
@@ -23442,7 +23336,7 @@
     <row r="106" spans="2:15" s="5" customFormat="1">
       <c r="B106"/>
       <c r="C106" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E106"/>
       <c r="H106"/>
@@ -23457,7 +23351,7 @@
     <row r="107" spans="2:15" s="5" customFormat="1">
       <c r="B107"/>
       <c r="C107" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E107"/>
       <c r="H107"/>
@@ -23472,7 +23366,7 @@
     <row r="108" spans="2:15" s="5" customFormat="1">
       <c r="B108"/>
       <c r="C108" s="4" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="E108"/>
       <c r="H108"/>
@@ -23484,26 +23378,11 @@
       <c r="N108"/>
       <c r="O108"/>
     </row>
-    <row r="109" spans="2:15" s="5" customFormat="1">
-      <c r="B109"/>
-      <c r="C109" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E109"/>
-      <c r="H109"/>
-      <c r="I109"/>
-      <c r="J109"/>
-      <c r="K109"/>
-      <c r="L109"/>
-      <c r="M109"/>
-      <c r="N109"/>
-      <c r="O109"/>
-    </row>
     <row r="110" spans="2:15" s="5" customFormat="1">
-      <c r="B110"/>
-      <c r="C110" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="B110" t="s">
+        <v>5</v>
+      </c>
+      <c r="C110"/>
       <c r="E110"/>
       <c r="H110"/>
       <c r="I110"/>
@@ -23514,11 +23393,26 @@
       <c r="N110"/>
       <c r="O110"/>
     </row>
+    <row r="111" spans="2:15" s="5" customFormat="1">
+      <c r="B111"/>
+      <c r="C111" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E111"/>
+      <c r="H111"/>
+      <c r="I111"/>
+      <c r="J111"/>
+      <c r="K111"/>
+      <c r="L111"/>
+      <c r="M111"/>
+      <c r="N111"/>
+      <c r="O111"/>
+    </row>
     <row r="112" spans="2:15" s="5" customFormat="1">
-      <c r="B112" t="s">
-        <v>5</v>
-      </c>
-      <c r="C112"/>
+      <c r="B112"/>
+      <c r="C112" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="E112"/>
       <c r="H112"/>
       <c r="I112"/>
@@ -23532,7 +23426,7 @@
     <row r="113" spans="2:15" s="5" customFormat="1">
       <c r="B113"/>
       <c r="C113" s="4" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="E113"/>
       <c r="H113"/>
@@ -23547,7 +23441,7 @@
     <row r="114" spans="2:15" s="5" customFormat="1">
       <c r="B114"/>
       <c r="C114" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E114"/>
       <c r="H114"/>
@@ -23562,7 +23456,7 @@
     <row r="115" spans="2:15" s="5" customFormat="1">
       <c r="B115"/>
       <c r="C115" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E115"/>
       <c r="H115"/>
@@ -23577,7 +23471,7 @@
     <row r="116" spans="2:15" s="5" customFormat="1">
       <c r="B116"/>
       <c r="C116" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E116"/>
       <c r="H116"/>
@@ -23589,52 +23483,22 @@
       <c r="N116"/>
       <c r="O116"/>
     </row>
-    <row r="117" spans="2:15" s="5" customFormat="1">
-      <c r="B117"/>
-      <c r="C117" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E117"/>
-      <c r="H117"/>
-      <c r="I117"/>
-      <c r="J117"/>
-      <c r="K117"/>
-      <c r="L117"/>
-      <c r="M117"/>
-      <c r="N117"/>
-      <c r="O117"/>
-    </row>
-    <row r="118" spans="2:15" s="5" customFormat="1">
-      <c r="B118"/>
-      <c r="C118" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E118"/>
-      <c r="H118"/>
-      <c r="I118"/>
-      <c r="J118"/>
-      <c r="K118"/>
-      <c r="L118"/>
-      <c r="M118"/>
-      <c r="N118"/>
-      <c r="O118"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B7:E7"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F51:F53 F11:F13 F15:F31 F33">
-      <formula1>$C$113:$C$118</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F49:F51 F11:F13 F15:F29 F31">
+      <formula1>$C$111:$C$116</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="E51:E53 E11:E13 E15:E31 E33">
-      <formula1>$C$106:$C$110</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="E49:E51 E11:E13 E15:E29 E31">
+      <formula1>$C$104:$C$108</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D51:D53 D11:D13 D15:D25 D33 D27:D31">
-      <formula1>$C$100:$C$104</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D49:D51 D11:D13 D15:D23 D31 D25:D29">
+      <formula1>$C$98:$C$102</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F54:F90">
-      <formula1>$C$114:$C$118</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F52:F88">
+      <formula1>$C$112:$C$116</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23651,7 +23515,7 @@
   <dimension ref="B2:O119"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -25181,7 +25045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:O121"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -26751,7 +26615,7 @@
   <dimension ref="B2:O121"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>